<commit_message>
adding to AB pattern
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B77FA69-2856-E543-8905-2223FCC0F626}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C58D98D-13B0-404E-86C1-E7B085AF3F1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19440" windowHeight="15000" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -26,21 +26,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3019" uniqueCount="1442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3027" uniqueCount="1450">
   <si>
     <t>Status</t>
   </si>
@@ -4200,12 +4191,6 @@
     <t>humerus length</t>
   </si>
   <si>
-    <t>humerus length 1</t>
-  </si>
-  <si>
-    <t>humerus length 2</t>
-  </si>
-  <si>
     <t>subclass</t>
   </si>
   <si>
@@ -4438,6 +4423,36 @@
   </si>
   <si>
     <t>femur length to head of femur?</t>
+  </si>
+  <si>
+    <t>humerus length from trochlea to greater tubercle</t>
+  </si>
+  <si>
+    <t>humerus length from trochlea to caput</t>
+  </si>
+  <si>
+    <t>femur length from greater trochanter to medial condyle</t>
+  </si>
+  <si>
+    <t>femur length from caput to medial condyle</t>
+  </si>
+  <si>
+    <t>trochlea of humerus</t>
+  </si>
+  <si>
+    <t>proximal head of humerus</t>
+  </si>
+  <si>
+    <t>ventral tubercle of humerus</t>
+  </si>
+  <si>
+    <t>medial condyle of femur</t>
+  </si>
+  <si>
+    <t>greater trochanter</t>
+  </si>
+  <si>
+    <t>head of femur</t>
   </si>
 </sst>
 </file>
@@ -4918,8 +4933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581405C8-F852-7340-B9C9-201B714E3AD5}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4929,15 +4944,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="C1" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>117</v>
@@ -4945,10 +4960,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4956,12 +4971,12 @@
         <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>119</v>
@@ -4969,26 +4984,26 @@
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="3" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="C6" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="3" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D8" t="s">
         <v>1436</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1437</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5044,7 +5059,7 @@
         <v>7500051</v>
       </c>
       <c r="D15" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5052,7 +5067,7 @@
         <v>7500060</v>
       </c>
       <c r="D16" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -5060,7 +5075,7 @@
         <v>7500045</v>
       </c>
       <c r="D17" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="18" spans="3:4">
@@ -5068,7 +5083,7 @@
         <v>7500050</v>
       </c>
       <c r="D18" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
   </sheetData>
@@ -5081,9 +5096,9 @@
   <dimension ref="A1:AD531"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
+      <selection pane="bottomLeft" activeCell="A372" sqref="A372:A526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -19409,10 +19424,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BA4F15-3142-994E-BF8B-16093E97474D}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -19436,7 +19451,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -19490,7 +19505,7 @@
         <v>1318</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D10" si="1">"line that connects "&amp;B7&amp;" and "&amp;C7</f>
+        <f t="shared" ref="D7:D14" si="1">"line that connects "&amp;B7&amp;" and "&amp;C7</f>
         <v>line that connects helix and intertragic notch</v>
       </c>
     </row>
@@ -19541,18 +19556,62 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>1362</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1361</v>
+        <v>1440</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>line that connects trochlea of humerus and ventral tubercle of humerus</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>1363</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1361</v>
+        <v>1441</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>line that connects trochlea of humerus and proximal head of humerus</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>line that connects medial condyle of femur and greater trochanter</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>line that connects medial condyle of femur and head of femur</v>
       </c>
     </row>
   </sheetData>
@@ -20496,13 +20555,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="B2" t="s">
         <v>1199</v>
       </c>
       <c r="C2" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -20513,7 +20572,7 @@
         <v>1199</v>
       </c>
       <c r="C3" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -20521,7 +20580,7 @@
         <v>1250</v>
       </c>
       <c r="C4" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -20529,7 +20588,7 @@
         <v>1249</v>
       </c>
       <c r="C5" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -20537,7 +20596,7 @@
         <v>1247</v>
       </c>
       <c r="C6" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -20545,63 +20604,63 @@
         <v>1248</v>
       </c>
       <c r="C7" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="C8" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="C9" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="C10" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="C11" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="C12" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="C13" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="C14" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -20609,7 +20668,7 @@
         <v>1299</v>
       </c>
       <c r="C15" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -20617,7 +20676,7 @@
         <v>1300</v>
       </c>
       <c r="C16" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -20625,7 +20684,7 @@
         <v>1301</v>
       </c>
       <c r="C17" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -20633,7 +20692,7 @@
         <v>1302</v>
       </c>
       <c r="C18" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -20641,7 +20700,7 @@
         <v>1303</v>
       </c>
       <c r="C19" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -20649,7 +20708,7 @@
         <v>1304</v>
       </c>
       <c r="C20" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -20657,7 +20716,7 @@
         <v>1305</v>
       </c>
       <c r="C21" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -20665,7 +20724,7 @@
         <v>1306</v>
       </c>
       <c r="C22" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -20673,7 +20732,7 @@
         <v>1307</v>
       </c>
       <c r="C23" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -20681,7 +20740,7 @@
         <v>1308</v>
       </c>
       <c r="C24" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -20689,7 +20748,7 @@
         <v>1309</v>
       </c>
       <c r="C25" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -20697,7 +20756,7 @@
         <v>1310</v>
       </c>
       <c r="C26" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -21207,7 +21266,7 @@
         <v>1341</v>
       </c>
       <c r="C42" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="I42" t="s">
         <v>1359</v>
@@ -21331,7 +21390,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="G56" t="s">
         <v>1361</v>
@@ -21339,7 +21398,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="G57" t="s">
         <v>1361</v>
@@ -21347,23 +21406,23 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
+        <v>1366</v>
+      </c>
+      <c r="G58" t="s">
         <v>1368</v>
-      </c>
-      <c r="G58" t="s">
-        <v>1370</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="G59" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="B60" t="s">
         <v>273</v>
@@ -21371,157 +21430,157 @@
     </row>
     <row r="61" spans="1:9">
       <c r="I61" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added molar 1 axis patterns
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32F9E70-2074-4662-947E-33C863E2CDC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA7BB89-EF50-41E0-91C9-05F8F710E7B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3956" uniqueCount="1841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1852">
   <si>
     <t>Status</t>
   </si>
@@ -5635,6 +5635,39 @@
   </si>
   <si>
     <t>Lower primary molar 1 width</t>
+  </si>
+  <si>
+    <t>upper molar 1</t>
+  </si>
+  <si>
+    <t>lower first secondary molar tooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower first primary molar tooth </t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of molar tooth 1</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper molar 1</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower first secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper first secondary molar tooth</t>
+  </si>
+  <si>
+    <t>upper first secondary molar tooth</t>
+  </si>
+  <si>
+    <t>upper first primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper first primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of first primary molar tooth</t>
   </si>
 </sst>
 </file>
@@ -20284,8 +20317,8 @@
   <dimension ref="A1:D313"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A144" sqref="A144"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -22309,35 +22342,86 @@
       <c r="C137" t="s">
         <v>1834</v>
       </c>
+      <c r="D137" t="s">
+        <v>1844</v>
+      </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>1835</v>
       </c>
+      <c r="B138" t="s">
+        <v>108</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1845</v>
+      </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>1836</v>
       </c>
+      <c r="B139" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>1837</v>
       </c>
+      <c r="B140" t="s">
+        <v>108</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1847</v>
+      </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>1838</v>
       </c>
+      <c r="B141" t="s">
+        <v>108</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1849</v>
+      </c>
+      <c r="D141" t="s">
+        <v>1850</v>
+      </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>1839</v>
       </c>
+      <c r="B142" t="s">
+        <v>108</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D142" t="s">
+        <v>1846</v>
+      </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>1840</v>
+      </c>
+      <c r="B143" t="s">
+        <v>108</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1851</v>
       </c>
     </row>
     <row r="154" spans="2:2">

</xml_diff>

<commit_message>
Added molar length and width terms
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA7BB89-EF50-41E0-91C9-05F8F710E7B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA8E22A-EED3-4527-BE77-213C8D72E3FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4155" uniqueCount="1965">
   <si>
     <t>Status</t>
   </si>
@@ -5586,9 +5586,6 @@
     <t>occlusal surface of tooth</t>
   </si>
   <si>
-    <t>Surface of a tooth that contacts another tooth.</t>
-  </si>
-  <si>
     <t>done in fovt</t>
   </si>
   <si>
@@ -5668,6 +5665,348 @@
   </si>
   <si>
     <t>line along medial-lateral axis of first primary molar tooth</t>
+  </si>
+  <si>
+    <t>lower molar 1</t>
+  </si>
+  <si>
+    <t>First molar (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>molar tooth 1' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower molar 1</t>
+  </si>
+  <si>
+    <t>Molar 1 length</t>
+  </si>
+  <si>
+    <t>Upper molar 1 length</t>
+  </si>
+  <si>
+    <t>Lower molar 1 length</t>
+  </si>
+  <si>
+    <t>Upper secondary molar 1 length</t>
+  </si>
+  <si>
+    <t>Upper primary molar 1 length</t>
+  </si>
+  <si>
+    <t>Lower secondary molar 1 length</t>
+  </si>
+  <si>
+    <t>Lower primary molar 1 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of molar tooth 1</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper molar 1</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower molar 1</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper first secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper first primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower first secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower first primary molar tooth</t>
+  </si>
+  <si>
+    <t>Molar 2 width</t>
+  </si>
+  <si>
+    <t>Upper molar 2 width</t>
+  </si>
+  <si>
+    <t>Lower molar 2 width</t>
+  </si>
+  <si>
+    <t>Upper secondary molar 2 width</t>
+  </si>
+  <si>
+    <t>Upper primary molar 2 width</t>
+  </si>
+  <si>
+    <t>Lower secondary molar 2 width</t>
+  </si>
+  <si>
+    <t>Lower primary molar 2 width</t>
+  </si>
+  <si>
+    <t>molar tooth 2</t>
+  </si>
+  <si>
+    <t>upper molar 2</t>
+  </si>
+  <si>
+    <t>Second molar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>molar tooth 2' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>lower molar 2</t>
+  </si>
+  <si>
+    <t>Surface of a tooth that contacts another tooth</t>
+  </si>
+  <si>
+    <t>Second molar (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>molar tooth 2' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>upper second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>lower second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>upper second primary molar tooth</t>
+  </si>
+  <si>
+    <t>lower second primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper molar 2</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower molar 2</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper second primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower second primary molar tooth</t>
+  </si>
+  <si>
+    <t>Molar 2 length</t>
+  </si>
+  <si>
+    <t>Upper molar 2 length</t>
+  </si>
+  <si>
+    <t>Lower molar 2 length</t>
+  </si>
+  <si>
+    <t>Upper secondary molar 2 length</t>
+  </si>
+  <si>
+    <t>Upper primary molar 2 length</t>
+  </si>
+  <si>
+    <t>Lower secondary molar 2 length</t>
+  </si>
+  <si>
+    <t>Lower primary molar 2 length</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of molar tooth 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of molar tooth 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper molar 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower molar 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper second primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower second primary molar tooth</t>
+  </si>
+  <si>
+    <t>Molar 3 width</t>
+  </si>
+  <si>
+    <t>Upper molar 3 width</t>
+  </si>
+  <si>
+    <t>Lower molar 3 width</t>
+  </si>
+  <si>
+    <t>Upper secondary molar 3 width</t>
+  </si>
+  <si>
+    <t>Upper primary molar 3 width</t>
+  </si>
+  <si>
+    <t>Lower secondary molar 3 width</t>
+  </si>
+  <si>
+    <t>Lower primary molar 3 width</t>
+  </si>
+  <si>
+    <t>molar tooth 3</t>
+  </si>
+  <si>
+    <t>lower molar 3</t>
+  </si>
+  <si>
+    <t>lower third secondary molar tooth</t>
+  </si>
+  <si>
+    <t>upper third secondary molar tooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper molar 3 </t>
+  </si>
+  <si>
+    <t>Third molar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>molar tooth 3' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>upper molar 3</t>
+  </si>
+  <si>
+    <t>lower third primary molar tooth</t>
+  </si>
+  <si>
+    <t>upper third primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of molar tooth 3</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper molar 3</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower molar 3</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper third secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper third primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower third secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower third primary molar tooth</t>
+  </si>
+  <si>
+    <t>Molar 3 length</t>
+  </si>
+  <si>
+    <t>Upper molar 3 length</t>
+  </si>
+  <si>
+    <t>Lower molar 3 length</t>
+  </si>
+  <si>
+    <t>Upper primary molar 3 length</t>
+  </si>
+  <si>
+    <t>Upper secondary molar 3 length</t>
+  </si>
+  <si>
+    <t>Lower secondary molar 3 length</t>
+  </si>
+  <si>
+    <t>Lower primary molar 3 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of molar tooth 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper molar 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower molar 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper third secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper third primary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower third secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower third primary molar tooth</t>
+  </si>
+  <si>
+    <t>Molar 4 length</t>
+  </si>
+  <si>
+    <t>Molar 4 width</t>
+  </si>
+  <si>
+    <t>Lower molar 4 width</t>
+  </si>
+  <si>
+    <t>Upper molar 4 width</t>
+  </si>
+  <si>
+    <t>upper molar 4</t>
+  </si>
+  <si>
+    <t>lower molar 4</t>
+  </si>
+  <si>
+    <t>Fourth molar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>Fourth molar (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>molar tooth 4' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>molar tooth 4' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of molar tooth 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper molar 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower molar 4</t>
+  </si>
+  <si>
+    <t>Upper molar 4 length</t>
+  </si>
+  <si>
+    <t>Lower molar 4 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of molar tooth 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper molar 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower molar 4</t>
   </si>
 </sst>
 </file>
@@ -6348,19 +6687,19 @@
     <row r="20" spans="1:4">
       <c r="A20" s="11"/>
       <c r="B20" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="25"/>
       <c r="B21" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="26"/>
       <c r="B22" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -6376,9 +6715,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
+      <selection pane="bottomLeft" activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6453,7 +6792,7 @@
         <v>994</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -6507,7 +6846,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
@@ -6553,7 +6892,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -6595,7 +6934,7 @@
         <v>343</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -6622,7 +6961,7 @@
     <row r="6" spans="1:30" s="11" customFormat="1">
       <c r="A6" s="31"/>
       <c r="B6" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
@@ -6658,7 +6997,7 @@
     <row r="7" spans="1:30" s="11" customFormat="1">
       <c r="A7" s="31"/>
       <c r="B7" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -6710,7 +7049,7 @@
     <row r="8" spans="1:30" s="11" customFormat="1">
       <c r="A8" s="31"/>
       <c r="B8" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -6764,7 +7103,7 @@
         <v>995</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6808,7 +7147,7 @@
     <row r="10" spans="1:30">
       <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6852,7 +7191,7 @@
     <row r="11" spans="1:30">
       <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6896,7 +7235,7 @@
     <row r="12" spans="1:30" s="26" customFormat="1">
       <c r="A12" s="31"/>
       <c r="B12" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -6904,7 +7243,7 @@
         <v>15</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
@@ -6940,7 +7279,7 @@
     <row r="13" spans="1:30" s="26" customFormat="1">
       <c r="A13" s="31"/>
       <c r="B13" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -6948,7 +7287,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G13" s="29"/>
       <c r="H13" s="28"/>
@@ -6984,7 +7323,7 @@
     <row r="14" spans="1:30" s="11" customFormat="1">
       <c r="A14" s="31"/>
       <c r="B14" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -7034,7 +7373,7 @@
     <row r="15" spans="1:30" s="11" customFormat="1">
       <c r="A15" s="31"/>
       <c r="B15" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -7082,7 +7421,7 @@
     <row r="16" spans="1:30" s="26" customFormat="1">
       <c r="A16" s="31"/>
       <c r="B16" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -7126,7 +7465,7 @@
     <row r="17" spans="1:30" s="11" customFormat="1">
       <c r="A17" s="31"/>
       <c r="B17" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -7178,7 +7517,7 @@
     <row r="18" spans="1:30" s="11" customFormat="1">
       <c r="A18" s="31"/>
       <c r="B18" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C18" s="10"/>
       <c r="F18" s="10" t="s">
@@ -7462,7 +7801,7 @@
     <row r="30" spans="1:30">
       <c r="A30" s="31"/>
       <c r="B30" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -7506,7 +7845,7 @@
     <row r="31" spans="1:30">
       <c r="A31" s="31"/>
       <c r="B31" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -7550,7 +7889,7 @@
     <row r="32" spans="1:30">
       <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -7594,7 +7933,7 @@
     <row r="33" spans="1:30" s="26" customFormat="1">
       <c r="A33" s="31"/>
       <c r="B33" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C33" s="28"/>
       <c r="D33" s="28"/>
@@ -7640,7 +7979,7 @@
     <row r="34" spans="1:30" s="26" customFormat="1">
       <c r="A34" s="31"/>
       <c r="B34" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C34" s="28"/>
       <c r="D34" s="28"/>
@@ -7686,7 +8025,7 @@
     <row r="35" spans="1:30" s="11" customFormat="1">
       <c r="A35" s="31"/>
       <c r="B35" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -7738,7 +8077,7 @@
     <row r="36" spans="1:30" s="11" customFormat="1">
       <c r="A36" s="31"/>
       <c r="B36" s="10" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -8264,7 +8603,7 @@
         <v>997</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -8308,7 +8647,7 @@
     <row r="54" spans="1:30">
       <c r="A54" s="31"/>
       <c r="B54" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -8352,7 +8691,7 @@
     <row r="55" spans="1:30">
       <c r="A55" s="31"/>
       <c r="B55" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -8396,10 +8735,10 @@
     <row r="56" spans="1:30" s="26" customFormat="1">
       <c r="A56" s="31"/>
       <c r="B56" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D56" s="28"/>
       <c r="E56" s="28" t="s">
@@ -8444,10 +8783,10 @@
     <row r="57" spans="1:30" s="26" customFormat="1">
       <c r="A57" s="31"/>
       <c r="B57" s="28" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D57" s="28"/>
       <c r="E57" s="28" t="s">
@@ -9276,7 +9615,7 @@
         <v>998</v>
       </c>
       <c r="B84" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="C84" s="17"/>
       <c r="E84" s="3" t="s">
@@ -9312,7 +9651,7 @@
     <row r="85" spans="1:21">
       <c r="A85" s="32"/>
       <c r="B85" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="C85" s="17"/>
       <c r="E85" s="3" t="s">
@@ -9352,7 +9691,7 @@
         <v>15</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3" t="s">
@@ -9424,7 +9763,7 @@
         <v>15</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2" t="s">
@@ -9498,7 +9837,7 @@
         <v>15</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2" t="s">
@@ -9574,7 +9913,7 @@
         <v>15</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3" t="s">
@@ -9646,7 +9985,7 @@
         <v>15</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3" t="s">
@@ -9782,7 +10121,7 @@
         <v>15</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="3" t="s">
@@ -11913,7 +12252,7 @@
         <v>1002</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -11959,7 +12298,7 @@
     <row r="177" spans="1:30">
       <c r="A177" s="31"/>
       <c r="B177" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -12002,7 +12341,7 @@
     <row r="178" spans="1:30">
       <c r="A178" s="31"/>
       <c r="B178" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -12048,7 +12387,7 @@
     <row r="179" spans="1:30">
       <c r="A179" s="31"/>
       <c r="B179" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -12096,7 +12435,7 @@
     <row r="180" spans="1:30">
       <c r="A180" s="31"/>
       <c r="B180" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -12297,9 +12636,7 @@
     </row>
     <row r="187" spans="1:30" s="11" customFormat="1">
       <c r="A187" s="31"/>
-      <c r="C187" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C187" s="10"/>
       <c r="E187" s="9" t="s">
         <v>343</v>
       </c>
@@ -12336,9 +12673,7 @@
     </row>
     <row r="188" spans="1:30" s="11" customFormat="1">
       <c r="A188" s="31"/>
-      <c r="C188" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C188" s="10"/>
       <c r="E188" s="9" t="s">
         <v>343</v>
       </c>
@@ -12375,9 +12710,7 @@
     </row>
     <row r="189" spans="1:30" s="11" customFormat="1">
       <c r="A189" s="31"/>
-      <c r="C189" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C189" s="10"/>
       <c r="E189" s="9" t="s">
         <v>343</v>
       </c>
@@ -12414,9 +12747,7 @@
     </row>
     <row r="190" spans="1:30" s="11" customFormat="1">
       <c r="A190" s="31"/>
-      <c r="C190" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C190" s="10"/>
       <c r="E190" s="9" t="s">
         <v>343</v>
       </c>
@@ -12766,7 +13097,7 @@
     <row r="199" spans="1:30">
       <c r="A199" s="31"/>
       <c r="B199" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
@@ -12814,7 +13145,7 @@
     <row r="200" spans="1:30">
       <c r="A200" s="31"/>
       <c r="B200" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
@@ -12860,7 +13191,7 @@
     <row r="201" spans="1:30">
       <c r="A201" s="31"/>
       <c r="B201" s="1" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -20314,11 +20645,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D313"/>
+  <dimension ref="A1:D309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D144" sqref="D144"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -22334,213 +22665,788 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B137" t="s">
         <v>108</v>
       </c>
       <c r="C137" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D137" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B138" t="s">
         <v>108</v>
       </c>
       <c r="C138" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D138" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="B139" t="s">
         <v>108</v>
       </c>
+      <c r="C139" t="s">
+        <v>1851</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1854</v>
+      </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="B140" t="s">
         <v>108</v>
       </c>
       <c r="C140" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="D140" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="B141" t="s">
         <v>108</v>
       </c>
       <c r="C141" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D141" t="s">
         <v>1849</v>
-      </c>
-      <c r="D141" t="s">
-        <v>1850</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B142" t="s">
         <v>108</v>
       </c>
       <c r="C142" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D142" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="B143" t="s">
         <v>108</v>
       </c>
       <c r="C143" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="D143" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B144" t="s">
+        <v>112</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B145" t="s">
+        <v>112</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1840</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B146" t="s">
+        <v>112</v>
+      </c>
+      <c r="C146" t="s">
         <v>1851</v>
       </c>
-    </row>
-    <row r="154" spans="2:2">
-      <c r="B154" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4">
+      <c r="D146" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B147" t="s">
+        <v>112</v>
+      </c>
+      <c r="C147" t="s">
+        <v>1847</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B148" t="s">
+        <v>112</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B149" t="s">
+        <v>112</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D149" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B150" t="s">
+        <v>112</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B151" t="s">
+        <v>108</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1876</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B152" t="s">
+        <v>108</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D152" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B153" t="s">
+        <v>108</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1880</v>
+      </c>
+      <c r="D153" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B154" t="s">
+        <v>108</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1884</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B155" t="s">
+        <v>108</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B156" t="s">
+        <v>108</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1885</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B157" t="s">
+        <v>108</v>
+      </c>
+      <c r="C157" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D157" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B158" t="s">
+        <v>112</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1876</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B159" t="s">
+        <v>112</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B160" t="s">
+        <v>112</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1880</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B161" t="s">
+        <v>112</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1884</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B162" t="s">
+        <v>112</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B163" t="s">
+        <v>112</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1885</v>
+      </c>
+      <c r="D163" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B164" t="s">
+        <v>112</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D164" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B165" t="s">
+        <v>108</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1916</v>
+      </c>
+      <c r="D165" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B166" t="s">
+        <v>108</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D166" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B167" t="s">
+        <v>108</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D167" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B168" t="s">
+        <v>108</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B169" t="s">
+        <v>108</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B170" t="s">
+        <v>108</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1918</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B171" t="s">
+        <v>108</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1924</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B172" t="s">
+        <v>112</v>
+      </c>
+      <c r="C172" t="s">
+        <v>1916</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B173" t="s">
+        <v>112</v>
+      </c>
+      <c r="C173" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B174" t="s">
+        <v>112</v>
+      </c>
+      <c r="C174" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D174" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B175" t="s">
+        <v>112</v>
+      </c>
+      <c r="C175" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D175" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B176" t="s">
+        <v>112</v>
+      </c>
+      <c r="C176" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D176" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B177" t="s">
+        <v>112</v>
+      </c>
+      <c r="C177" t="s">
+        <v>1918</v>
+      </c>
+      <c r="D177" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B178" t="s">
+        <v>112</v>
+      </c>
+      <c r="C178" t="s">
+        <v>1924</v>
+      </c>
+      <c r="D178" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B179" t="s">
+        <v>108</v>
+      </c>
+      <c r="C179" t="s">
+        <v>67</v>
+      </c>
+      <c r="D179" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B180" t="s">
+        <v>108</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1951</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B181" t="s">
+        <v>108</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D181" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B182" t="s">
+        <v>112</v>
+      </c>
+      <c r="C182" t="s">
+        <v>67</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B183" t="s">
+        <v>112</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1951</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B184" t="s">
+        <v>112</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="A285" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B285" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C285" s="22" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D285" t="str">
+        <f>"line along "&amp;B285&amp;" of "&amp;C285</f>
+        <v>line along proximal-distal of lateral side' some talus</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="A286" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B286" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D286" t="str">
+        <f>"line along "&amp;B286&amp;" of "&amp;C286</f>
+        <v>line along proximal-distal of pes</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="A287" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B289" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C289" s="22" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D289" t="str">
-        <f>"line along "&amp;B289&amp;" of "&amp;C289</f>
-        <v>line along proximal-distal of lateral side' some talus</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B290" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C290" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D290" t="str">
-        <f>"line along "&amp;B290&amp;" of "&amp;C290</f>
-        <v>line along proximal-distal of pes</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="295" spans="1:4">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="296" spans="1:4">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="297" spans="1:4">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4">
-      <c r="A298" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="299" spans="1:4">
-      <c r="A299" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="300" spans="1:4">
-      <c r="A300" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4">
-      <c r="A301" t="s">
         <v>537</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" s="1" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" s="1" t="s">
+        <v>1129</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" s="1" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" s="1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1">
-      <c r="A310" s="1" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1">
-      <c r="A311" s="1" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1">
-      <c r="A312" s="1" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="313" spans="1:1">
-      <c r="A313" s="1" t="s">
         <v>630</v>
       </c>
     </row>
@@ -22552,18 +23458,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.875" customWidth="1"/>
+    <col min="4" max="4" width="44.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1103</v>
       </c>
@@ -22573,8 +23481,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1272</v>
       </c>
@@ -22585,7 +23496,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1131</v>
       </c>
@@ -22596,7 +23507,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>1805</v>
       </c>
@@ -22604,7 +23515,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>1807</v>
       </c>
@@ -22612,7 +23523,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>1806</v>
       </c>
@@ -22620,7 +23531,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>1804</v>
       </c>
@@ -22628,7 +23539,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>1808</v>
       </c>
@@ -22636,7 +23547,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>1157</v>
       </c>
@@ -22644,7 +23555,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>1156</v>
       </c>
@@ -22652,7 +23563,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>1154</v>
       </c>
@@ -22660,7 +23571,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>1155</v>
       </c>
@@ -22668,7 +23579,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>1267</v>
       </c>
@@ -22676,7 +23587,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>1276</v>
       </c>
@@ -22684,7 +23595,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>1268</v>
       </c>
@@ -22692,7 +23603,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>1269</v>
       </c>
@@ -22828,7 +23739,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>1200</v>
       </c>
@@ -22836,7 +23747,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>1821</v>
       </c>
@@ -22844,7 +23755,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>1208</v>
       </c>
@@ -22852,12 +23763,88 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>1823</v>
       </c>
       <c r="C38" t="s">
-        <v>1824</v>
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1878</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1882</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>1920</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1921</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1953</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1954</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>1956</v>
       </c>
     </row>
   </sheetData>
@@ -22870,7 +23857,7 @@
   <dimension ref="A1:X195"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added premolar 1-3 lengths and widths
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA8E22A-EED3-4527-BE77-213C8D72E3FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F33B23F-6FE8-4ED1-B3DA-E822C982B25C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4155" uniqueCount="1965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="2074">
   <si>
     <t>Status</t>
   </si>
@@ -6007,6 +6007,333 @@
   </si>
   <si>
     <t>line along anterior-posterior axis of lower molar 4</t>
+  </si>
+  <si>
+    <t>premolar 1</t>
+  </si>
+  <si>
+    <t>Premolar 1 width</t>
+  </si>
+  <si>
+    <t>Upper premolar 1 width</t>
+  </si>
+  <si>
+    <t>Lower premolar 1 width</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 1 width</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 1 width</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 1 width</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 1 width</t>
+  </si>
+  <si>
+    <t>lower premolar 1</t>
+  </si>
+  <si>
+    <t>upper first secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>upper first primary premolar tooth</t>
+  </si>
+  <si>
+    <t>lower first secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>lower first primary premolar tooth</t>
+  </si>
+  <si>
+    <t>upper premolar 1</t>
+  </si>
+  <si>
+    <t>First premolar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>premolar tooth 1' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of premolar 1</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper premolar 1</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower premolar 1</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper first secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper first primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower first secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower first primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 1 length</t>
+  </si>
+  <si>
+    <t>Upper premolar 1 length</t>
+  </si>
+  <si>
+    <t>Lower premolar 1 length</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 1 length</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 1 length</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 1 length</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 1 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar 1</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar 1</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar 1</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper first secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper first primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower first secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower first primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 2 width</t>
+  </si>
+  <si>
+    <t>Upper premolar 2 width</t>
+  </si>
+  <si>
+    <t>Lower premolar 2 width</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 2 width</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 2 width</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 2 width</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 2 width</t>
+  </si>
+  <si>
+    <t>premolar 2</t>
+  </si>
+  <si>
+    <t>upper premolar 2</t>
+  </si>
+  <si>
+    <t>lower premolar 2</t>
+  </si>
+  <si>
+    <t>lower second secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>upper second secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>Second premolar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>upper second primary premolar tooth</t>
+  </si>
+  <si>
+    <t>lower second primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of premolar 2</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper premolar 2</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower premolar 2</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper second secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper second primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower second secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower second primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 2 length</t>
+  </si>
+  <si>
+    <t>Upper premolar 2 length</t>
+  </si>
+  <si>
+    <t>Lower premolar 2 length</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 2 length</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 2 length</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 2 length</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 2 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar 2</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper second secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper second primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower second secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower second primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 3 width</t>
+  </si>
+  <si>
+    <t>Upper premolar 3 width</t>
+  </si>
+  <si>
+    <t>Lower premolar 3 width</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 3 width</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 3 width</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 3 width</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 3 width</t>
+  </si>
+  <si>
+    <t>upper premolar 3</t>
+  </si>
+  <si>
+    <t>lower premolar 3</t>
+  </si>
+  <si>
+    <t>Third premolar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>premolar tooth 2' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>premolar tooth 3' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>Third premolar (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>upper third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>lower third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of premolar 3</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper premolar 3</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower premolar 3</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper third secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower third secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 3 length</t>
+  </si>
+  <si>
+    <t>Upper premolar 3 length</t>
+  </si>
+  <si>
+    <t>Lower premolar 3 length</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 3 length</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 3 length</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 3 length</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 3 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper third secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower third secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower third primary premolar tooth</t>
   </si>
 </sst>
 </file>
@@ -6715,9 +7042,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C191" sqref="C191"/>
+      <selection pane="bottomLeft" activeCell="C202" sqref="C202:C205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12784,9 +13111,7 @@
     </row>
     <row r="191" spans="1:30" s="11" customFormat="1">
       <c r="A191" s="31"/>
-      <c r="C191" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C191" s="10"/>
       <c r="E191" s="9" t="s">
         <v>343</v>
       </c>
@@ -12823,9 +13148,7 @@
     </row>
     <row r="192" spans="1:30" s="11" customFormat="1">
       <c r="A192" s="31"/>
-      <c r="C192" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C192" s="10"/>
       <c r="E192" s="9" t="s">
         <v>343</v>
       </c>
@@ -12862,9 +13185,7 @@
     </row>
     <row r="193" spans="1:30" s="11" customFormat="1">
       <c r="A193" s="31"/>
-      <c r="C193" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C193" s="10"/>
       <c r="E193" s="9" t="s">
         <v>343</v>
       </c>
@@ -12901,9 +13222,7 @@
     </row>
     <row r="194" spans="1:30" s="11" customFormat="1">
       <c r="A194" s="31"/>
-      <c r="C194" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C194" s="10"/>
       <c r="E194" s="9" t="s">
         <v>343</v>
       </c>
@@ -12940,9 +13259,7 @@
     </row>
     <row r="195" spans="1:30" s="11" customFormat="1">
       <c r="A195" s="31"/>
-      <c r="C195" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C195" s="10"/>
       <c r="E195" s="9" t="s">
         <v>343</v>
       </c>
@@ -12979,9 +13296,7 @@
     </row>
     <row r="196" spans="1:30" s="11" customFormat="1">
       <c r="A196" s="31"/>
-      <c r="C196" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C196" s="10"/>
       <c r="E196" s="9" t="s">
         <v>343</v>
       </c>
@@ -13018,9 +13333,7 @@
     </row>
     <row r="197" spans="1:30" s="11" customFormat="1">
       <c r="A197" s="31"/>
-      <c r="C197" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C197" s="10"/>
       <c r="E197" s="9" t="s">
         <v>343</v>
       </c>
@@ -13057,9 +13370,7 @@
     </row>
     <row r="198" spans="1:30" s="11" customFormat="1">
       <c r="A198" s="31"/>
-      <c r="C198" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C198" s="10"/>
       <c r="E198" s="9" t="s">
         <v>343</v>
       </c>
@@ -20648,8 +20959,8 @@
   <dimension ref="A1:D309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D185" sqref="D185"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D227" sqref="D227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -23335,6 +23646,594 @@
         <v>1964</v>
       </c>
     </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B185" t="s">
+        <v>108</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B186" t="s">
+        <v>108</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1978</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B187" t="s">
+        <v>108</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B188" t="s">
+        <v>108</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B189" t="s">
+        <v>108</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D189" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B190" t="s">
+        <v>108</v>
+      </c>
+      <c r="C190" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D190" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B191" t="s">
+        <v>108</v>
+      </c>
+      <c r="C191" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D191" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B192" t="s">
+        <v>112</v>
+      </c>
+      <c r="C192" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D192" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B193" t="s">
+        <v>112</v>
+      </c>
+      <c r="C193" t="s">
+        <v>1978</v>
+      </c>
+      <c r="D193" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B194" t="s">
+        <v>112</v>
+      </c>
+      <c r="C194" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D194" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B195" t="s">
+        <v>112</v>
+      </c>
+      <c r="C195" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D195" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B196" t="s">
+        <v>112</v>
+      </c>
+      <c r="C196" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D196" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B197" t="s">
+        <v>112</v>
+      </c>
+      <c r="C197" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D197" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B198" t="s">
+        <v>112</v>
+      </c>
+      <c r="C198" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D198" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B199" t="s">
+        <v>108</v>
+      </c>
+      <c r="C199" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D199" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B200" t="s">
+        <v>108</v>
+      </c>
+      <c r="C200" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D200" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B201" t="s">
+        <v>108</v>
+      </c>
+      <c r="C201" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D201" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B202" t="s">
+        <v>108</v>
+      </c>
+      <c r="C202" t="s">
+        <v>2013</v>
+      </c>
+      <c r="D202" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B203" t="s">
+        <v>108</v>
+      </c>
+      <c r="C203" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D203" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B204" t="s">
+        <v>108</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D204" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B205" t="s">
+        <v>108</v>
+      </c>
+      <c r="C205" t="s">
+        <v>2016</v>
+      </c>
+      <c r="D205" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B206" t="s">
+        <v>112</v>
+      </c>
+      <c r="C206" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D206" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="s">
+        <v>2025</v>
+      </c>
+      <c r="B207" t="s">
+        <v>112</v>
+      </c>
+      <c r="C207" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D207" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B208" t="s">
+        <v>112</v>
+      </c>
+      <c r="C208" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D208" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B209" t="s">
+        <v>112</v>
+      </c>
+      <c r="C209" t="s">
+        <v>2013</v>
+      </c>
+      <c r="D209" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B210" t="s">
+        <v>112</v>
+      </c>
+      <c r="C210" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D210" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" t="s">
+        <v>2029</v>
+      </c>
+      <c r="B211" t="s">
+        <v>112</v>
+      </c>
+      <c r="C211" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D211" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B212" t="s">
+        <v>112</v>
+      </c>
+      <c r="C212" t="s">
+        <v>2016</v>
+      </c>
+      <c r="D212" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" t="s">
+        <v>2038</v>
+      </c>
+      <c r="B213" t="s">
+        <v>108</v>
+      </c>
+      <c r="C213" t="s">
+        <v>74</v>
+      </c>
+      <c r="D213" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" t="s">
+        <v>2039</v>
+      </c>
+      <c r="B214" t="s">
+        <v>108</v>
+      </c>
+      <c r="C214" t="s">
+        <v>2045</v>
+      </c>
+      <c r="D214" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B215" t="s">
+        <v>108</v>
+      </c>
+      <c r="C215" t="s">
+        <v>2046</v>
+      </c>
+      <c r="D215" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" t="s">
+        <v>2041</v>
+      </c>
+      <c r="B216" t="s">
+        <v>108</v>
+      </c>
+      <c r="C216" t="s">
+        <v>104</v>
+      </c>
+      <c r="D216" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B217" t="s">
+        <v>108</v>
+      </c>
+      <c r="C217" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D217" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" t="s">
+        <v>2043</v>
+      </c>
+      <c r="B218" t="s">
+        <v>108</v>
+      </c>
+      <c r="C218" t="s">
+        <v>63</v>
+      </c>
+      <c r="D218" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" t="s">
+        <v>2044</v>
+      </c>
+      <c r="B219" t="s">
+        <v>108</v>
+      </c>
+      <c r="C219" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D219" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B220" t="s">
+        <v>112</v>
+      </c>
+      <c r="C220" t="s">
+        <v>74</v>
+      </c>
+      <c r="D220" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" t="s">
+        <v>2061</v>
+      </c>
+      <c r="B221" t="s">
+        <v>112</v>
+      </c>
+      <c r="C221" t="s">
+        <v>2045</v>
+      </c>
+      <c r="D221" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" t="s">
+        <v>2062</v>
+      </c>
+      <c r="B222" t="s">
+        <v>112</v>
+      </c>
+      <c r="C222" t="s">
+        <v>2046</v>
+      </c>
+      <c r="D222" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B223" t="s">
+        <v>112</v>
+      </c>
+      <c r="C223" t="s">
+        <v>104</v>
+      </c>
+      <c r="D223" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B224" t="s">
+        <v>112</v>
+      </c>
+      <c r="C224" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D224" t="s">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" t="s">
+        <v>2065</v>
+      </c>
+      <c r="B225" t="s">
+        <v>112</v>
+      </c>
+      <c r="C225" t="s">
+        <v>63</v>
+      </c>
+      <c r="D225" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B226" t="s">
+        <v>112</v>
+      </c>
+      <c r="C226" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D226" t="s">
+        <v>2073</v>
+      </c>
+    </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
         <v>1230</v>
@@ -23458,16 +24357,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.875" customWidth="1"/>
+    <col min="3" max="3" width="51.5" customWidth="1"/>
     <col min="4" max="4" width="44.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23845,6 +24744,80 @@
       </c>
       <c r="D46" s="22" t="s">
         <v>1956</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>2052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added premolar 4-5 lengths and widths
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F33B23F-6FE8-4ED1-B3DA-E822C982B25C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D41F9F-244F-4E8B-9B96-3E6DEF6E0BAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="2074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="2142">
   <si>
     <t>Status</t>
   </si>
@@ -6334,6 +6334,210 @@
   </si>
   <si>
     <t>line along anterior-posterior axis of lower third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 4 width</t>
+  </si>
+  <si>
+    <t>Upper premolar 4 width</t>
+  </si>
+  <si>
+    <t>Lower premolar 4 width</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 4 width</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 4 width</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 4 width</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 4 width</t>
+  </si>
+  <si>
+    <t>premolar tooth 4</t>
+  </si>
+  <si>
+    <t>upper premolar 4</t>
+  </si>
+  <si>
+    <t>lower premolar 4</t>
+  </si>
+  <si>
+    <t>upper fourth primary premolar tooth</t>
+  </si>
+  <si>
+    <t>lower fourth primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Fourth premolar (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>premolar tooth 4' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of premolar tooth 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper premolar 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower premolar 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper fourth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper fourth primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower fourth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower fourth primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 4 length</t>
+  </si>
+  <si>
+    <t>Upper premolar 4 length</t>
+  </si>
+  <si>
+    <t>Lower premolar 4 length</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 4 length</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 4 length</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 4 length</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 4 length</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar tooth 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper fourth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper fourth primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower fourth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower fourth primary premolar tooth</t>
+  </si>
+  <si>
+    <t>Premolar 5 width</t>
+  </si>
+  <si>
+    <t>Upper premolar 5 width</t>
+  </si>
+  <si>
+    <t>Lower premolar 5 width</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 5 width</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 5 width</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 5 width</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 5 width</t>
+  </si>
+  <si>
+    <t>premolar tooth 5</t>
+  </si>
+  <si>
+    <t>lower deciduous premolar 5</t>
+  </si>
+  <si>
+    <t>upper deciduous premolar 5</t>
+  </si>
+  <si>
+    <t>upper premolar 5</t>
+  </si>
+  <si>
+    <t>lower premolar 5</t>
+  </si>
+  <si>
+    <t>upper fifth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>lower fifth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>Fifth premolar (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>Fifth premolar (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>premolar tooth 5' and ('part of ' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>premolar tooth 3' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>premolar tooth 5' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of premolar tooth 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper premolar 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower premolar 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper fifth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper deciduous premolar 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower fifth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower deciduous premolar 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar tooth 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper deciduous premolar 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower deciduous premolar 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper fifth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower fifth secondary premolar tooth</t>
   </si>
 </sst>
 </file>
@@ -7042,9 +7246,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C202" sqref="C202:C205"/>
+      <selection pane="bottomLeft" activeCell="I213" sqref="I213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -13547,9 +13751,7 @@
     </row>
     <row r="202" spans="1:30" s="11" customFormat="1">
       <c r="A202" s="31"/>
-      <c r="C202" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C202" s="10"/>
       <c r="E202" s="9" t="s">
         <v>343</v>
       </c>
@@ -13586,9 +13788,7 @@
     </row>
     <row r="203" spans="1:30" s="11" customFormat="1">
       <c r="A203" s="31"/>
-      <c r="C203" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C203" s="10"/>
       <c r="E203" s="9" t="s">
         <v>343</v>
       </c>
@@ -13625,9 +13825,7 @@
     </row>
     <row r="204" spans="1:30" s="11" customFormat="1">
       <c r="A204" s="31"/>
-      <c r="C204" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C204" s="10"/>
       <c r="E204" s="9" t="s">
         <v>343</v>
       </c>
@@ -13664,9 +13862,7 @@
     </row>
     <row r="205" spans="1:30" s="11" customFormat="1">
       <c r="A205" s="31"/>
-      <c r="C205" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C205" s="10"/>
       <c r="E205" s="9" t="s">
         <v>343</v>
       </c>
@@ -13703,9 +13899,7 @@
     </row>
     <row r="206" spans="1:30" s="11" customFormat="1">
       <c r="A206" s="31"/>
-      <c r="C206" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C206" s="10"/>
       <c r="E206" s="9" t="s">
         <v>343</v>
       </c>
@@ -13730,9 +13924,7 @@
     </row>
     <row r="207" spans="1:30" s="11" customFormat="1">
       <c r="A207" s="31"/>
-      <c r="C207" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C207" s="10"/>
       <c r="E207" s="9" t="s">
         <v>343</v>
       </c>
@@ -13757,9 +13949,7 @@
     </row>
     <row r="208" spans="1:30" s="11" customFormat="1">
       <c r="A208" s="31"/>
-      <c r="C208" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C208" s="10"/>
       <c r="E208" s="9" t="s">
         <v>343</v>
       </c>
@@ -13796,9 +13986,7 @@
     </row>
     <row r="209" spans="1:21" s="11" customFormat="1">
       <c r="A209" s="31"/>
-      <c r="C209" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C209" s="10"/>
       <c r="E209" s="9" t="s">
         <v>343</v>
       </c>
@@ -13835,9 +14023,7 @@
     </row>
     <row r="210" spans="1:21" s="11" customFormat="1">
       <c r="A210" s="31"/>
-      <c r="C210" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C210" s="10"/>
       <c r="E210" s="9" t="s">
         <v>343</v>
       </c>
@@ -13874,9 +14060,7 @@
     </row>
     <row r="211" spans="1:21" s="11" customFormat="1">
       <c r="A211" s="31"/>
-      <c r="C211" s="10" t="s">
-        <v>983</v>
-      </c>
+      <c r="C211" s="10"/>
       <c r="E211" s="9" t="s">
         <v>343</v>
       </c>
@@ -20959,8 +21143,8 @@
   <dimension ref="A1:D309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D227" sqref="D227"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A255" sqref="A255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -24234,6 +24418,398 @@
         <v>2073</v>
       </c>
     </row>
+    <row r="227" spans="1:4">
+      <c r="A227" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B227" t="s">
+        <v>108</v>
+      </c>
+      <c r="C227" t="s">
+        <v>2081</v>
+      </c>
+      <c r="D227" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B228" t="s">
+        <v>108</v>
+      </c>
+      <c r="C228" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D228" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B229" t="s">
+        <v>108</v>
+      </c>
+      <c r="C229" t="s">
+        <v>2083</v>
+      </c>
+      <c r="D229" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B230" t="s">
+        <v>108</v>
+      </c>
+      <c r="C230" t="s">
+        <v>100</v>
+      </c>
+      <c r="D230" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B231" t="s">
+        <v>108</v>
+      </c>
+      <c r="C231" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D231" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B232" t="s">
+        <v>108</v>
+      </c>
+      <c r="C232" t="s">
+        <v>59</v>
+      </c>
+      <c r="D232" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B233" t="s">
+        <v>108</v>
+      </c>
+      <c r="C233" t="s">
+        <v>2085</v>
+      </c>
+      <c r="D233" t="s">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B234" t="s">
+        <v>112</v>
+      </c>
+      <c r="C234" t="s">
+        <v>2081</v>
+      </c>
+      <c r="D234" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B235" t="s">
+        <v>112</v>
+      </c>
+      <c r="C235" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D235" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B236" t="s">
+        <v>112</v>
+      </c>
+      <c r="C236" t="s">
+        <v>2083</v>
+      </c>
+      <c r="D236" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B237" t="s">
+        <v>112</v>
+      </c>
+      <c r="C237" t="s">
+        <v>100</v>
+      </c>
+      <c r="D237" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B238" t="s">
+        <v>112</v>
+      </c>
+      <c r="C238" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D238" t="s">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B239" t="s">
+        <v>112</v>
+      </c>
+      <c r="C239" t="s">
+        <v>59</v>
+      </c>
+      <c r="D239" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" t="s">
+        <v>2101</v>
+      </c>
+      <c r="B240" t="s">
+        <v>112</v>
+      </c>
+      <c r="C240" t="s">
+        <v>2085</v>
+      </c>
+      <c r="D240" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" t="s">
+        <v>2109</v>
+      </c>
+      <c r="B241" t="s">
+        <v>108</v>
+      </c>
+      <c r="C241" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D241" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B242" t="s">
+        <v>108</v>
+      </c>
+      <c r="C242" t="s">
+        <v>2119</v>
+      </c>
+      <c r="D242" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B243" t="s">
+        <v>108</v>
+      </c>
+      <c r="C243" t="s">
+        <v>2120</v>
+      </c>
+      <c r="D243" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B244" t="s">
+        <v>108</v>
+      </c>
+      <c r="C244" t="s">
+        <v>2121</v>
+      </c>
+      <c r="D244" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" t="s">
+        <v>2113</v>
+      </c>
+      <c r="B245" t="s">
+        <v>108</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2118</v>
+      </c>
+      <c r="D245" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B246" t="s">
+        <v>108</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D246" t="s">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247" t="s">
+        <v>2115</v>
+      </c>
+      <c r="B247" t="s">
+        <v>108</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D247" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248" t="s">
+        <v>2109</v>
+      </c>
+      <c r="B248" t="s">
+        <v>112</v>
+      </c>
+      <c r="C248" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D248" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B249" t="s">
+        <v>112</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2119</v>
+      </c>
+      <c r="D249" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B250" t="s">
+        <v>112</v>
+      </c>
+      <c r="C250" t="s">
+        <v>2120</v>
+      </c>
+      <c r="D250" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B251" t="s">
+        <v>112</v>
+      </c>
+      <c r="C251" t="s">
+        <v>2121</v>
+      </c>
+      <c r="D251" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" t="s">
+        <v>2113</v>
+      </c>
+      <c r="B252" t="s">
+        <v>112</v>
+      </c>
+      <c r="C252" t="s">
+        <v>2118</v>
+      </c>
+      <c r="D252" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B253" t="s">
+        <v>112</v>
+      </c>
+      <c r="C253" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D253" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" t="s">
+        <v>2115</v>
+      </c>
+      <c r="B254" t="s">
+        <v>112</v>
+      </c>
+      <c r="C254" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D254" t="s">
+        <v>2139</v>
+      </c>
+    </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
         <v>1230</v>
@@ -24357,10 +24933,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -24807,7 +25383,7 @@
         <v>2050</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>2049</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -24818,6 +25394,59 @@
     <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>2052</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>2083</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2086</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2124</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2123</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>2122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added canine length and width terms
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D41F9F-244F-4E8B-9B96-3E6DEF6E0BAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B574044-9C1E-473E-A905-7716315B4D04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="2142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4529" uniqueCount="2181">
   <si>
     <t>Status</t>
   </si>
@@ -6538,6 +6538,123 @@
   </si>
   <si>
     <t>line along anterior-posterior axis of lower fifth secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>In pattern</t>
+  </si>
+  <si>
+    <t>Canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary canine anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>upper primary canine tooth</t>
+  </si>
+  <si>
+    <t>upper secondary canine tooth</t>
+  </si>
+  <si>
+    <t>lower secondary canine tooth</t>
+  </si>
+  <si>
+    <t>lower primary canine tooth</t>
+  </si>
+  <si>
+    <t>upper canine 1</t>
+  </si>
+  <si>
+    <t>lower canine tooth</t>
+  </si>
+  <si>
+    <t>canine tooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canine </t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior posterior-axis of upper canine 1</t>
+  </si>
+  <si>
+    <t>line along anterior posterior-axis of lower canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior posterior axis of upper secondary canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior posterior axis of upper primary canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior posterior axis of lower secondary canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior posterior axis of lower primary canine tooth</t>
+  </si>
+  <si>
+    <t>Canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary canine medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of canine tooth</t>
+  </si>
+  <si>
+    <t>line along medial lateral-axis of upper canine 1</t>
+  </si>
+  <si>
+    <t>line along medial lateral-axis of lower canine tooth</t>
+  </si>
+  <si>
+    <t>line along medial lateral axis of upper secondary canine tooth</t>
+  </si>
+  <si>
+    <t>line along medial lateral axis of upper primary canine tooth</t>
+  </si>
+  <si>
+    <t>line along medial lateral axis of lower secondary canine tooth</t>
+  </si>
+  <si>
+    <t>line along medial lateral axis of lower primary canine tooth</t>
+  </si>
+  <si>
+    <t>Canine crown height</t>
+  </si>
+  <si>
+    <t>upper-lower axis</t>
   </si>
 </sst>
 </file>
@@ -6647,7 +6764,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6684,6 +6801,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6698,7 +6821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6740,6 +6863,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7246,9 +7370,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I213" sqref="I213"/>
+      <selection pane="bottomLeft" activeCell="J245" sqref="J245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -13167,7 +13291,9 @@
     </row>
     <row r="187" spans="1:30" s="11" customFormat="1">
       <c r="A187" s="31"/>
-      <c r="C187" s="10"/>
+      <c r="C187" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E187" s="9" t="s">
         <v>343</v>
       </c>
@@ -13204,7 +13330,9 @@
     </row>
     <row r="188" spans="1:30" s="11" customFormat="1">
       <c r="A188" s="31"/>
-      <c r="C188" s="10"/>
+      <c r="C188" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E188" s="9" t="s">
         <v>343</v>
       </c>
@@ -13241,7 +13369,9 @@
     </row>
     <row r="189" spans="1:30" s="11" customFormat="1">
       <c r="A189" s="31"/>
-      <c r="C189" s="10"/>
+      <c r="C189" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E189" s="9" t="s">
         <v>343</v>
       </c>
@@ -13278,7 +13408,9 @@
     </row>
     <row r="190" spans="1:30" s="11" customFormat="1">
       <c r="A190" s="31"/>
-      <c r="C190" s="10"/>
+      <c r="C190" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E190" s="9" t="s">
         <v>343</v>
       </c>
@@ -13315,7 +13447,9 @@
     </row>
     <row r="191" spans="1:30" s="11" customFormat="1">
       <c r="A191" s="31"/>
-      <c r="C191" s="10"/>
+      <c r="C191" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E191" s="9" t="s">
         <v>343</v>
       </c>
@@ -13352,7 +13486,9 @@
     </row>
     <row r="192" spans="1:30" s="11" customFormat="1">
       <c r="A192" s="31"/>
-      <c r="C192" s="10"/>
+      <c r="C192" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E192" s="9" t="s">
         <v>343</v>
       </c>
@@ -13389,7 +13525,9 @@
     </row>
     <row r="193" spans="1:30" s="11" customFormat="1">
       <c r="A193" s="31"/>
-      <c r="C193" s="10"/>
+      <c r="C193" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E193" s="9" t="s">
         <v>343</v>
       </c>
@@ -13426,7 +13564,9 @@
     </row>
     <row r="194" spans="1:30" s="11" customFormat="1">
       <c r="A194" s="31"/>
-      <c r="C194" s="10"/>
+      <c r="C194" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E194" s="9" t="s">
         <v>343</v>
       </c>
@@ -13463,7 +13603,9 @@
     </row>
     <row r="195" spans="1:30" s="11" customFormat="1">
       <c r="A195" s="31"/>
-      <c r="C195" s="10"/>
+      <c r="C195" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E195" s="9" t="s">
         <v>343</v>
       </c>
@@ -13500,7 +13642,9 @@
     </row>
     <row r="196" spans="1:30" s="11" customFormat="1">
       <c r="A196" s="31"/>
-      <c r="C196" s="10"/>
+      <c r="C196" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E196" s="9" t="s">
         <v>343</v>
       </c>
@@ -13537,7 +13681,9 @@
     </row>
     <row r="197" spans="1:30" s="11" customFormat="1">
       <c r="A197" s="31"/>
-      <c r="C197" s="10"/>
+      <c r="C197" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E197" s="9" t="s">
         <v>343</v>
       </c>
@@ -13574,7 +13720,9 @@
     </row>
     <row r="198" spans="1:30" s="11" customFormat="1">
       <c r="A198" s="31"/>
-      <c r="C198" s="10"/>
+      <c r="C198" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E198" s="9" t="s">
         <v>343</v>
       </c>
@@ -13751,7 +13899,9 @@
     </row>
     <row r="202" spans="1:30" s="11" customFormat="1">
       <c r="A202" s="31"/>
-      <c r="C202" s="10"/>
+      <c r="C202" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E202" s="9" t="s">
         <v>343</v>
       </c>
@@ -13788,7 +13938,9 @@
     </row>
     <row r="203" spans="1:30" s="11" customFormat="1">
       <c r="A203" s="31"/>
-      <c r="C203" s="10"/>
+      <c r="C203" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E203" s="9" t="s">
         <v>343</v>
       </c>
@@ -13825,7 +13977,9 @@
     </row>
     <row r="204" spans="1:30" s="11" customFormat="1">
       <c r="A204" s="31"/>
-      <c r="C204" s="10"/>
+      <c r="C204" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E204" s="9" t="s">
         <v>343</v>
       </c>
@@ -13862,7 +14016,9 @@
     </row>
     <row r="205" spans="1:30" s="11" customFormat="1">
       <c r="A205" s="31"/>
-      <c r="C205" s="10"/>
+      <c r="C205" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E205" s="9" t="s">
         <v>343</v>
       </c>
@@ -13899,7 +14055,9 @@
     </row>
     <row r="206" spans="1:30" s="11" customFormat="1">
       <c r="A206" s="31"/>
-      <c r="C206" s="10"/>
+      <c r="C206" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E206" s="9" t="s">
         <v>343</v>
       </c>
@@ -13924,7 +14082,9 @@
     </row>
     <row r="207" spans="1:30" s="11" customFormat="1">
       <c r="A207" s="31"/>
-      <c r="C207" s="10"/>
+      <c r="C207" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E207" s="9" t="s">
         <v>343</v>
       </c>
@@ -13949,7 +14109,9 @@
     </row>
     <row r="208" spans="1:30" s="11" customFormat="1">
       <c r="A208" s="31"/>
-      <c r="C208" s="10"/>
+      <c r="C208" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E208" s="9" t="s">
         <v>343</v>
       </c>
@@ -13986,7 +14148,9 @@
     </row>
     <row r="209" spans="1:21" s="11" customFormat="1">
       <c r="A209" s="31"/>
-      <c r="C209" s="10"/>
+      <c r="C209" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E209" s="9" t="s">
         <v>343</v>
       </c>
@@ -14023,7 +14187,9 @@
     </row>
     <row r="210" spans="1:21" s="11" customFormat="1">
       <c r="A210" s="31"/>
-      <c r="C210" s="10"/>
+      <c r="C210" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E210" s="9" t="s">
         <v>343</v>
       </c>
@@ -14060,7 +14226,9 @@
     </row>
     <row r="211" spans="1:21" s="11" customFormat="1">
       <c r="A211" s="31"/>
-      <c r="C211" s="10"/>
+      <c r="C211" s="10" t="s">
+        <v>2142</v>
+      </c>
       <c r="E211" s="9" t="s">
         <v>343</v>
       </c>
@@ -14766,6 +14934,7 @@
     </row>
     <row r="237" spans="1:21">
       <c r="A237" s="31"/>
+      <c r="C237" s="33"/>
       <c r="E237" s="1" t="s">
         <v>15</v>
       </c>
@@ -14799,6 +14968,7 @@
     </row>
     <row r="238" spans="1:21">
       <c r="A238" s="31"/>
+      <c r="C238" s="33"/>
       <c r="E238" s="1" t="s">
         <v>15</v>
       </c>
@@ -14830,6 +15000,7 @@
     </row>
     <row r="239" spans="1:21">
       <c r="A239" s="31"/>
+      <c r="C239" s="33"/>
       <c r="E239" s="1" t="s">
         <v>15</v>
       </c>
@@ -14859,6 +15030,7 @@
     </row>
     <row r="240" spans="1:21">
       <c r="A240" s="31"/>
+      <c r="C240" s="33"/>
       <c r="E240" s="1" t="s">
         <v>15</v>
       </c>
@@ -14888,6 +15060,7 @@
     </row>
     <row r="241" spans="1:21">
       <c r="A241" s="31"/>
+      <c r="C241" s="33"/>
       <c r="E241" s="1" t="s">
         <v>15</v>
       </c>
@@ -14917,6 +15090,7 @@
     </row>
     <row r="242" spans="1:21">
       <c r="A242" s="31"/>
+      <c r="C242" s="33"/>
       <c r="E242" s="1" t="s">
         <v>15</v>
       </c>
@@ -21143,8 +21317,8 @@
   <dimension ref="A1:D309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A255" sqref="A255"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A270" sqref="A270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -24810,6 +24984,210 @@
         <v>2139</v>
       </c>
     </row>
+    <row r="255" spans="1:4">
+      <c r="A255" s="33" t="s">
+        <v>2143</v>
+      </c>
+      <c r="B255" t="s">
+        <v>112</v>
+      </c>
+      <c r="C255" s="33" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D255" t="s">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256" s="33" t="s">
+        <v>2144</v>
+      </c>
+      <c r="B256" t="s">
+        <v>112</v>
+      </c>
+      <c r="C256" s="33" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D256" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" s="33" t="s">
+        <v>2145</v>
+      </c>
+      <c r="B257" t="s">
+        <v>112</v>
+      </c>
+      <c r="C257" s="33" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D257" t="s">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" s="33" t="s">
+        <v>2146</v>
+      </c>
+      <c r="B258" t="s">
+        <v>112</v>
+      </c>
+      <c r="C258" t="s">
+        <v>2151</v>
+      </c>
+      <c r="D258" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" s="33" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B259" t="s">
+        <v>112</v>
+      </c>
+      <c r="C259" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D259" t="s">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" s="33" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B260" t="s">
+        <v>112</v>
+      </c>
+      <c r="C260" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D260" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" s="33" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B261" t="s">
+        <v>112</v>
+      </c>
+      <c r="C261" t="s">
+        <v>2153</v>
+      </c>
+      <c r="D261" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" s="16" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B262" t="s">
+        <v>108</v>
+      </c>
+      <c r="C262" s="33" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D262" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" s="16" t="s">
+        <v>2166</v>
+      </c>
+      <c r="B263" t="s">
+        <v>108</v>
+      </c>
+      <c r="C263" s="33" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D263" t="s">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" s="16" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B264" t="s">
+        <v>108</v>
+      </c>
+      <c r="C264" s="33" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D264" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" s="16" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B265" t="s">
+        <v>108</v>
+      </c>
+      <c r="C265" t="s">
+        <v>2151</v>
+      </c>
+      <c r="D265" t="s">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" s="16" t="s">
+        <v>2169</v>
+      </c>
+      <c r="B266" t="s">
+        <v>108</v>
+      </c>
+      <c r="C266" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D266" t="s">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267" s="16" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B267" t="s">
+        <v>108</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D267" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" s="16" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B268" t="s">
+        <v>108</v>
+      </c>
+      <c r="C268" t="s">
+        <v>2153</v>
+      </c>
+      <c r="D268" t="s">
+        <v>2178</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
+      <c r="A269" s="16" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B269" s="33" t="s">
+        <v>2180</v>
+      </c>
+    </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
         <v>1230</v>
@@ -24933,10 +25311,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -25447,6 +25825,11 @@
     <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>2122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>2157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added questions on Terms sheet
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D2FC11-3605-4B6C-972A-5147E3757306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C5AA66-4F89-4D5F-BC7A-8E082C79575D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -42,24 +42,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={53A7FE65-1F7B-4505-868C-8CB7EF24B36F}</author>
     <author>tc={1796211E-4A4F-425A-9398-FE54A7FB8340}</author>
-    <author>tc={3A0E1335-8615-4DEC-BC8F-1EF90DFAD0D5}</author>
+    <author>tc={EB2EF5AD-17D9-4410-88A0-2E3B0BDD28FB}</author>
   </authors>
   <commentList>
-    <comment ref="H260" authorId="0" shapeId="0" xr:uid="{1796211E-4A4F-425A-9398-FE54A7FB8340}">
+    <comment ref="H234" authorId="0" shapeId="0" xr:uid="{53A7FE65-1F7B-4505-868C-8CB7EF24B36F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    I think these would be skull measurements?</t>
+    How to format these if the teeth included in the tooth row differ?</t>
       </text>
     </comment>
-    <comment ref="H261" authorId="1" shapeId="0" xr:uid="{3A0E1335-8615-4DEC-BC8F-1EF90DFAD0D5}">
+    <comment ref="H260" authorId="1" shapeId="0" xr:uid="{1796211E-4A4F-425A-9398-FE54A7FB8340}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    anterior or posterior to P3?</t>
+    I think these would be skull measurements?
+Reply:
+    this would be a Point AB pattern from the midpoint of another Point AB pattern</t>
+      </text>
+    </comment>
+    <comment ref="H262" authorId="2" shapeId="0" xr:uid="{EB2EF5AD-17D9-4410-88A0-2E3B0BDD28FB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Same with this one</t>
       </text>
     </comment>
   </commentList>
@@ -7098,15 +7109,6 @@
     <t>lower secondary canine to premolar 3 length</t>
   </si>
   <si>
-    <t>anatomical point' and ('posteriormost part of' some 'premolar 3')</t>
-  </si>
-  <si>
-    <t>anatomical point' and ('posteriormost part of' some 'upper third secondary premolar tooth')</t>
-  </si>
-  <si>
-    <t>anatomical point' and ('posteriormost part of' some 'lower third secondary premolar tooth')</t>
-  </si>
-  <si>
     <t>anatomical point' and ('posteriormost part of' some 'canine tooth')</t>
   </si>
   <si>
@@ -7131,9 +7133,6 @@
     <t>anatomical point' and ('posteriormost part of' some 'mandible angular process')</t>
   </si>
   <si>
-    <t>mandibular symphysis to angle length</t>
-  </si>
-  <si>
     <t>Molar 5 length</t>
   </si>
   <si>
@@ -7270,6 +7269,18 @@
   </si>
   <si>
     <t>line along medial-lateral axis of lower molar 5</t>
+  </si>
+  <si>
+    <t>mandibular symphysis to mandibular angle length</t>
+  </si>
+  <si>
+    <t>anatomical point' and ('anteriormost part of' some 'premolar 3')</t>
+  </si>
+  <si>
+    <t>anatomical point' and ('anteriormost part of' some 'lower third secondary premolar tooth')</t>
+  </si>
+  <si>
+    <t>anatomical point' and ('anteriormost part of' some 'upper third secondary premolar tooth')</t>
   </si>
 </sst>
 </file>
@@ -7823,11 +7834,17 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H234" dT="2021-04-21T17:27:34.71" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{53A7FE65-1F7B-4505-868C-8CB7EF24B36F}">
+    <text>How to format these if the teeth included in the tooth row differ?</text>
+  </threadedComment>
   <threadedComment ref="H260" dT="2021-04-16T18:35:06.64" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{1796211E-4A4F-425A-9398-FE54A7FB8340}">
     <text>I think these would be skull measurements?</text>
   </threadedComment>
-  <threadedComment ref="H261" dT="2021-04-16T18:43:07.52" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{3A0E1335-8615-4DEC-BC8F-1EF90DFAD0D5}">
-    <text>anterior or posterior to P3?</text>
+  <threadedComment ref="H260" dT="2021-04-21T17:26:12.94" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{977E2FC2-C377-4B55-A523-9D124B655417}" parentId="{1796211E-4A4F-425A-9398-FE54A7FB8340}">
+    <text>this would be a Point AB pattern from the midpoint of another Point AB pattern</text>
+  </threadedComment>
+  <threadedComment ref="H262" dT="2021-04-21T17:27:09.97" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{EB2EF5AD-17D9-4410-88A0-2E3B0BDD28FB}">
+    <text>Same with this one</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -8038,9 +8055,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H269" sqref="H269"/>
+      <selection pane="bottomLeft" activeCell="H238" sqref="H238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16293,7 +16310,7 @@
     </row>
     <row r="261" spans="1:21">
       <c r="A261" s="37"/>
-      <c r="C261" s="31" t="s">
+      <c r="C261" s="16" t="s">
         <v>2113</v>
       </c>
       <c r="H261" s="36" t="s">
@@ -21857,8 +21874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BA4F15-3142-994E-BF8B-16093E97474D}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -22393,22 +22410,22 @@
       <c r="A43" t="s">
         <v>2310</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="39" t="s">
+        <v>2368</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>2313</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>2316</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="36" t="s">
         <v>2311</v>
       </c>
-      <c r="B44" s="32" t="s">
-        <v>2315</v>
+      <c r="B44" s="39" t="s">
+        <v>2369</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>2317</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -22416,32 +22433,32 @@
         <v>2312</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>2314</v>
+        <v>2370</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>2318</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="31" t="s">
-        <v>2319</v>
+        <v>2316</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>2320</v>
+        <v>2317</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>2321</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="22" t="s">
-        <v>2324</v>
+        <v>2367</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>2322</v>
+        <v>2319</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>2323</v>
+        <v>2320</v>
       </c>
     </row>
   </sheetData>
@@ -22453,7 +22470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
   <dimension ref="A1:D338"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
     </sheetView>
@@ -25297,72 +25314,72 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>2325</v>
+        <v>2321</v>
       </c>
       <c r="B199" t="s">
         <v>112</v>
       </c>
       <c r="C199" s="22" t="s">
-        <v>2330</v>
+        <v>2326</v>
       </c>
       <c r="D199" t="s">
-        <v>2365</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>2326</v>
+        <v>2322</v>
       </c>
       <c r="B200" t="s">
         <v>112</v>
       </c>
       <c r="C200" s="22" t="s">
-        <v>2363</v>
+        <v>2359</v>
       </c>
       <c r="D200" t="s">
-        <v>2366</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>2327</v>
+        <v>2323</v>
       </c>
       <c r="B201" t="s">
         <v>112</v>
       </c>
       <c r="C201" s="22" t="s">
-        <v>2364</v>
+        <v>2360</v>
       </c>
       <c r="D201" t="s">
-        <v>2367</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>2328</v>
+        <v>2324</v>
       </c>
       <c r="B202" t="s">
         <v>108</v>
       </c>
       <c r="C202" s="22" t="s">
-        <v>2330</v>
+        <v>2326</v>
       </c>
       <c r="D202" t="s">
-        <v>2368</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>2329</v>
+        <v>2325</v>
       </c>
       <c r="B203" t="s">
         <v>108</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>2363</v>
+        <v>2359</v>
       </c>
       <c r="D203" t="s">
-        <v>2369</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -25373,10 +25390,10 @@
         <v>108</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>2364</v>
+        <v>2360</v>
       </c>
       <c r="D204" t="s">
-        <v>2370</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -27199,7 +27216,7 @@
         <v>2150</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>2339</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -27226,35 +27243,35 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>2331</v>
+        <v>2327</v>
       </c>
       <c r="C47" t="s">
-        <v>2332</v>
+        <v>2328</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>2333</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>2334</v>
+        <v>2330</v>
       </c>
       <c r="C48" t="s">
-        <v>2335</v>
+        <v>2331</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>2336</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>2337</v>
+        <v>2333</v>
       </c>
       <c r="C49" t="s">
-        <v>2338</v>
+        <v>2334</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>2340</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -27273,10 +27290,10 @@
         <v>1956</v>
       </c>
       <c r="C51" t="s">
-        <v>2343</v>
+        <v>2339</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>2344</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -27284,10 +27301,10 @@
         <v>1957</v>
       </c>
       <c r="C52" t="s">
-        <v>2345</v>
+        <v>2341</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>2346</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -27306,10 +27323,10 @@
         <v>1991</v>
       </c>
       <c r="C54" t="s">
-        <v>2348</v>
+        <v>2344</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>2349</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -27317,10 +27334,10 @@
         <v>1992</v>
       </c>
       <c r="C55" t="s">
-        <v>2347</v>
+        <v>2343</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>2350</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -27350,10 +27367,10 @@
         <v>2027</v>
       </c>
       <c r="C58" t="s">
-        <v>2341</v>
+        <v>2337</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>2342</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -27361,10 +27378,10 @@
         <v>2028</v>
       </c>
       <c r="C59" t="s">
-        <v>2351</v>
+        <v>2347</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>2352</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -27383,10 +27400,10 @@
         <v>2058</v>
       </c>
       <c r="C61" t="s">
-        <v>2353</v>
+        <v>2349</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>2355</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -27394,10 +27411,10 @@
         <v>2059</v>
       </c>
       <c r="C62" t="s">
-        <v>2354</v>
+        <v>2350</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>2356</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -27427,10 +27444,10 @@
         <v>2092</v>
       </c>
       <c r="C65" t="s">
-        <v>2358</v>
+        <v>2354</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>2359</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -27438,10 +27455,10 @@
         <v>2093</v>
       </c>
       <c r="C66" t="s">
-        <v>2357</v>
+        <v>2353</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>2360</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -27449,10 +27466,10 @@
         <v>2121</v>
       </c>
       <c r="C67" t="s">
-        <v>2362</v>
+        <v>2358</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>2361</v>
+        <v>2357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started talonid and trigonid widths
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C5AA66-4F89-4D5F-BC7A-8E082C79575D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE728F89-70EF-44DB-964C-785EE9A79CBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4800" uniqueCount="2371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4803" uniqueCount="2373">
   <si>
     <t>Status</t>
   </si>
@@ -7281,6 +7281,12 @@
   </si>
   <si>
     <t>anatomical point' and ('anteriormost part of' some 'upper third secondary premolar tooth')</t>
+  </si>
+  <si>
+    <t>Lower molar 3 trigonid width</t>
+  </si>
+  <si>
+    <t>occlusal surface' and ('part of' some 'lower third secondary molar tooth')</t>
   </si>
 </sst>
 </file>
@@ -8055,9 +8061,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H238" sqref="H238"/>
+      <selection pane="bottomLeft" activeCell="H312" sqref="H312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -22468,11 +22474,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D338"/>
+  <dimension ref="A1:D344"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -25132,1573 +25138,1554 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>1917</v>
+        <v>2371</v>
       </c>
       <c r="B186" t="s">
-        <v>112</v>
-      </c>
-      <c r="C186" t="s">
-        <v>2166</v>
-      </c>
-      <c r="D186" t="s">
-        <v>1924</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
-      <c r="A187" t="s">
-        <v>1918</v>
-      </c>
-      <c r="B187" t="s">
-        <v>112</v>
-      </c>
-      <c r="C187" t="s">
-        <v>2167</v>
-      </c>
-      <c r="D187" t="s">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" t="s">
-        <v>1919</v>
-      </c>
-      <c r="B188" t="s">
-        <v>112</v>
-      </c>
-      <c r="C188" t="s">
-        <v>2168</v>
-      </c>
-      <c r="D188" t="s">
-        <v>1926</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
-      <c r="A189" t="s">
-        <v>1921</v>
-      </c>
-      <c r="B189" t="s">
-        <v>112</v>
-      </c>
-      <c r="C189" t="s">
-        <v>2169</v>
-      </c>
-      <c r="D189" t="s">
-        <v>1927</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
-      <c r="A190" t="s">
-        <v>1920</v>
-      </c>
-      <c r="B190" t="s">
-        <v>112</v>
-      </c>
-      <c r="C190" t="s">
-        <v>2170</v>
-      </c>
-      <c r="D190" t="s">
-        <v>1928</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
-      <c r="A191" t="s">
-        <v>1922</v>
-      </c>
-      <c r="B191" t="s">
-        <v>112</v>
-      </c>
-      <c r="C191" t="s">
-        <v>2171</v>
-      </c>
-      <c r="D191" t="s">
-        <v>1929</v>
+        <v>108</v>
+      </c>
+      <c r="C186" s="22" t="s">
+        <v>2372</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>1923</v>
+        <v>1917</v>
       </c>
       <c r="B192" t="s">
         <v>112</v>
       </c>
       <c r="C192" t="s">
-        <v>2172</v>
+        <v>2166</v>
       </c>
       <c r="D192" t="s">
-        <v>1930</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>1932</v>
+        <v>1918</v>
       </c>
       <c r="B193" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C193" t="s">
-        <v>2173</v>
+        <v>2167</v>
       </c>
       <c r="D193" t="s">
-        <v>1941</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>1934</v>
+        <v>1919</v>
       </c>
       <c r="B194" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C194" t="s">
-        <v>2174</v>
+        <v>2168</v>
       </c>
       <c r="D194" t="s">
-        <v>1942</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>1933</v>
+        <v>1921</v>
       </c>
       <c r="B195" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C195" t="s">
-        <v>2175</v>
+        <v>2169</v>
       </c>
       <c r="D195" t="s">
-        <v>1943</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>1931</v>
+        <v>1920</v>
       </c>
       <c r="B196" t="s">
         <v>112</v>
       </c>
       <c r="C196" t="s">
-        <v>2173</v>
+        <v>2170</v>
       </c>
       <c r="D196" t="s">
-        <v>1946</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>1944</v>
+        <v>1922</v>
       </c>
       <c r="B197" t="s">
         <v>112</v>
       </c>
       <c r="C197" t="s">
-        <v>2174</v>
+        <v>2171</v>
       </c>
       <c r="D197" t="s">
-        <v>1947</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>1945</v>
+        <v>1923</v>
       </c>
       <c r="B198" t="s">
         <v>112</v>
       </c>
       <c r="C198" t="s">
-        <v>2175</v>
+        <v>2172</v>
       </c>
       <c r="D198" t="s">
-        <v>1948</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>2321</v>
+        <v>1932</v>
       </c>
       <c r="B199" t="s">
-        <v>112</v>
-      </c>
-      <c r="C199" s="22" t="s">
-        <v>2326</v>
+        <v>108</v>
+      </c>
+      <c r="C199" t="s">
+        <v>2173</v>
       </c>
       <c r="D199" t="s">
-        <v>2361</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>2322</v>
+        <v>1934</v>
       </c>
       <c r="B200" t="s">
-        <v>112</v>
-      </c>
-      <c r="C200" s="22" t="s">
-        <v>2359</v>
+        <v>108</v>
+      </c>
+      <c r="C200" t="s">
+        <v>2174</v>
       </c>
       <c r="D200" t="s">
-        <v>2362</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>2323</v>
+        <v>1933</v>
       </c>
       <c r="B201" t="s">
-        <v>112</v>
-      </c>
-      <c r="C201" s="22" t="s">
-        <v>2360</v>
+        <v>108</v>
+      </c>
+      <c r="C201" t="s">
+        <v>2175</v>
       </c>
       <c r="D201" t="s">
-        <v>2363</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>2324</v>
+        <v>1931</v>
       </c>
       <c r="B202" t="s">
-        <v>108</v>
-      </c>
-      <c r="C202" s="22" t="s">
-        <v>2326</v>
+        <v>112</v>
+      </c>
+      <c r="C202" t="s">
+        <v>2173</v>
       </c>
       <c r="D202" t="s">
-        <v>2364</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>2325</v>
+        <v>1944</v>
       </c>
       <c r="B203" t="s">
-        <v>108</v>
-      </c>
-      <c r="C203" s="22" t="s">
-        <v>2359</v>
+        <v>112</v>
+      </c>
+      <c r="C203" t="s">
+        <v>2174</v>
       </c>
       <c r="D203" t="s">
-        <v>2365</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>1933</v>
+        <v>1945</v>
       </c>
       <c r="B204" t="s">
-        <v>108</v>
-      </c>
-      <c r="C204" s="22" t="s">
-        <v>2360</v>
+        <v>112</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2175</v>
       </c>
       <c r="D204" t="s">
-        <v>2366</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>1949</v>
+        <v>2321</v>
       </c>
       <c r="B205" t="s">
-        <v>108</v>
-      </c>
-      <c r="C205" t="s">
-        <v>2176</v>
+        <v>112</v>
+      </c>
+      <c r="C205" s="22" t="s">
+        <v>2326</v>
       </c>
       <c r="D205" t="s">
-        <v>1961</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>1950</v>
+        <v>2322</v>
       </c>
       <c r="B206" t="s">
-        <v>108</v>
-      </c>
-      <c r="C206" t="s">
-        <v>2177</v>
+        <v>112</v>
+      </c>
+      <c r="C206" s="22" t="s">
+        <v>2359</v>
       </c>
       <c r="D206" t="s">
-        <v>1962</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>1951</v>
+        <v>2323</v>
       </c>
       <c r="B207" t="s">
-        <v>108</v>
-      </c>
-      <c r="C207" t="s">
-        <v>2178</v>
+        <v>112</v>
+      </c>
+      <c r="C207" s="22" t="s">
+        <v>2360</v>
       </c>
       <c r="D207" t="s">
-        <v>1963</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>1952</v>
+        <v>2324</v>
       </c>
       <c r="B208" t="s">
         <v>108</v>
       </c>
-      <c r="C208" t="s">
-        <v>2179</v>
+      <c r="C208" s="22" t="s">
+        <v>2326</v>
       </c>
       <c r="D208" t="s">
-        <v>1964</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>1953</v>
+        <v>2325</v>
       </c>
       <c r="B209" t="s">
         <v>108</v>
       </c>
-      <c r="C209" t="s">
-        <v>2180</v>
+      <c r="C209" s="22" t="s">
+        <v>2359</v>
       </c>
       <c r="D209" t="s">
-        <v>1965</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>1954</v>
+        <v>1933</v>
       </c>
       <c r="B210" t="s">
         <v>108</v>
       </c>
-      <c r="C210" t="s">
-        <v>2181</v>
+      <c r="C210" s="22" t="s">
+        <v>2360</v>
       </c>
       <c r="D210" t="s">
-        <v>1966</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>1955</v>
+        <v>1949</v>
       </c>
       <c r="B211" t="s">
         <v>108</v>
       </c>
       <c r="C211" t="s">
-        <v>2182</v>
+        <v>2176</v>
       </c>
       <c r="D211" t="s">
-        <v>1967</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>1968</v>
+        <v>1950</v>
       </c>
       <c r="B212" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C212" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
       <c r="D212" t="s">
-        <v>1975</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>1969</v>
+        <v>1951</v>
       </c>
       <c r="B213" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C213" t="s">
-        <v>2177</v>
+        <v>2178</v>
       </c>
       <c r="D213" t="s">
-        <v>1976</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>1970</v>
+        <v>1952</v>
       </c>
       <c r="B214" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C214" t="s">
-        <v>2178</v>
+        <v>2179</v>
       </c>
       <c r="D214" t="s">
-        <v>1977</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>1971</v>
+        <v>1953</v>
       </c>
       <c r="B215" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C215" t="s">
-        <v>2179</v>
+        <v>2180</v>
       </c>
       <c r="D215" t="s">
-        <v>1978</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>1972</v>
+        <v>1954</v>
       </c>
       <c r="B216" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C216" t="s">
-        <v>2180</v>
+        <v>2181</v>
       </c>
       <c r="D216" t="s">
-        <v>1979</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>1973</v>
+        <v>1955</v>
       </c>
       <c r="B217" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C217" t="s">
-        <v>2181</v>
+        <v>2182</v>
       </c>
       <c r="D217" t="s">
-        <v>1980</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>1974</v>
+        <v>1968</v>
       </c>
       <c r="B218" t="s">
         <v>112</v>
       </c>
       <c r="C218" t="s">
-        <v>2182</v>
+        <v>2176</v>
       </c>
       <c r="D218" t="s">
-        <v>1981</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>1982</v>
+        <v>1969</v>
       </c>
       <c r="B219" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C219" t="s">
-        <v>2183</v>
+        <v>2177</v>
       </c>
       <c r="D219" t="s">
-        <v>1993</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>1983</v>
+        <v>1970</v>
       </c>
       <c r="B220" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C220" t="s">
-        <v>2184</v>
+        <v>2178</v>
       </c>
       <c r="D220" t="s">
-        <v>1994</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>1984</v>
+        <v>1971</v>
       </c>
       <c r="B221" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C221" t="s">
-        <v>2185</v>
+        <v>2179</v>
       </c>
       <c r="D221" t="s">
-        <v>1995</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>1985</v>
+        <v>1972</v>
       </c>
       <c r="B222" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C222" t="s">
-        <v>2186</v>
+        <v>2180</v>
       </c>
       <c r="D222" t="s">
-        <v>1996</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>1986</v>
+        <v>1973</v>
       </c>
       <c r="B223" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C223" t="s">
-        <v>2187</v>
+        <v>2181</v>
       </c>
       <c r="D223" t="s">
-        <v>1997</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>1987</v>
+        <v>1974</v>
       </c>
       <c r="B224" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C224" t="s">
-        <v>2188</v>
+        <v>2182</v>
       </c>
       <c r="D224" t="s">
-        <v>1998</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>1988</v>
+        <v>1982</v>
       </c>
       <c r="B225" t="s">
         <v>108</v>
       </c>
       <c r="C225" t="s">
-        <v>2189</v>
+        <v>2183</v>
       </c>
       <c r="D225" t="s">
-        <v>1999</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>2000</v>
+        <v>1983</v>
       </c>
       <c r="B226" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C226" t="s">
-        <v>2183</v>
+        <v>2184</v>
       </c>
       <c r="D226" t="s">
-        <v>2007</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>2001</v>
+        <v>1984</v>
       </c>
       <c r="B227" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C227" t="s">
-        <v>2184</v>
+        <v>2185</v>
       </c>
       <c r="D227" t="s">
-        <v>2008</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>2002</v>
+        <v>1985</v>
       </c>
       <c r="B228" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C228" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
       <c r="D228" t="s">
-        <v>2009</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>2003</v>
+        <v>1986</v>
       </c>
       <c r="B229" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C229" t="s">
-        <v>2186</v>
+        <v>2187</v>
       </c>
       <c r="D229" t="s">
-        <v>2010</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>2004</v>
+        <v>1987</v>
       </c>
       <c r="B230" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C230" t="s">
-        <v>2187</v>
+        <v>2188</v>
       </c>
       <c r="D230" t="s">
-        <v>2011</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>2005</v>
+        <v>1988</v>
       </c>
       <c r="B231" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C231" t="s">
-        <v>2188</v>
+        <v>2189</v>
       </c>
       <c r="D231" t="s">
-        <v>2012</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="B232" t="s">
         <v>112</v>
       </c>
       <c r="C232" t="s">
-        <v>2189</v>
+        <v>2183</v>
       </c>
       <c r="D232" t="s">
-        <v>2013</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B233" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C233" t="s">
-        <v>2190</v>
+        <v>2184</v>
       </c>
       <c r="D233" t="s">
-        <v>2029</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="B234" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C234" t="s">
-        <v>2191</v>
+        <v>2185</v>
       </c>
       <c r="D234" t="s">
-        <v>2030</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="B235" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C235" t="s">
-        <v>2192</v>
+        <v>2186</v>
       </c>
       <c r="D235" t="s">
-        <v>2031</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="B236" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C236" t="s">
-        <v>2193</v>
+        <v>2187</v>
       </c>
       <c r="D236" t="s">
-        <v>2032</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="B237" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C237" t="s">
-        <v>2194</v>
+        <v>2188</v>
       </c>
       <c r="D237" t="s">
-        <v>2033</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>2019</v>
+        <v>2006</v>
       </c>
       <c r="B238" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C238" t="s">
-        <v>2195</v>
+        <v>2189</v>
       </c>
       <c r="D238" t="s">
-        <v>2034</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="B239" t="s">
         <v>108</v>
       </c>
       <c r="C239" t="s">
-        <v>2196</v>
+        <v>2190</v>
       </c>
       <c r="D239" t="s">
-        <v>2035</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>2036</v>
+        <v>2015</v>
       </c>
       <c r="B240" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C240" t="s">
-        <v>2190</v>
+        <v>2191</v>
       </c>
       <c r="D240" t="s">
-        <v>2043</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>2037</v>
+        <v>2016</v>
       </c>
       <c r="B241" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C241" t="s">
-        <v>2191</v>
+        <v>2192</v>
       </c>
       <c r="D241" t="s">
-        <v>2044</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>2038</v>
+        <v>2017</v>
       </c>
       <c r="B242" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C242" t="s">
-        <v>2192</v>
+        <v>2193</v>
       </c>
       <c r="D242" t="s">
-        <v>2045</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>2039</v>
+        <v>2018</v>
       </c>
       <c r="B243" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C243" t="s">
-        <v>2193</v>
+        <v>2194</v>
       </c>
       <c r="D243" t="s">
-        <v>2046</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>2040</v>
+        <v>2019</v>
       </c>
       <c r="B244" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C244" t="s">
-        <v>2194</v>
+        <v>2195</v>
       </c>
       <c r="D244" t="s">
-        <v>2047</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>2041</v>
+        <v>2020</v>
       </c>
       <c r="B245" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C245" t="s">
-        <v>2195</v>
+        <v>2196</v>
       </c>
       <c r="D245" t="s">
-        <v>2048</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>2042</v>
+        <v>2036</v>
       </c>
       <c r="B246" t="s">
         <v>112</v>
       </c>
       <c r="C246" t="s">
-        <v>2196</v>
+        <v>2190</v>
       </c>
       <c r="D246" t="s">
-        <v>2049</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="B247" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C247" t="s">
-        <v>2197</v>
+        <v>2191</v>
       </c>
       <c r="D247" t="s">
-        <v>2062</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="B248" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C248" t="s">
-        <v>2198</v>
+        <v>2192</v>
       </c>
       <c r="D248" t="s">
-        <v>2063</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="B249" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C249" t="s">
-        <v>2199</v>
+        <v>2193</v>
       </c>
       <c r="D249" t="s">
-        <v>2064</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>2053</v>
+        <v>2040</v>
       </c>
       <c r="B250" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C250" t="s">
-        <v>2200</v>
+        <v>2194</v>
       </c>
       <c r="D250" t="s">
-        <v>2065</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>2054</v>
+        <v>2041</v>
       </c>
       <c r="B251" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C251" t="s">
-        <v>2201</v>
+        <v>2195</v>
       </c>
       <c r="D251" t="s">
-        <v>2066</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>2055</v>
+        <v>2042</v>
       </c>
       <c r="B252" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C252" t="s">
-        <v>2202</v>
+        <v>2196</v>
       </c>
       <c r="D252" t="s">
-        <v>2067</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>2056</v>
+        <v>2050</v>
       </c>
       <c r="B253" t="s">
         <v>108</v>
       </c>
       <c r="C253" t="s">
-        <v>2203</v>
+        <v>2197</v>
       </c>
       <c r="D253" t="s">
-        <v>2068</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>2069</v>
+        <v>2051</v>
       </c>
       <c r="B254" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C254" t="s">
-        <v>2197</v>
+        <v>2198</v>
       </c>
       <c r="D254" t="s">
-        <v>2076</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>2070</v>
+        <v>2052</v>
       </c>
       <c r="B255" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C255" t="s">
-        <v>2198</v>
+        <v>2199</v>
       </c>
       <c r="D255" t="s">
-        <v>2077</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>2071</v>
+        <v>2053</v>
       </c>
       <c r="B256" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C256" t="s">
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="D256" t="s">
-        <v>2078</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>2072</v>
+        <v>2054</v>
       </c>
       <c r="B257" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C257" t="s">
-        <v>2200</v>
+        <v>2201</v>
       </c>
       <c r="D257" t="s">
-        <v>2079</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>2073</v>
+        <v>2055</v>
       </c>
       <c r="B258" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C258" t="s">
-        <v>2201</v>
+        <v>2202</v>
       </c>
       <c r="D258" t="s">
-        <v>2080</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>2074</v>
+        <v>2056</v>
       </c>
       <c r="B259" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C259" t="s">
-        <v>2202</v>
+        <v>2203</v>
       </c>
       <c r="D259" t="s">
-        <v>2081</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>2075</v>
+        <v>2069</v>
       </c>
       <c r="B260" t="s">
         <v>112</v>
       </c>
       <c r="C260" t="s">
-        <v>2203</v>
+        <v>2197</v>
       </c>
       <c r="D260" t="s">
-        <v>2082</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>2083</v>
+        <v>2070</v>
       </c>
       <c r="B261" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C261" t="s">
-        <v>2204</v>
+        <v>2198</v>
       </c>
       <c r="D261" t="s">
-        <v>2099</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>2084</v>
+        <v>2071</v>
       </c>
       <c r="B262" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C262" t="s">
-        <v>2205</v>
+        <v>2199</v>
       </c>
       <c r="D262" t="s">
-        <v>2100</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>2085</v>
+        <v>2072</v>
       </c>
       <c r="B263" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C263" t="s">
-        <v>2206</v>
+        <v>2200</v>
       </c>
       <c r="D263" t="s">
-        <v>2101</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>2086</v>
+        <v>2073</v>
       </c>
       <c r="B264" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C264" t="s">
-        <v>2207</v>
+        <v>2201</v>
       </c>
       <c r="D264" t="s">
-        <v>2102</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>2087</v>
+        <v>2074</v>
       </c>
       <c r="B265" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C265" t="s">
-        <v>2208</v>
+        <v>2202</v>
       </c>
       <c r="D265" t="s">
-        <v>2103</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>2088</v>
+        <v>2075</v>
       </c>
       <c r="B266" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C266" t="s">
-        <v>2209</v>
+        <v>2203</v>
       </c>
       <c r="D266" t="s">
-        <v>2104</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>2089</v>
+        <v>2083</v>
       </c>
       <c r="B267" t="s">
         <v>108</v>
       </c>
       <c r="C267" t="s">
-        <v>2210</v>
+        <v>2204</v>
       </c>
       <c r="D267" t="s">
-        <v>2105</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="B268" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C268" t="s">
-        <v>2204</v>
+        <v>2205</v>
       </c>
       <c r="D268" t="s">
-        <v>2106</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>2084</v>
+        <v>2085</v>
       </c>
       <c r="B269" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C269" t="s">
-        <v>2205</v>
+        <v>2206</v>
       </c>
       <c r="D269" t="s">
-        <v>2107</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>2085</v>
+        <v>2086</v>
       </c>
       <c r="B270" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C270" t="s">
-        <v>2206</v>
+        <v>2207</v>
       </c>
       <c r="D270" t="s">
-        <v>2108</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>2086</v>
+        <v>2087</v>
       </c>
       <c r="B271" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C271" t="s">
-        <v>2207</v>
+        <v>2208</v>
       </c>
       <c r="D271" t="s">
-        <v>2111</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>2087</v>
+        <v>2088</v>
       </c>
       <c r="B272" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C272" t="s">
-        <v>2208</v>
+        <v>2209</v>
       </c>
       <c r="D272" t="s">
-        <v>2109</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>2088</v>
+        <v>2089</v>
       </c>
       <c r="B273" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C273" t="s">
-        <v>2209</v>
+        <v>2210</v>
       </c>
       <c r="D273" t="s">
-        <v>2112</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>2089</v>
+        <v>2083</v>
       </c>
       <c r="B274" t="s">
         <v>112</v>
       </c>
       <c r="C274" t="s">
-        <v>2210</v>
+        <v>2204</v>
       </c>
       <c r="D274" t="s">
-        <v>2110</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="275" spans="1:4">
-      <c r="A275" s="31" t="s">
-        <v>2114</v>
+      <c r="A275" t="s">
+        <v>2084</v>
       </c>
       <c r="B275" t="s">
         <v>112</v>
       </c>
-      <c r="C275" s="16" t="s">
-        <v>2211</v>
+      <c r="C275" t="s">
+        <v>2205</v>
       </c>
       <c r="D275" t="s">
-        <v>2122</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="276" spans="1:4">
-      <c r="A276" s="31" t="s">
-        <v>2115</v>
+      <c r="A276" t="s">
+        <v>2085</v>
       </c>
       <c r="B276" t="s">
         <v>112</v>
       </c>
-      <c r="C276" s="16" t="s">
-        <v>2212</v>
+      <c r="C276" t="s">
+        <v>2206</v>
       </c>
       <c r="D276" t="s">
-        <v>2123</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="277" spans="1:4">
-      <c r="A277" s="31" t="s">
-        <v>2116</v>
+      <c r="A277" t="s">
+        <v>2086</v>
       </c>
       <c r="B277" t="s">
         <v>112</v>
       </c>
-      <c r="C277" s="16" t="s">
-        <v>2213</v>
+      <c r="C277" t="s">
+        <v>2207</v>
       </c>
       <c r="D277" t="s">
-        <v>2124</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="278" spans="1:4">
-      <c r="A278" s="31" t="s">
-        <v>2117</v>
+      <c r="A278" t="s">
+        <v>2087</v>
       </c>
       <c r="B278" t="s">
         <v>112</v>
       </c>
-      <c r="C278" s="16" t="s">
-        <v>2214</v>
+      <c r="C278" t="s">
+        <v>2208</v>
       </c>
       <c r="D278" t="s">
-        <v>2125</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="279" spans="1:4">
-      <c r="A279" s="31" t="s">
-        <v>2118</v>
+      <c r="A279" t="s">
+        <v>2088</v>
       </c>
       <c r="B279" t="s">
         <v>112</v>
       </c>
-      <c r="C279" s="16" t="s">
-        <v>2215</v>
+      <c r="C279" t="s">
+        <v>2209</v>
       </c>
       <c r="D279" t="s">
-        <v>2126</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="280" spans="1:4">
-      <c r="A280" s="31" t="s">
-        <v>2119</v>
+      <c r="A280" t="s">
+        <v>2089</v>
       </c>
       <c r="B280" t="s">
         <v>112</v>
       </c>
-      <c r="C280" s="16" t="s">
-        <v>2216</v>
+      <c r="C280" t="s">
+        <v>2210</v>
       </c>
       <c r="D280" t="s">
-        <v>2127</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="31" t="s">
-        <v>2120</v>
+        <v>2114</v>
       </c>
       <c r="B281" t="s">
         <v>112</v>
       </c>
       <c r="C281" s="16" t="s">
-        <v>2217</v>
+        <v>2211</v>
       </c>
       <c r="D281" t="s">
-        <v>2128</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="31" t="s">
-        <v>2129</v>
+        <v>2115</v>
       </c>
       <c r="B282" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C282" s="16" t="s">
-        <v>2211</v>
+        <v>2212</v>
       </c>
       <c r="D282" t="s">
-        <v>2136</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="283" spans="1:4">
       <c r="A283" s="31" t="s">
-        <v>2130</v>
+        <v>2116</v>
       </c>
       <c r="B283" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C283" s="16" t="s">
-        <v>2212</v>
+        <v>2213</v>
       </c>
       <c r="D283" t="s">
-        <v>2137</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" s="31" t="s">
-        <v>2131</v>
+        <v>2117</v>
       </c>
       <c r="B284" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C284" s="16" t="s">
-        <v>2213</v>
+        <v>2214</v>
       </c>
       <c r="D284" t="s">
-        <v>2138</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="285" spans="1:4">
       <c r="A285" s="31" t="s">
-        <v>2132</v>
+        <v>2118</v>
       </c>
       <c r="B285" t="s">
-        <v>108</v>
-      </c>
-      <c r="C285" t="s">
-        <v>2214</v>
+        <v>112</v>
+      </c>
+      <c r="C285" s="16" t="s">
+        <v>2215</v>
       </c>
       <c r="D285" t="s">
-        <v>2139</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="31" t="s">
-        <v>2133</v>
+        <v>2119</v>
       </c>
       <c r="B286" t="s">
-        <v>108</v>
-      </c>
-      <c r="C286" t="s">
-        <v>2215</v>
+        <v>112</v>
+      </c>
+      <c r="C286" s="16" t="s">
+        <v>2216</v>
       </c>
       <c r="D286" t="s">
-        <v>2140</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" s="31" t="s">
-        <v>2134</v>
+        <v>2120</v>
       </c>
       <c r="B287" t="s">
-        <v>108</v>
-      </c>
-      <c r="C287" t="s">
-        <v>2216</v>
+        <v>112</v>
+      </c>
+      <c r="C287" s="16" t="s">
+        <v>2217</v>
       </c>
       <c r="D287" t="s">
-        <v>2141</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="31" t="s">
-        <v>2135</v>
+        <v>2129</v>
       </c>
       <c r="B288" t="s">
         <v>108</v>
       </c>
-      <c r="C288" t="s">
+      <c r="C288" s="16" t="s">
+        <v>2211</v>
+      </c>
+      <c r="D288" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="A289" s="31" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B289" t="s">
+        <v>108</v>
+      </c>
+      <c r="C289" s="16" t="s">
+        <v>2212</v>
+      </c>
+      <c r="D289" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="A290" s="31" t="s">
+        <v>2131</v>
+      </c>
+      <c r="B290" t="s">
+        <v>108</v>
+      </c>
+      <c r="C290" s="16" t="s">
+        <v>2213</v>
+      </c>
+      <c r="D290" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="A291" s="31" t="s">
+        <v>2132</v>
+      </c>
+      <c r="B291" t="s">
+        <v>108</v>
+      </c>
+      <c r="C291" t="s">
+        <v>2214</v>
+      </c>
+      <c r="D291" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4">
+      <c r="A292" s="31" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B292" t="s">
+        <v>108</v>
+      </c>
+      <c r="C292" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D292" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4">
+      <c r="A293" s="31" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B293" t="s">
+        <v>108</v>
+      </c>
+      <c r="C293" t="s">
+        <v>2216</v>
+      </c>
+      <c r="D293" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
+      <c r="A294" s="31" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B294" t="s">
+        <v>108</v>
+      </c>
+      <c r="C294" t="s">
         <v>2217</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D294" t="s">
         <v>2142</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4">
-      <c r="A289" s="16" t="s">
-        <v>2143</v>
-      </c>
-      <c r="B289" s="16" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C289" s="32" t="s">
-        <v>2226</v>
-      </c>
-      <c r="D289" t="s">
-        <v>2218</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4">
-      <c r="A290" s="16" t="s">
-        <v>2219</v>
-      </c>
-      <c r="B290" s="16" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C290" s="32" t="s">
-        <v>2225</v>
-      </c>
-      <c r="D290" t="s">
-        <v>2232</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4">
-      <c r="A291" s="16" t="s">
-        <v>2220</v>
-      </c>
-      <c r="B291" s="16" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C291" s="32" t="s">
-        <v>2227</v>
-      </c>
-      <c r="D291" t="s">
-        <v>2233</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4">
-      <c r="A292" s="16" t="s">
-        <v>2221</v>
-      </c>
-      <c r="B292" s="16" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C292" s="32" t="s">
-        <v>2228</v>
-      </c>
-      <c r="D292" t="s">
-        <v>2234</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4">
-      <c r="A293" s="16" t="s">
-        <v>2222</v>
-      </c>
-      <c r="B293" s="16" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C293" s="32" t="s">
-        <v>2229</v>
-      </c>
-      <c r="D293" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4">
-      <c r="A294" s="16" t="s">
-        <v>2223</v>
-      </c>
-      <c r="B294" s="16" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C294" s="32" t="s">
-        <v>2230</v>
-      </c>
-      <c r="D294" t="s">
-        <v>2235</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="16" t="s">
-        <v>2224</v>
+        <v>2143</v>
       </c>
       <c r="B295" s="16" t="s">
         <v>2144</v>
       </c>
       <c r="C295" s="32" t="s">
+        <v>2226</v>
+      </c>
+      <c r="D295" t="s">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="A296" s="16" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B296" s="16" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C296" s="32" t="s">
+        <v>2225</v>
+      </c>
+      <c r="D296" t="s">
+        <v>2232</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="A297" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B297" s="16" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C297" s="32" t="s">
+        <v>2227</v>
+      </c>
+      <c r="D297" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4">
+      <c r="A298" s="16" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B298" s="16" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C298" s="32" t="s">
+        <v>2228</v>
+      </c>
+      <c r="D298" t="s">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
+      <c r="A299" s="16" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B299" s="16" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C299" s="32" t="s">
+        <v>2229</v>
+      </c>
+      <c r="D299" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
+      <c r="A300" s="16" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B300" s="16" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C300" s="32" t="s">
+        <v>2230</v>
+      </c>
+      <c r="D300" t="s">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301" s="16" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B301" s="16" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C301" s="32" t="s">
         <v>2231</v>
       </c>
-      <c r="D295" t="s">
+      <c r="D301" t="s">
         <v>2237</v>
       </c>
-    </row>
-    <row r="296" spans="1:4">
-      <c r="A296" s="16"/>
-      <c r="B296" s="16"/>
-      <c r="C296" s="39"/>
-    </row>
-    <row r="297" spans="1:4">
-      <c r="A297" s="16"/>
-      <c r="B297" s="16"/>
-      <c r="C297" s="39"/>
-    </row>
-    <row r="298" spans="1:4">
-      <c r="A298" s="16"/>
-      <c r="B298" s="16"/>
-      <c r="C298" s="39"/>
-    </row>
-    <row r="299" spans="1:4">
-      <c r="A299" s="16"/>
-      <c r="B299" s="16"/>
-      <c r="C299" s="39"/>
-    </row>
-    <row r="300" spans="1:4">
-      <c r="A300" s="16"/>
-      <c r="B300" s="16"/>
-      <c r="C300" s="39"/>
-    </row>
-    <row r="301" spans="1:4">
-      <c r="A301" s="16"/>
-      <c r="B301" s="16"/>
-      <c r="C301" s="39"/>
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="16"/>
@@ -26715,118 +26702,148 @@
       <c r="B304" s="16"/>
       <c r="C304" s="39"/>
     </row>
-    <row r="314" spans="1:4">
-      <c r="A314" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B314" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C314" s="22" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D314" t="str">
-        <f>"line along "&amp;B314&amp;" of "&amp;C314</f>
-        <v>line along proximal-distal of lateral side' some talus</v>
-      </c>
-    </row>
-    <row r="315" spans="1:4">
-      <c r="A315" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B315" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C315" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D315" t="str">
-        <f>"line along "&amp;B315&amp;" of "&amp;C315</f>
-        <v>line along proximal-distal of pes</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4">
-      <c r="A316" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4">
-      <c r="A317" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4">
-      <c r="A318" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="319" spans="1:4">
-      <c r="A319" t="s">
-        <v>1223</v>
-      </c>
+    <row r="305" spans="1:4">
+      <c r="A305" s="16"/>
+      <c r="B305" s="16"/>
+      <c r="C305" s="39"/>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="A306" s="16"/>
+      <c r="B306" s="16"/>
+      <c r="C306" s="39"/>
+    </row>
+    <row r="307" spans="1:4">
+      <c r="A307" s="16"/>
+      <c r="B307" s="16"/>
+      <c r="C307" s="39"/>
+    </row>
+    <row r="308" spans="1:4">
+      <c r="A308" s="16"/>
+      <c r="B308" s="16"/>
+      <c r="C308" s="39"/>
+    </row>
+    <row r="309" spans="1:4">
+      <c r="A309" s="16"/>
+      <c r="B309" s="16"/>
+      <c r="C309" s="39"/>
+    </row>
+    <row r="310" spans="1:4">
+      <c r="A310" s="16"/>
+      <c r="B310" s="16"/>
+      <c r="C310" s="39"/>
     </row>
     <row r="320" spans="1:4">
       <c r="A320" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C320" s="22" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D320" t="str">
+        <f>"line along "&amp;B320&amp;" of "&amp;C320</f>
+        <v>line along proximal-distal of lateral side' some talus</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4">
+      <c r="A321" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B321" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C321" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D321" t="str">
+        <f>"line along "&amp;B321&amp;" of "&amp;C321</f>
+        <v>line along proximal-distal of pes</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4">
+      <c r="A322" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4">
+      <c r="A323" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4">
+      <c r="A324" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4">
+      <c r="A325" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4">
+      <c r="A326" t="s">
         <v>1224</v>
       </c>
     </row>
-    <row r="321" spans="1:1">
-      <c r="A321" t="s">
+    <row r="327" spans="1:4">
+      <c r="A327" t="s">
         <v>1225</v>
       </c>
     </row>
-    <row r="322" spans="1:1">
-      <c r="A322" t="s">
+    <row r="328" spans="1:4">
+      <c r="A328" t="s">
         <v>1226</v>
       </c>
     </row>
-    <row r="323" spans="1:1">
-      <c r="A323" t="s">
+    <row r="329" spans="1:4">
+      <c r="A329" t="s">
         <v>1227</v>
       </c>
     </row>
-    <row r="324" spans="1:1">
-      <c r="A324" t="s">
+    <row r="330" spans="1:4">
+      <c r="A330" t="s">
         <v>1228</v>
       </c>
     </row>
-    <row r="325" spans="1:1">
-      <c r="A325" t="s">
+    <row r="331" spans="1:4">
+      <c r="A331" t="s">
         <v>1229</v>
       </c>
     </row>
-    <row r="326" spans="1:1">
-      <c r="A326" t="s">
+    <row r="332" spans="1:4">
+      <c r="A332" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="333" spans="1:1">
-      <c r="A333" s="1" t="s">
+    <row r="339" spans="1:1">
+      <c r="A339" s="1" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="334" spans="1:1">
-      <c r="A334" s="1" t="s">
+    <row r="340" spans="1:1">
+      <c r="A340" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="335" spans="1:1">
-      <c r="A335" s="1" t="s">
+    <row r="341" spans="1:1">
+      <c r="A341" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="336" spans="1:1">
-      <c r="A336" s="1" t="s">
+    <row r="342" spans="1:1">
+      <c r="A342" s="1" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="337" spans="1:1">
-      <c r="A337" s="1" t="s">
+    <row r="343" spans="1:1">
+      <c r="A343" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="338" spans="1:1">
-      <c r="A338" s="1" t="s">
+    <row r="344" spans="1:1">
+      <c r="A344" s="1" t="s">
         <v>630</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added incisor structures, tooth row length AB and axis patterns
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19F2DCB-931E-460B-83FD-38C5EF033AC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC71355-35B5-409D-9756-4216962C4201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="4" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4818" uniqueCount="2386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="2433">
   <si>
     <t>Status</t>
   </si>
@@ -7325,14 +7325,155 @@
     <t>occlusal surface' and ('part of' some 'tooth crown') and ('part of' some 'incisor 1')</t>
   </si>
   <si>
-    <t>incisor 1</t>
+    <t>anatomical point' and ('part of' some 'skull') and ('anteriormost part of' some 'alveolar ridge')</t>
+  </si>
+  <si>
+    <t>anatomical point' and ('anteriormost part of' some 'foramen magnum')</t>
+  </si>
+  <si>
+    <t>incisor 3</t>
+  </si>
+  <si>
+    <t>incisor 4</t>
+  </si>
+  <si>
+    <t>incisor 5</t>
+  </si>
+  <si>
+    <t>incisor 6</t>
+  </si>
+  <si>
+    <t>Synonymize incisor 1 and 2 (central and lateral incisors)</t>
+  </si>
+  <si>
+    <t>anatomical row' and ('has number' some 'occlusal surface') and ('part of' some 'premolar tooth')</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar tooth row</t>
+  </si>
+  <si>
+    <t>Length of premolar row at alveoli</t>
+  </si>
+  <si>
+    <t>anatomical row' and ('has number' some 'alveolar ridge') and ('part of' some 'premolar tooth')</t>
+  </si>
+  <si>
+    <t>Length of molar row at alveoli</t>
+  </si>
+  <si>
+    <t>molar 1-2 lengths, 1-3 etc</t>
+  </si>
+  <si>
+    <t>other tooth row lengths</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the jaw)</t>
+  </si>
+  <si>
+    <t>upper incisor 3</t>
+  </si>
+  <si>
+    <t>lower incisor 3</t>
+  </si>
+  <si>
+    <t>upper incisor 4</t>
+  </si>
+  <si>
+    <t>lower incisor 4</t>
+  </si>
+  <si>
+    <t>upper incisor 5</t>
+  </si>
+  <si>
+    <t>lower incisor 5</t>
+  </si>
+  <si>
+    <t>upper incisor 6</t>
+  </si>
+  <si>
+    <t>lower incisor 6</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the jaw)</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the jaw)</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the jaw)</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the upper jaw)</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the lower jaw)</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of' some 'jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of' some 'jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of' some 'jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of' some 'jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of' some 'upper jaw region')</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of' some 'lower jaw region')</t>
+  </si>
+  <si>
+    <t>Length of premolar tooth row</t>
+  </si>
+  <si>
+    <t>Length of molar tooth row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7440,12 +7581,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -7904,10 +8039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581405C8-F852-7340-B9C9-201B714E3AD5}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -8088,6 +8223,11 @@
     <row r="24" spans="1:4">
       <c r="B24" t="s">
         <v>2148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" t="s">
+        <v>2391</v>
       </c>
     </row>
   </sheetData>
@@ -8100,9 +8240,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H263" sqref="H263"/>
+      <selection pane="bottomLeft" activeCell="H240" sqref="H240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -15225,7 +15365,7 @@
     <row r="218" spans="1:21" s="16" customFormat="1">
       <c r="A218" s="38"/>
       <c r="C218" s="17" t="s">
-        <v>983</v>
+        <v>2261</v>
       </c>
       <c r="E218" s="18" t="s">
         <v>343</v>
@@ -15253,7 +15393,7 @@
     <row r="219" spans="1:21" s="16" customFormat="1">
       <c r="A219" s="38"/>
       <c r="C219" s="17" t="s">
-        <v>983</v>
+        <v>2261</v>
       </c>
       <c r="E219" s="18" t="s">
         <v>343</v>
@@ -15309,7 +15449,7 @@
     <row r="221" spans="1:21" s="16" customFormat="1">
       <c r="A221" s="38"/>
       <c r="C221" s="17" t="s">
-        <v>2113</v>
+        <v>2261</v>
       </c>
       <c r="E221" s="18" t="s">
         <v>343</v>
@@ -15337,7 +15477,7 @@
     <row r="222" spans="1:21" s="16" customFormat="1" ht="19.05" customHeight="1">
       <c r="A222" s="38"/>
       <c r="C222" s="17" t="s">
-        <v>983</v>
+        <v>2113</v>
       </c>
       <c r="E222" s="18" t="s">
         <v>343</v>
@@ -15365,7 +15505,7 @@
     <row r="223" spans="1:21" s="16" customFormat="1">
       <c r="A223" s="38"/>
       <c r="C223" s="17" t="s">
-        <v>983</v>
+        <v>2113</v>
       </c>
       <c r="E223" s="18" t="s">
         <v>343</v>
@@ -21917,10 +22057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BA4F15-3142-994E-BF8B-16093E97474D}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -22506,6 +22646,27 @@
         <v>2314</v>
       </c>
     </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>2385</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>2398</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22513,11 +22674,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D344"/>
+  <dimension ref="A1:D346"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A302" sqref="A302"/>
+      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -26773,31 +26934,54 @@
     <row r="303" spans="1:4">
       <c r="A303" s="16"/>
       <c r="B303" s="16"/>
-      <c r="C303" s="37"/>
+      <c r="C303" s="32"/>
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="16"/>
       <c r="B304" s="16"/>
-      <c r="C304" s="37"/>
+      <c r="C304" s="32"/>
     </row>
     <row r="305" spans="1:4">
-      <c r="A305" s="16"/>
-      <c r="B305" s="16"/>
-      <c r="C305" s="37"/>
+      <c r="A305" s="16" t="s">
+        <v>2431</v>
+      </c>
+      <c r="B305" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C305" s="37" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D305" t="s">
+        <v>2393</v>
+      </c>
     </row>
     <row r="306" spans="1:4">
-      <c r="A306" s="16"/>
-      <c r="B306" s="16"/>
-      <c r="C306" s="37"/>
+      <c r="A306" s="16" t="s">
+        <v>2394</v>
+      </c>
+      <c r="B306" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C306" s="37" t="s">
+        <v>2395</v>
+      </c>
     </row>
     <row r="307" spans="1:4">
-      <c r="A307" s="16"/>
-      <c r="B307" s="16"/>
+      <c r="A307" s="16" t="s">
+        <v>2432</v>
+      </c>
+      <c r="B307" s="16" t="s">
+        <v>112</v>
+      </c>
       <c r="C307" s="37"/>
     </row>
     <row r="308" spans="1:4">
-      <c r="A308" s="16"/>
-      <c r="B308" s="16"/>
+      <c r="A308" s="16" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B308" s="16" t="s">
+        <v>112</v>
+      </c>
       <c r="C308" s="37"/>
     </row>
     <row r="309" spans="1:4">
@@ -26810,118 +26994,128 @@
       <c r="B310" s="16"/>
       <c r="C310" s="37"/>
     </row>
-    <row r="320" spans="1:4">
-      <c r="A320" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B320" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C320" s="22" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D320" t="str">
-        <f>"line along "&amp;B320&amp;" of "&amp;C320</f>
-        <v>line along proximal-distal of lateral side' some talus</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4">
-      <c r="A321" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B321" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C321" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D321" t="str">
-        <f>"line along "&amp;B321&amp;" of "&amp;C321</f>
-        <v>line along proximal-distal of pes</v>
-      </c>
+    <row r="311" spans="1:4">
+      <c r="A311" s="16"/>
+      <c r="B311" s="16"/>
+      <c r="C311" s="37"/>
+    </row>
+    <row r="312" spans="1:4">
+      <c r="A312" s="16"/>
+      <c r="B312" s="16"/>
+      <c r="C312" s="37"/>
     </row>
     <row r="322" spans="1:4">
       <c r="A322" t="s">
-        <v>1220</v>
+        <v>1230</v>
+      </c>
+      <c r="B322" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C322" s="22" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D322" t="str">
+        <f>"line along "&amp;B322&amp;" of "&amp;C322</f>
+        <v>line along proximal-distal of lateral side' some talus</v>
       </c>
     </row>
     <row r="323" spans="1:4">
       <c r="A323" t="s">
-        <v>1221</v>
+        <v>1216</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C323" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D323" t="str">
+        <f>"line along "&amp;B323&amp;" of "&amp;C323</f>
+        <v>line along proximal-distal of pes</v>
       </c>
     </row>
     <row r="324" spans="1:4">
       <c r="A324" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="325" spans="1:4">
       <c r="A325" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="326" spans="1:4">
       <c r="A326" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="327" spans="1:4">
       <c r="A327" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="328" spans="1:4">
       <c r="A328" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="329" spans="1:4">
       <c r="A329" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="330" spans="1:4">
       <c r="A330" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="331" spans="1:4">
       <c r="A331" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="332" spans="1:4">
       <c r="A332" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4">
+      <c r="A333" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4">
+      <c r="A334" t="s">
         <v>537</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1">
-      <c r="A339" s="1" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1">
-      <c r="A340" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" s="1" t="s">
-        <v>1130</v>
+        <v>620</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" s="1" t="s">
-        <v>1129</v>
+        <v>623</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" s="1" t="s">
-        <v>629</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" s="1" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1">
+      <c r="A345" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1">
+      <c r="A346" s="1" t="s">
         <v>630</v>
       </c>
     </row>
@@ -26935,10 +27129,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -27569,10 +27763,138 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>2385</v>
+        <v>2387</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>2400</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>2401</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2409</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>2421</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>2388</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2410</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>2403</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2411</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2415</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>2404</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2413</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2414</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>2390</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2417</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2418</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>2430</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added incisor terms and I1-2 axis patterns
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC71355-35B5-409D-9756-4216962C4201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6B8521-3FE4-4496-A693-402EDB706C20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -81,6 +81,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={0D4CF0A9-8CA0-4BED-8E0F-2717916146F3}</author>
+    <author>tc={763FEFB1-51CA-4FC1-A6F7-E523DCC18069}</author>
   </authors>
   <commentList>
     <comment ref="C151" authorId="0" shapeId="0" xr:uid="{0D4CF0A9-8CA0-4BED-8E0F-2717916146F3}">
@@ -91,12 +92,20 @@
     check these?</t>
       </text>
     </comment>
+    <comment ref="C302" authorId="1" shapeId="0" xr:uid="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure if this needs a term other than 'occlusal surface'?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="2433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5041" uniqueCount="2535">
   <si>
     <t>Status</t>
   </si>
@@ -6545,18 +6554,6 @@
     <t>line along anterior posterior-axis of lower canine tooth</t>
   </si>
   <si>
-    <t>line along anterior posterior axis of upper secondary canine tooth</t>
-  </si>
-  <si>
-    <t>line along anterior posterior axis of upper primary canine tooth</t>
-  </si>
-  <si>
-    <t>line along anterior posterior axis of lower secondary canine tooth</t>
-  </si>
-  <si>
-    <t>line along anterior posterior axis of lower primary canine tooth</t>
-  </si>
-  <si>
     <t>Canine medial-lateral diameter at base</t>
   </si>
   <si>
@@ -6620,9 +6617,6 @@
     <t>occlusal surface' and ('part of' some 'molar tooth 1')</t>
   </si>
   <si>
-    <t>Third molar (counting anteriorposteriorly in the lower jaw) of the first set of teeth</t>
-  </si>
-  <si>
     <t>molar tooth 3' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
@@ -7163,39 +7157,21 @@
     <t>molar tooth 5' and ('part of' some 'lower jaw region')</t>
   </si>
   <si>
-    <t>Third premolar (counting anteriorposteriorly in the upper jaw) of the first set of teeth</t>
-  </si>
-  <si>
     <t>premolar tooth 3' and ('part of' some 'upper jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
-    <t>First premolar (counting anteriorposteriorly in the upper jaw) of the first set of teeth</t>
-  </si>
-  <si>
     <t>premolar tooth 1' and ('part of' some 'upper jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
-    <t>First premolar (counting anteriorposteriorly in the lower jaw) of the first set of teeth</t>
-  </si>
-  <si>
     <t>premolar tooth 1' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
-    <t>Second premolar (counting anteriorposteriorly in the lower jaw) of the first set of teeth</t>
-  </si>
-  <si>
-    <t>Second premolar (counting anteriorposteriorly in the upper jaw) of the first set of teeth</t>
-  </si>
-  <si>
     <t>premolar tooth 2' and ('part of' some 'upper jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
     <t>premolar tooth 2' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
-    <t>Third premolar (counting anteriorposteriorly in the lower jaw) of the first set of teeth</t>
-  </si>
-  <si>
     <t>premolar tooth 3' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
   </si>
   <si>
@@ -7322,9 +7298,6 @@
     <t>Incisor 1 anterior-posterior diameter at base</t>
   </si>
   <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown') and ('part of' some 'incisor 1')</t>
-  </si>
-  <si>
     <t>anatomical point' and ('part of' some 'skull') and ('anteriormost part of' some 'alveolar ridge')</t>
   </si>
   <si>
@@ -7346,9 +7319,6 @@
     <t>Synonymize incisor 1 and 2 (central and lateral incisors)</t>
   </si>
   <si>
-    <t>anatomical row' and ('has number' some 'occlusal surface') and ('part of' some 'premolar tooth')</t>
-  </si>
-  <si>
     <t>line along anterior-posterior axis of premolar tooth row</t>
   </si>
   <si>
@@ -7467,13 +7437,358 @@
   </si>
   <si>
     <t>Length of molar tooth row</t>
+  </si>
+  <si>
+    <t>Upper incisor 1 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 1 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 1 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 1 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 1 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 1 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 1')</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper secondary canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper primary canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower secondary canine tooth</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower primary canine tooth</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper central incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower central incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper central secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower central secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower central primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper central primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>Incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>upper third secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>upper third primary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower third secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower third primary incisor tooth</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the upper jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Third premolar (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Third premolar (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Second premolar (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Second premolar (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>First premolar (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>First premolar (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Third molar (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the lower jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Third incisor (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>upper fourth secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>upper fourth primary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower fourth secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower fourth primary incisor tooth</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the upper jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the lower jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Fourth incisor (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of' some 'upper jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of' some 'lower jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 3' and ('part of some 'upper jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of' some 'upper jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of some 'upper jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of' some 'lower jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 4' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>upper fifth secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the upper jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the lower jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Fifth incisor (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of' some 'upper jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of some 'upper jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of' some 'lower jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 5' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>upper fifth primary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower fifth secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower fifth primary incisor tooth</t>
+  </si>
+  <si>
+    <t>upper sixth secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>upper sixth primary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower sixth secondary incisor tooth</t>
+  </si>
+  <si>
+    <t>lower sixth primary incisor tooth</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the upper jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the upper jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the lower jaw) of the secondary set of teeth</t>
+  </si>
+  <si>
+    <t>Sixth incisor (counting anteriorposteriorly in the lower jaw) of the primary set of teeth</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of' some 'upper jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of some 'upper jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of' some 'lower jaw region') and ('part of' some 'secondary dentition')</t>
+  </si>
+  <si>
+    <t>incisor tooth 6' and ('part of' some 'lower jaw region') and ('part of' some 'primary dentition')</t>
+  </si>
+  <si>
+    <t>Incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Upper incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 1 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Lower incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 1 crown height</t>
+  </si>
+  <si>
+    <t>Incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 2 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 2 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>Upper incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>Lower incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 2 crown height</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lateral incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper lateral incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper lateral secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper lateral primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>anterior-posterior axis' and ('part of' some ('premolar tooth' 'part of' some 'tooth row'))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7582,6 +7897,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -7640,7 +7961,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7693,6 +8014,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8034,6 +8356,9 @@
   <threadedComment ref="C151" dT="2021-04-21T23:28:43.22" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{0D4CF0A9-8CA0-4BED-8E0F-2717916146F3}">
     <text>check these?</text>
   </threadedComment>
+  <threadedComment ref="C302" dT="2021-04-23T17:10:42.70" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
+    <text>Not sure if this needs a term other than 'occlusal surface'?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -8041,7 +8366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581405C8-F852-7340-B9C9-201B714E3AD5}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -8222,12 +8547,12 @@
     </row>
     <row r="24" spans="1:4">
       <c r="B24" t="s">
-        <v>2148</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="B25" t="s">
-        <v>2391</v>
+        <v>2379</v>
       </c>
     </row>
   </sheetData>
@@ -8240,9 +8565,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H240" sqref="H240"/>
+      <selection pane="bottomLeft" activeCell="I244" sqref="I244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -15173,7 +15498,7 @@
     <row r="212" spans="1:21">
       <c r="A212" s="38"/>
       <c r="C212" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>15</v>
@@ -15206,7 +15531,7 @@
     <row r="213" spans="1:21" s="16" customFormat="1">
       <c r="A213" s="38"/>
       <c r="C213" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E213" s="18" t="s">
         <v>343</v>
@@ -15241,7 +15566,7 @@
     <row r="214" spans="1:21" s="16" customFormat="1">
       <c r="A214" s="38"/>
       <c r="C214" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E214" s="30" t="s">
         <v>15</v>
@@ -15274,7 +15599,7 @@
     <row r="215" spans="1:21" s="16" customFormat="1">
       <c r="A215" s="38"/>
       <c r="C215" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E215" s="18" t="s">
         <v>343</v>
@@ -15309,7 +15634,7 @@
     <row r="216" spans="1:21" s="16" customFormat="1">
       <c r="A216" s="38"/>
       <c r="C216" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E216" s="18" t="s">
         <v>343</v>
@@ -15337,7 +15662,7 @@
     <row r="217" spans="1:21" s="16" customFormat="1">
       <c r="A217" s="38"/>
       <c r="C217" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E217" s="18" t="s">
         <v>343</v>
@@ -15365,7 +15690,7 @@
     <row r="218" spans="1:21" s="16" customFormat="1">
       <c r="A218" s="38"/>
       <c r="C218" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E218" s="18" t="s">
         <v>343</v>
@@ -15393,7 +15718,7 @@
     <row r="219" spans="1:21" s="16" customFormat="1">
       <c r="A219" s="38"/>
       <c r="C219" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E219" s="18" t="s">
         <v>343</v>
@@ -15421,7 +15746,7 @@
     <row r="220" spans="1:21" s="16" customFormat="1">
       <c r="A220" s="38"/>
       <c r="C220" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E220" s="18" t="s">
         <v>343</v>
@@ -15449,7 +15774,7 @@
     <row r="221" spans="1:21" s="16" customFormat="1">
       <c r="A221" s="38"/>
       <c r="C221" s="17" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="E221" s="18" t="s">
         <v>343</v>
@@ -22059,8 +22384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BA4F15-3142-994E-BF8B-16093E97474D}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -22362,288 +22687,288 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>2145</v>
+        <v>2141</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>2146</v>
+        <v>2142</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>2147</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>2257</v>
+        <v>2252</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>2258</v>
+        <v>2253</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>2270</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>2259</v>
+        <v>2254</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>2260</v>
+        <v>2255</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>2271</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>2263</v>
+        <v>2258</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>2266</v>
+        <v>2261</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>2300</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>2262</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>2267</v>
-      </c>
       <c r="C26" s="22" t="s">
-        <v>2301</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>2264</v>
+        <v>2259</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>2268</v>
+        <v>2263</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>2302</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>2265</v>
+        <v>2260</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>2269</v>
+        <v>2264</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>2303</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>2274</v>
+        <v>2269</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>2272</v>
+        <v>2267</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>2147</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>2275</v>
+        <v>2270</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>2273</v>
+        <v>2268</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>2270</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>2276</v>
       </c>
-      <c r="B31" s="22" t="s">
-        <v>2281</v>
-      </c>
       <c r="C31" s="22" t="s">
-        <v>2271</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>2277</v>
       </c>
-      <c r="B32" s="22" t="s">
-        <v>2282</v>
-      </c>
       <c r="C32" s="22" t="s">
-        <v>2300</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>2273</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>2278</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>2283</v>
-      </c>
       <c r="C33" s="22" t="s">
-        <v>2301</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>2279</v>
       </c>
-      <c r="B34" s="22" t="s">
-        <v>2284</v>
-      </c>
       <c r="C34" s="22" t="s">
-        <v>2302</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>2275</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>2280</v>
       </c>
-      <c r="B35" s="22" t="s">
-        <v>2285</v>
-      </c>
       <c r="C35" s="22" t="s">
-        <v>2303</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>2286</v>
+        <v>2281</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>2272</v>
+        <v>2267</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>2287</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>2288</v>
+        <v>2283</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>2273</v>
+        <v>2268</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>2294</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>2289</v>
+        <v>2284</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>2281</v>
+        <v>2276</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>2295</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>2290</v>
+        <v>2285</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>2282</v>
+        <v>2277</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>2296</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>2291</v>
+        <v>2286</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>2283</v>
+        <v>2278</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>2292</v>
+        <v>2287</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>2284</v>
+        <v>2279</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>2298</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>2293</v>
+        <v>2288</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>2285</v>
+        <v>2280</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>2299</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>2304</v>
+        <v>2299</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>2362</v>
+        <v>2351</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>2307</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="36" t="s">
-        <v>2305</v>
+      <c r="A44" s="40" t="s">
+        <v>2300</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>2363</v>
+        <v>2352</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>2308</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>2306</v>
+        <v>2301</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>2364</v>
+        <v>2353</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>2309</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="31" t="s">
-        <v>2310</v>
+        <v>2305</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>2311</v>
+        <v>2306</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>2312</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="22" t="s">
-        <v>2361</v>
+        <v>2350</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>2313</v>
+        <v>2308</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>2314</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -22651,34 +22976,35 @@
         <v>1013</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>2385</v>
+        <v>2373</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>2386</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>2397</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>2398</v>
+        <v>2385</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D346"/>
+  <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C366" sqref="C366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -24700,7 +25026,7 @@
         <v>108</v>
       </c>
       <c r="C137" s="22" t="s">
-        <v>2149</v>
+        <v>2145</v>
       </c>
       <c r="D137" t="s">
         <v>1839</v>
@@ -24714,7 +25040,7 @@
         <v>108</v>
       </c>
       <c r="C138" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="D138" t="s">
         <v>1840</v>
@@ -24728,7 +25054,7 @@
         <v>108</v>
       </c>
       <c r="C139" t="s">
-        <v>2153</v>
+        <v>2148</v>
       </c>
       <c r="D139" t="s">
         <v>1848</v>
@@ -24742,7 +25068,7 @@
         <v>108</v>
       </c>
       <c r="C140" t="s">
-        <v>2154</v>
+        <v>2149</v>
       </c>
       <c r="D140" t="s">
         <v>1842</v>
@@ -24756,7 +25082,7 @@
         <v>108</v>
       </c>
       <c r="C141" t="s">
-        <v>2155</v>
+        <v>2150</v>
       </c>
       <c r="D141" t="s">
         <v>1843</v>
@@ -24770,7 +25096,7 @@
         <v>108</v>
       </c>
       <c r="C142" t="s">
-        <v>2156</v>
+        <v>2151</v>
       </c>
       <c r="D142" t="s">
         <v>1841</v>
@@ -24784,7 +25110,7 @@
         <v>108</v>
       </c>
       <c r="C143" t="s">
-        <v>2157</v>
+        <v>2152</v>
       </c>
       <c r="D143" t="s">
         <v>1844</v>
@@ -24798,7 +25124,7 @@
         <v>112</v>
       </c>
       <c r="C144" t="s">
-        <v>2158</v>
+        <v>2153</v>
       </c>
       <c r="D144" t="s">
         <v>1856</v>
@@ -24812,7 +25138,7 @@
         <v>112</v>
       </c>
       <c r="C145" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="D145" t="s">
         <v>1857</v>
@@ -24826,7 +25152,7 @@
         <v>112</v>
       </c>
       <c r="C146" t="s">
-        <v>2153</v>
+        <v>2148</v>
       </c>
       <c r="D146" t="s">
         <v>1858</v>
@@ -24840,7 +25166,7 @@
         <v>112</v>
       </c>
       <c r="C147" t="s">
-        <v>2154</v>
+        <v>2149</v>
       </c>
       <c r="D147" t="s">
         <v>1859</v>
@@ -24854,7 +25180,7 @@
         <v>112</v>
       </c>
       <c r="C148" t="s">
-        <v>2155</v>
+        <v>2150</v>
       </c>
       <c r="D148" t="s">
         <v>1860</v>
@@ -24868,7 +25194,7 @@
         <v>112</v>
       </c>
       <c r="C149" t="s">
-        <v>2156</v>
+        <v>2151</v>
       </c>
       <c r="D149" t="s">
         <v>1861</v>
@@ -24882,7 +25208,7 @@
         <v>112</v>
       </c>
       <c r="C150" t="s">
-        <v>2157</v>
+        <v>2152</v>
       </c>
       <c r="D150" t="s">
         <v>1862</v>
@@ -24890,100 +25216,100 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>2238</v>
+        <v>2233</v>
       </c>
       <c r="B151" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C151" s="32" t="s">
-        <v>2368</v>
+        <v>2357</v>
       </c>
       <c r="D151" s="37" t="s">
-        <v>2374</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>2239</v>
+        <v>2234</v>
       </c>
       <c r="B152" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C152" s="32" t="s">
-        <v>2367</v>
+        <v>2356</v>
       </c>
       <c r="D152" t="s">
-        <v>2375</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>2240</v>
+        <v>2235</v>
       </c>
       <c r="B153" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C153" s="32" t="s">
-        <v>2369</v>
+        <v>2358</v>
       </c>
       <c r="D153" t="s">
-        <v>2376</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>2241</v>
+        <v>2236</v>
       </c>
       <c r="B154" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C154" s="32" t="s">
-        <v>2370</v>
+        <v>2359</v>
       </c>
       <c r="D154" t="s">
-        <v>2380</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>2242</v>
+        <v>2237</v>
       </c>
       <c r="B155" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C155" s="32" t="s">
-        <v>2371</v>
+        <v>2360</v>
       </c>
       <c r="D155" t="s">
-        <v>2379</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>2243</v>
+        <v>2238</v>
       </c>
       <c r="B156" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C156" s="32" t="s">
-        <v>2372</v>
+        <v>2361</v>
       </c>
       <c r="D156" t="s">
-        <v>2381</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>2244</v>
+        <v>2239</v>
       </c>
       <c r="B157" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C157" s="32" t="s">
-        <v>2373</v>
+        <v>2362</v>
       </c>
       <c r="D157" t="s">
-        <v>2382</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -24994,7 +25320,7 @@
         <v>108</v>
       </c>
       <c r="C158" t="s">
-        <v>2159</v>
+        <v>2154</v>
       </c>
       <c r="D158" t="s">
         <v>1890</v>
@@ -25008,7 +25334,7 @@
         <v>108</v>
       </c>
       <c r="C159" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
       <c r="D159" t="s">
         <v>1877</v>
@@ -25022,7 +25348,7 @@
         <v>108</v>
       </c>
       <c r="C160" t="s">
-        <v>2161</v>
+        <v>2156</v>
       </c>
       <c r="D160" t="s">
         <v>1878</v>
@@ -25036,7 +25362,7 @@
         <v>108</v>
       </c>
       <c r="C161" t="s">
-        <v>2162</v>
+        <v>2157</v>
       </c>
       <c r="D161" t="s">
         <v>1879</v>
@@ -25050,7 +25376,7 @@
         <v>108</v>
       </c>
       <c r="C162" t="s">
-        <v>2163</v>
+        <v>2158</v>
       </c>
       <c r="D162" t="s">
         <v>1880</v>
@@ -25064,7 +25390,7 @@
         <v>108</v>
       </c>
       <c r="C163" t="s">
-        <v>2164</v>
+        <v>2159</v>
       </c>
       <c r="D163" t="s">
         <v>1881</v>
@@ -25078,7 +25404,7 @@
         <v>108</v>
       </c>
       <c r="C164" t="s">
-        <v>2165</v>
+        <v>2160</v>
       </c>
       <c r="D164" t="s">
         <v>1882</v>
@@ -25092,7 +25418,7 @@
         <v>112</v>
       </c>
       <c r="C165" t="s">
-        <v>2159</v>
+        <v>2154</v>
       </c>
       <c r="D165" t="s">
         <v>1891</v>
@@ -25106,7 +25432,7 @@
         <v>112</v>
       </c>
       <c r="C166" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
       <c r="D166" t="s">
         <v>1892</v>
@@ -25120,7 +25446,7 @@
         <v>112</v>
       </c>
       <c r="C167" t="s">
-        <v>2161</v>
+        <v>2156</v>
       </c>
       <c r="D167" t="s">
         <v>1893</v>
@@ -25134,7 +25460,7 @@
         <v>112</v>
       </c>
       <c r="C168" t="s">
-        <v>2162</v>
+        <v>2157</v>
       </c>
       <c r="D168" t="s">
         <v>1894</v>
@@ -25148,7 +25474,7 @@
         <v>112</v>
       </c>
       <c r="C169" t="s">
-        <v>2163</v>
+        <v>2158</v>
       </c>
       <c r="D169" t="s">
         <v>1895</v>
@@ -25162,7 +25488,7 @@
         <v>112</v>
       </c>
       <c r="C170" t="s">
-        <v>2164</v>
+        <v>2159</v>
       </c>
       <c r="D170" t="s">
         <v>1896</v>
@@ -25176,7 +25502,7 @@
         <v>112</v>
       </c>
       <c r="C171" t="s">
-        <v>2165</v>
+        <v>2160</v>
       </c>
       <c r="D171" t="s">
         <v>1897</v>
@@ -25184,21 +25510,21 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>2245</v>
+        <v>2240</v>
       </c>
       <c r="B172" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C172" s="32" t="s">
-        <v>2252</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>2247</v>
+        <v>2242</v>
       </c>
       <c r="B173" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C173" s="32" t="s">
         <v>1870</v>
@@ -25206,10 +25532,10 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>2246</v>
+        <v>2241</v>
       </c>
       <c r="B174" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C174" s="32" t="s">
         <v>1873</v>
@@ -25217,58 +25543,58 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B175" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C175" s="32" t="s">
         <v>2248</v>
       </c>
-      <c r="B175" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C175" s="32" t="s">
-        <v>2253</v>
-      </c>
       <c r="D175" t="s">
-        <v>2377</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B176" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C176" s="32" t="s">
         <v>2249</v>
       </c>
-      <c r="B176" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C176" s="32" t="s">
-        <v>2254</v>
-      </c>
       <c r="D176" t="s">
-        <v>2378</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B177" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C177" s="32" t="s">
         <v>2250</v>
       </c>
-      <c r="B177" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C177" s="32" t="s">
-        <v>2255</v>
-      </c>
       <c r="D177" t="s">
-        <v>2377</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B178" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C178" s="32" t="s">
         <v>2251</v>
       </c>
-      <c r="B178" t="s">
-        <v>2144</v>
-      </c>
-      <c r="C178" s="32" t="s">
-        <v>2256</v>
-      </c>
       <c r="D178" t="s">
-        <v>2378</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -25279,7 +25605,7 @@
         <v>108</v>
       </c>
       <c r="C179" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
       <c r="D179" t="s">
         <v>1910</v>
@@ -25293,7 +25619,7 @@
         <v>108</v>
       </c>
       <c r="C180" t="s">
-        <v>2167</v>
+        <v>2162</v>
       </c>
       <c r="D180" t="s">
         <v>1911</v>
@@ -25307,7 +25633,7 @@
         <v>108</v>
       </c>
       <c r="C181" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
       <c r="D181" t="s">
         <v>1912</v>
@@ -25321,7 +25647,7 @@
         <v>108</v>
       </c>
       <c r="C182" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
       <c r="D182" t="s">
         <v>1913</v>
@@ -25335,7 +25661,7 @@
         <v>108</v>
       </c>
       <c r="C183" t="s">
-        <v>2170</v>
+        <v>2165</v>
       </c>
       <c r="D183" t="s">
         <v>1914</v>
@@ -25349,7 +25675,7 @@
         <v>108</v>
       </c>
       <c r="C184" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="D184" t="s">
         <v>1915</v>
@@ -25363,7 +25689,7 @@
         <v>108</v>
       </c>
       <c r="C185" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
       <c r="D185" t="s">
         <v>1916</v>
@@ -25371,13 +25697,13 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>2365</v>
+        <v>2354</v>
       </c>
       <c r="B186" t="s">
         <v>108</v>
       </c>
       <c r="C186" s="22" t="s">
-        <v>2366</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -25388,7 +25714,7 @@
         <v>112</v>
       </c>
       <c r="C192" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
       <c r="D192" t="s">
         <v>1924</v>
@@ -25402,7 +25728,7 @@
         <v>112</v>
       </c>
       <c r="C193" t="s">
-        <v>2167</v>
+        <v>2162</v>
       </c>
       <c r="D193" t="s">
         <v>1925</v>
@@ -25416,7 +25742,7 @@
         <v>112</v>
       </c>
       <c r="C194" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
       <c r="D194" t="s">
         <v>1926</v>
@@ -25430,7 +25756,7 @@
         <v>112</v>
       </c>
       <c r="C195" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
       <c r="D195" t="s">
         <v>1927</v>
@@ -25444,7 +25770,7 @@
         <v>112</v>
       </c>
       <c r="C196" t="s">
-        <v>2170</v>
+        <v>2165</v>
       </c>
       <c r="D196" t="s">
         <v>1928</v>
@@ -25458,7 +25784,7 @@
         <v>112</v>
       </c>
       <c r="C197" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="D197" t="s">
         <v>1929</v>
@@ -25472,7 +25798,7 @@
         <v>112</v>
       </c>
       <c r="C198" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
       <c r="D198" t="s">
         <v>1930</v>
@@ -25486,7 +25812,7 @@
         <v>108</v>
       </c>
       <c r="C199" t="s">
-        <v>2173</v>
+        <v>2168</v>
       </c>
       <c r="D199" t="s">
         <v>1941</v>
@@ -25500,7 +25826,7 @@
         <v>108</v>
       </c>
       <c r="C200" t="s">
-        <v>2174</v>
+        <v>2169</v>
       </c>
       <c r="D200" t="s">
         <v>1942</v>
@@ -25514,7 +25840,7 @@
         <v>108</v>
       </c>
       <c r="C201" t="s">
-        <v>2175</v>
+        <v>2170</v>
       </c>
       <c r="D201" t="s">
         <v>1943</v>
@@ -25528,7 +25854,7 @@
         <v>112</v>
       </c>
       <c r="C202" t="s">
-        <v>2173</v>
+        <v>2168</v>
       </c>
       <c r="D202" t="s">
         <v>1946</v>
@@ -25542,7 +25868,7 @@
         <v>112</v>
       </c>
       <c r="C203" t="s">
-        <v>2174</v>
+        <v>2169</v>
       </c>
       <c r="D203" t="s">
         <v>1947</v>
@@ -25556,7 +25882,7 @@
         <v>112</v>
       </c>
       <c r="C204" t="s">
-        <v>2175</v>
+        <v>2170</v>
       </c>
       <c r="D204" t="s">
         <v>1948</v>
@@ -25564,72 +25890,72 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>2315</v>
+        <v>2310</v>
       </c>
       <c r="B205" t="s">
         <v>112</v>
       </c>
       <c r="C205" s="22" t="s">
-        <v>2320</v>
+        <v>2315</v>
       </c>
       <c r="D205" t="s">
-        <v>2355</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>2316</v>
+        <v>2311</v>
       </c>
       <c r="B206" t="s">
         <v>112</v>
       </c>
       <c r="C206" s="22" t="s">
-        <v>2353</v>
+        <v>2342</v>
       </c>
       <c r="D206" t="s">
-        <v>2356</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>2317</v>
+        <v>2312</v>
       </c>
       <c r="B207" t="s">
         <v>112</v>
       </c>
       <c r="C207" s="22" t="s">
-        <v>2354</v>
+        <v>2343</v>
       </c>
       <c r="D207" t="s">
-        <v>2357</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>2318</v>
+        <v>2313</v>
       </c>
       <c r="B208" t="s">
         <v>108</v>
       </c>
       <c r="C208" s="22" t="s">
-        <v>2320</v>
+        <v>2315</v>
       </c>
       <c r="D208" t="s">
-        <v>2358</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>2319</v>
+        <v>2314</v>
       </c>
       <c r="B209" t="s">
         <v>108</v>
       </c>
       <c r="C209" s="22" t="s">
-        <v>2353</v>
+        <v>2342</v>
       </c>
       <c r="D209" t="s">
-        <v>2359</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -25640,10 +25966,10 @@
         <v>108</v>
       </c>
       <c r="C210" s="22" t="s">
-        <v>2354</v>
+        <v>2343</v>
       </c>
       <c r="D210" t="s">
-        <v>2360</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -25654,7 +25980,7 @@
         <v>108</v>
       </c>
       <c r="C211" t="s">
-        <v>2176</v>
+        <v>2171</v>
       </c>
       <c r="D211" t="s">
         <v>1961</v>
@@ -25668,7 +25994,7 @@
         <v>108</v>
       </c>
       <c r="C212" t="s">
-        <v>2177</v>
+        <v>2172</v>
       </c>
       <c r="D212" t="s">
         <v>1962</v>
@@ -25682,7 +26008,7 @@
         <v>108</v>
       </c>
       <c r="C213" t="s">
-        <v>2178</v>
+        <v>2173</v>
       </c>
       <c r="D213" t="s">
         <v>1963</v>
@@ -25696,7 +26022,7 @@
         <v>108</v>
       </c>
       <c r="C214" t="s">
-        <v>2179</v>
+        <v>2174</v>
       </c>
       <c r="D214" t="s">
         <v>1964</v>
@@ -25710,7 +26036,7 @@
         <v>108</v>
       </c>
       <c r="C215" t="s">
-        <v>2180</v>
+        <v>2175</v>
       </c>
       <c r="D215" t="s">
         <v>1965</v>
@@ -25724,7 +26050,7 @@
         <v>108</v>
       </c>
       <c r="C216" t="s">
-        <v>2181</v>
+        <v>2176</v>
       </c>
       <c r="D216" t="s">
         <v>1966</v>
@@ -25738,7 +26064,7 @@
         <v>108</v>
       </c>
       <c r="C217" t="s">
-        <v>2182</v>
+        <v>2177</v>
       </c>
       <c r="D217" t="s">
         <v>1967</v>
@@ -25752,7 +26078,7 @@
         <v>112</v>
       </c>
       <c r="C218" t="s">
-        <v>2176</v>
+        <v>2171</v>
       </c>
       <c r="D218" t="s">
         <v>1975</v>
@@ -25766,7 +26092,7 @@
         <v>112</v>
       </c>
       <c r="C219" t="s">
-        <v>2177</v>
+        <v>2172</v>
       </c>
       <c r="D219" t="s">
         <v>1976</v>
@@ -25780,7 +26106,7 @@
         <v>112</v>
       </c>
       <c r="C220" t="s">
-        <v>2178</v>
+        <v>2173</v>
       </c>
       <c r="D220" t="s">
         <v>1977</v>
@@ -25794,7 +26120,7 @@
         <v>112</v>
       </c>
       <c r="C221" t="s">
-        <v>2179</v>
+        <v>2174</v>
       </c>
       <c r="D221" t="s">
         <v>1978</v>
@@ -25808,7 +26134,7 @@
         <v>112</v>
       </c>
       <c r="C222" t="s">
-        <v>2180</v>
+        <v>2175</v>
       </c>
       <c r="D222" t="s">
         <v>1979</v>
@@ -25822,7 +26148,7 @@
         <v>112</v>
       </c>
       <c r="C223" t="s">
-        <v>2181</v>
+        <v>2176</v>
       </c>
       <c r="D223" t="s">
         <v>1980</v>
@@ -25836,7 +26162,7 @@
         <v>112</v>
       </c>
       <c r="C224" t="s">
-        <v>2182</v>
+        <v>2177</v>
       </c>
       <c r="D224" t="s">
         <v>1981</v>
@@ -25850,7 +26176,7 @@
         <v>108</v>
       </c>
       <c r="C225" t="s">
-        <v>2183</v>
+        <v>2178</v>
       </c>
       <c r="D225" t="s">
         <v>1993</v>
@@ -25864,7 +26190,7 @@
         <v>108</v>
       </c>
       <c r="C226" t="s">
-        <v>2184</v>
+        <v>2179</v>
       </c>
       <c r="D226" t="s">
         <v>1994</v>
@@ -25878,7 +26204,7 @@
         <v>108</v>
       </c>
       <c r="C227" t="s">
-        <v>2185</v>
+        <v>2180</v>
       </c>
       <c r="D227" t="s">
         <v>1995</v>
@@ -25892,7 +26218,7 @@
         <v>108</v>
       </c>
       <c r="C228" t="s">
-        <v>2186</v>
+        <v>2181</v>
       </c>
       <c r="D228" t="s">
         <v>1996</v>
@@ -25906,7 +26232,7 @@
         <v>108</v>
       </c>
       <c r="C229" t="s">
-        <v>2187</v>
+        <v>2182</v>
       </c>
       <c r="D229" t="s">
         <v>1997</v>
@@ -25920,7 +26246,7 @@
         <v>108</v>
       </c>
       <c r="C230" t="s">
-        <v>2188</v>
+        <v>2183</v>
       </c>
       <c r="D230" t="s">
         <v>1998</v>
@@ -25934,7 +26260,7 @@
         <v>108</v>
       </c>
       <c r="C231" t="s">
-        <v>2189</v>
+        <v>2184</v>
       </c>
       <c r="D231" t="s">
         <v>1999</v>
@@ -25948,7 +26274,7 @@
         <v>112</v>
       </c>
       <c r="C232" t="s">
-        <v>2183</v>
+        <v>2178</v>
       </c>
       <c r="D232" t="s">
         <v>2007</v>
@@ -25962,7 +26288,7 @@
         <v>112</v>
       </c>
       <c r="C233" t="s">
-        <v>2184</v>
+        <v>2179</v>
       </c>
       <c r="D233" t="s">
         <v>2008</v>
@@ -25976,7 +26302,7 @@
         <v>112</v>
       </c>
       <c r="C234" t="s">
-        <v>2185</v>
+        <v>2180</v>
       </c>
       <c r="D234" t="s">
         <v>2009</v>
@@ -25990,7 +26316,7 @@
         <v>112</v>
       </c>
       <c r="C235" t="s">
-        <v>2186</v>
+        <v>2181</v>
       </c>
       <c r="D235" t="s">
         <v>2010</v>
@@ -26004,7 +26330,7 @@
         <v>112</v>
       </c>
       <c r="C236" t="s">
-        <v>2187</v>
+        <v>2182</v>
       </c>
       <c r="D236" t="s">
         <v>2011</v>
@@ -26018,7 +26344,7 @@
         <v>112</v>
       </c>
       <c r="C237" t="s">
-        <v>2188</v>
+        <v>2183</v>
       </c>
       <c r="D237" t="s">
         <v>2012</v>
@@ -26032,7 +26358,7 @@
         <v>112</v>
       </c>
       <c r="C238" t="s">
-        <v>2189</v>
+        <v>2184</v>
       </c>
       <c r="D238" t="s">
         <v>2013</v>
@@ -26046,7 +26372,7 @@
         <v>108</v>
       </c>
       <c r="C239" t="s">
-        <v>2190</v>
+        <v>2185</v>
       </c>
       <c r="D239" t="s">
         <v>2029</v>
@@ -26060,7 +26386,7 @@
         <v>108</v>
       </c>
       <c r="C240" t="s">
-        <v>2191</v>
+        <v>2186</v>
       </c>
       <c r="D240" t="s">
         <v>2030</v>
@@ -26074,7 +26400,7 @@
         <v>108</v>
       </c>
       <c r="C241" t="s">
-        <v>2192</v>
+        <v>2187</v>
       </c>
       <c r="D241" t="s">
         <v>2031</v>
@@ -26088,7 +26414,7 @@
         <v>108</v>
       </c>
       <c r="C242" t="s">
-        <v>2193</v>
+        <v>2188</v>
       </c>
       <c r="D242" t="s">
         <v>2032</v>
@@ -26102,7 +26428,7 @@
         <v>108</v>
       </c>
       <c r="C243" t="s">
-        <v>2194</v>
+        <v>2189</v>
       </c>
       <c r="D243" t="s">
         <v>2033</v>
@@ -26116,7 +26442,7 @@
         <v>108</v>
       </c>
       <c r="C244" t="s">
-        <v>2195</v>
+        <v>2190</v>
       </c>
       <c r="D244" t="s">
         <v>2034</v>
@@ -26130,7 +26456,7 @@
         <v>108</v>
       </c>
       <c r="C245" t="s">
-        <v>2196</v>
+        <v>2191</v>
       </c>
       <c r="D245" t="s">
         <v>2035</v>
@@ -26144,7 +26470,7 @@
         <v>112</v>
       </c>
       <c r="C246" t="s">
-        <v>2190</v>
+        <v>2185</v>
       </c>
       <c r="D246" t="s">
         <v>2043</v>
@@ -26158,7 +26484,7 @@
         <v>112</v>
       </c>
       <c r="C247" t="s">
-        <v>2191</v>
+        <v>2186</v>
       </c>
       <c r="D247" t="s">
         <v>2044</v>
@@ -26172,7 +26498,7 @@
         <v>112</v>
       </c>
       <c r="C248" t="s">
-        <v>2192</v>
+        <v>2187</v>
       </c>
       <c r="D248" t="s">
         <v>2045</v>
@@ -26186,7 +26512,7 @@
         <v>112</v>
       </c>
       <c r="C249" t="s">
-        <v>2193</v>
+        <v>2188</v>
       </c>
       <c r="D249" t="s">
         <v>2046</v>
@@ -26200,7 +26526,7 @@
         <v>112</v>
       </c>
       <c r="C250" t="s">
-        <v>2194</v>
+        <v>2189</v>
       </c>
       <c r="D250" t="s">
         <v>2047</v>
@@ -26214,7 +26540,7 @@
         <v>112</v>
       </c>
       <c r="C251" t="s">
-        <v>2195</v>
+        <v>2190</v>
       </c>
       <c r="D251" t="s">
         <v>2048</v>
@@ -26228,7 +26554,7 @@
         <v>112</v>
       </c>
       <c r="C252" t="s">
-        <v>2196</v>
+        <v>2191</v>
       </c>
       <c r="D252" t="s">
         <v>2049</v>
@@ -26242,7 +26568,7 @@
         <v>108</v>
       </c>
       <c r="C253" t="s">
-        <v>2197</v>
+        <v>2192</v>
       </c>
       <c r="D253" t="s">
         <v>2062</v>
@@ -26256,7 +26582,7 @@
         <v>108</v>
       </c>
       <c r="C254" t="s">
-        <v>2198</v>
+        <v>2193</v>
       </c>
       <c r="D254" t="s">
         <v>2063</v>
@@ -26270,7 +26596,7 @@
         <v>108</v>
       </c>
       <c r="C255" t="s">
-        <v>2199</v>
+        <v>2194</v>
       </c>
       <c r="D255" t="s">
         <v>2064</v>
@@ -26284,7 +26610,7 @@
         <v>108</v>
       </c>
       <c r="C256" t="s">
-        <v>2200</v>
+        <v>2195</v>
       </c>
       <c r="D256" t="s">
         <v>2065</v>
@@ -26298,7 +26624,7 @@
         <v>108</v>
       </c>
       <c r="C257" t="s">
-        <v>2201</v>
+        <v>2196</v>
       </c>
       <c r="D257" t="s">
         <v>2066</v>
@@ -26312,7 +26638,7 @@
         <v>108</v>
       </c>
       <c r="C258" t="s">
-        <v>2202</v>
+        <v>2197</v>
       </c>
       <c r="D258" t="s">
         <v>2067</v>
@@ -26326,7 +26652,7 @@
         <v>108</v>
       </c>
       <c r="C259" t="s">
-        <v>2203</v>
+        <v>2198</v>
       </c>
       <c r="D259" t="s">
         <v>2068</v>
@@ -26340,7 +26666,7 @@
         <v>112</v>
       </c>
       <c r="C260" t="s">
-        <v>2197</v>
+        <v>2192</v>
       </c>
       <c r="D260" t="s">
         <v>2076</v>
@@ -26354,7 +26680,7 @@
         <v>112</v>
       </c>
       <c r="C261" t="s">
-        <v>2198</v>
+        <v>2193</v>
       </c>
       <c r="D261" t="s">
         <v>2077</v>
@@ -26368,7 +26694,7 @@
         <v>112</v>
       </c>
       <c r="C262" t="s">
-        <v>2199</v>
+        <v>2194</v>
       </c>
       <c r="D262" t="s">
         <v>2078</v>
@@ -26382,7 +26708,7 @@
         <v>112</v>
       </c>
       <c r="C263" t="s">
-        <v>2200</v>
+        <v>2195</v>
       </c>
       <c r="D263" t="s">
         <v>2079</v>
@@ -26396,7 +26722,7 @@
         <v>112</v>
       </c>
       <c r="C264" t="s">
-        <v>2201</v>
+        <v>2196</v>
       </c>
       <c r="D264" t="s">
         <v>2080</v>
@@ -26410,7 +26736,7 @@
         <v>112</v>
       </c>
       <c r="C265" t="s">
-        <v>2202</v>
+        <v>2197</v>
       </c>
       <c r="D265" t="s">
         <v>2081</v>
@@ -26424,7 +26750,7 @@
         <v>112</v>
       </c>
       <c r="C266" t="s">
-        <v>2203</v>
+        <v>2198</v>
       </c>
       <c r="D266" t="s">
         <v>2082</v>
@@ -26438,7 +26764,7 @@
         <v>108</v>
       </c>
       <c r="C267" t="s">
-        <v>2204</v>
+        <v>2199</v>
       </c>
       <c r="D267" t="s">
         <v>2099</v>
@@ -26452,7 +26778,7 @@
         <v>108</v>
       </c>
       <c r="C268" t="s">
-        <v>2205</v>
+        <v>2200</v>
       </c>
       <c r="D268" t="s">
         <v>2100</v>
@@ -26466,7 +26792,7 @@
         <v>108</v>
       </c>
       <c r="C269" t="s">
-        <v>2206</v>
+        <v>2201</v>
       </c>
       <c r="D269" t="s">
         <v>2101</v>
@@ -26480,7 +26806,7 @@
         <v>108</v>
       </c>
       <c r="C270" t="s">
-        <v>2207</v>
+        <v>2202</v>
       </c>
       <c r="D270" t="s">
         <v>2102</v>
@@ -26494,7 +26820,7 @@
         <v>108</v>
       </c>
       <c r="C271" t="s">
-        <v>2208</v>
+        <v>2203</v>
       </c>
       <c r="D271" t="s">
         <v>2103</v>
@@ -26508,7 +26834,7 @@
         <v>108</v>
       </c>
       <c r="C272" t="s">
-        <v>2209</v>
+        <v>2204</v>
       </c>
       <c r="D272" t="s">
         <v>2104</v>
@@ -26522,7 +26848,7 @@
         <v>108</v>
       </c>
       <c r="C273" t="s">
-        <v>2210</v>
+        <v>2205</v>
       </c>
       <c r="D273" t="s">
         <v>2105</v>
@@ -26536,7 +26862,7 @@
         <v>112</v>
       </c>
       <c r="C274" t="s">
-        <v>2204</v>
+        <v>2199</v>
       </c>
       <c r="D274" t="s">
         <v>2106</v>
@@ -26550,7 +26876,7 @@
         <v>112</v>
       </c>
       <c r="C275" t="s">
-        <v>2205</v>
+        <v>2200</v>
       </c>
       <c r="D275" t="s">
         <v>2107</v>
@@ -26564,7 +26890,7 @@
         <v>112</v>
       </c>
       <c r="C276" t="s">
-        <v>2206</v>
+        <v>2201</v>
       </c>
       <c r="D276" t="s">
         <v>2108</v>
@@ -26578,7 +26904,7 @@
         <v>112</v>
       </c>
       <c r="C277" t="s">
-        <v>2207</v>
+        <v>2202</v>
       </c>
       <c r="D277" t="s">
         <v>2111</v>
@@ -26592,7 +26918,7 @@
         <v>112</v>
       </c>
       <c r="C278" t="s">
-        <v>2208</v>
+        <v>2203</v>
       </c>
       <c r="D278" t="s">
         <v>2109</v>
@@ -26606,7 +26932,7 @@
         <v>112</v>
       </c>
       <c r="C279" t="s">
-        <v>2209</v>
+        <v>2204</v>
       </c>
       <c r="D279" t="s">
         <v>2112</v>
@@ -26620,7 +26946,7 @@
         <v>112</v>
       </c>
       <c r="C280" t="s">
-        <v>2210</v>
+        <v>2205</v>
       </c>
       <c r="D280" t="s">
         <v>2110</v>
@@ -26634,7 +26960,7 @@
         <v>112</v>
       </c>
       <c r="C281" s="16" t="s">
-        <v>2211</v>
+        <v>2206</v>
       </c>
       <c r="D281" t="s">
         <v>2122</v>
@@ -26648,7 +26974,7 @@
         <v>112</v>
       </c>
       <c r="C282" s="16" t="s">
-        <v>2212</v>
+        <v>2207</v>
       </c>
       <c r="D282" t="s">
         <v>2123</v>
@@ -26662,7 +26988,7 @@
         <v>112</v>
       </c>
       <c r="C283" s="16" t="s">
-        <v>2213</v>
+        <v>2208</v>
       </c>
       <c r="D283" t="s">
         <v>2124</v>
@@ -26676,10 +27002,10 @@
         <v>112</v>
       </c>
       <c r="C284" s="16" t="s">
-        <v>2214</v>
+        <v>2209</v>
       </c>
       <c r="D284" t="s">
-        <v>2125</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -26690,10 +27016,10 @@
         <v>112</v>
       </c>
       <c r="C285" s="16" t="s">
-        <v>2215</v>
+        <v>2210</v>
       </c>
       <c r="D285" t="s">
-        <v>2126</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -26704,10 +27030,10 @@
         <v>112</v>
       </c>
       <c r="C286" s="16" t="s">
-        <v>2216</v>
+        <v>2211</v>
       </c>
       <c r="D286" t="s">
-        <v>2127</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -26718,404 +27044,945 @@
         <v>112</v>
       </c>
       <c r="C287" s="16" t="s">
-        <v>2217</v>
+        <v>2212</v>
       </c>
       <c r="D287" t="s">
-        <v>2128</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="31" t="s">
-        <v>2129</v>
+        <v>2125</v>
       </c>
       <c r="B288" t="s">
         <v>108</v>
       </c>
       <c r="C288" s="16" t="s">
-        <v>2211</v>
+        <v>2206</v>
       </c>
       <c r="D288" t="s">
-        <v>2136</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="289" spans="1:4">
       <c r="A289" s="31" t="s">
-        <v>2130</v>
+        <v>2126</v>
       </c>
       <c r="B289" t="s">
         <v>108</v>
       </c>
       <c r="C289" s="16" t="s">
-        <v>2212</v>
+        <v>2207</v>
       </c>
       <c r="D289" t="s">
-        <v>2137</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="31" t="s">
-        <v>2131</v>
+        <v>2127</v>
       </c>
       <c r="B290" t="s">
         <v>108</v>
       </c>
       <c r="C290" s="16" t="s">
-        <v>2213</v>
+        <v>2208</v>
       </c>
       <c r="D290" t="s">
-        <v>2138</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="31" t="s">
-        <v>2132</v>
+        <v>2128</v>
       </c>
       <c r="B291" t="s">
         <v>108</v>
       </c>
       <c r="C291" t="s">
-        <v>2214</v>
+        <v>2209</v>
       </c>
       <c r="D291" t="s">
-        <v>2139</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="31" t="s">
-        <v>2133</v>
+        <v>2129</v>
       </c>
       <c r="B292" t="s">
         <v>108</v>
       </c>
       <c r="C292" t="s">
-        <v>2215</v>
+        <v>2210</v>
       </c>
       <c r="D292" t="s">
-        <v>2140</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="31" t="s">
-        <v>2134</v>
+        <v>2130</v>
       </c>
       <c r="B293" t="s">
         <v>108</v>
       </c>
       <c r="C293" t="s">
-        <v>2216</v>
+        <v>2211</v>
       </c>
       <c r="D293" t="s">
-        <v>2141</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="31" t="s">
-        <v>2135</v>
+        <v>2131</v>
       </c>
       <c r="B294" t="s">
         <v>108</v>
       </c>
       <c r="C294" t="s">
-        <v>2217</v>
+        <v>2212</v>
       </c>
       <c r="D294" t="s">
-        <v>2142</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="16" t="s">
-        <v>2143</v>
+        <v>2139</v>
       </c>
       <c r="B295" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C295" s="32" t="s">
-        <v>2226</v>
+        <v>2221</v>
       </c>
       <c r="D295" t="s">
-        <v>2218</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="296" spans="1:4">
       <c r="A296" s="16" t="s">
-        <v>2219</v>
+        <v>2214</v>
       </c>
       <c r="B296" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C296" s="32" t="s">
-        <v>2225</v>
+        <v>2220</v>
       </c>
       <c r="D296" t="s">
-        <v>2232</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="297" spans="1:4">
       <c r="A297" s="16" t="s">
-        <v>2220</v>
+        <v>2215</v>
       </c>
       <c r="B297" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C297" s="32" t="s">
-        <v>2227</v>
+        <v>2222</v>
       </c>
       <c r="D297" t="s">
-        <v>2233</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="298" spans="1:4">
       <c r="A298" s="16" t="s">
-        <v>2221</v>
+        <v>2216</v>
       </c>
       <c r="B298" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C298" s="32" t="s">
-        <v>2228</v>
+        <v>2223</v>
       </c>
       <c r="D298" t="s">
-        <v>2234</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="16" t="s">
-        <v>2222</v>
+        <v>2217</v>
       </c>
       <c r="B299" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C299" s="32" t="s">
-        <v>2229</v>
+        <v>2224</v>
       </c>
       <c r="D299" t="s">
-        <v>2236</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="16" t="s">
-        <v>2223</v>
+        <v>2218</v>
       </c>
       <c r="B300" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C300" s="32" t="s">
+        <v>2225</v>
+      </c>
+      <c r="D300" t="s">
         <v>2230</v>
-      </c>
-      <c r="D300" t="s">
-        <v>2235</v>
       </c>
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="16" t="s">
-        <v>2224</v>
+        <v>2219</v>
       </c>
       <c r="B301" s="16" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="C301" s="32" t="s">
-        <v>2231</v>
+        <v>2226</v>
       </c>
       <c r="D301" t="s">
-        <v>2237</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="16" t="s">
-        <v>2383</v>
+        <v>2372</v>
       </c>
       <c r="B302" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C302" s="32" t="s">
-        <v>2384</v>
+      <c r="C302" s="37" t="s">
+        <v>2426</v>
       </c>
     </row>
     <row r="303" spans="1:4">
-      <c r="A303" s="16"/>
-      <c r="B303" s="16"/>
-      <c r="C303" s="32"/>
-    </row>
-    <row r="304" spans="1:4">
-      <c r="A304" s="16"/>
-      <c r="B304" s="16"/>
-      <c r="C304" s="32"/>
-    </row>
-    <row r="305" spans="1:4">
+      <c r="A303" s="16" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B303" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C303" s="37" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A304" s="16" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B304" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C304" s="37" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A305" s="16" t="s">
-        <v>2431</v>
+        <v>2422</v>
       </c>
       <c r="B305" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C305" s="37" t="s">
-        <v>2392</v>
-      </c>
-      <c r="D305" t="s">
-        <v>2393</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A306" s="16" t="s">
-        <v>2394</v>
+        <v>2423</v>
       </c>
       <c r="B306" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C306" s="37" t="s">
-        <v>2395</v>
-      </c>
-    </row>
-    <row r="307" spans="1:4">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A307" s="16" t="s">
-        <v>2432</v>
+        <v>2424</v>
       </c>
       <c r="B307" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C307" s="37"/>
-    </row>
-    <row r="308" spans="1:4">
+      <c r="C307" s="37" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A308" s="16" t="s">
-        <v>2396</v>
+        <v>2425</v>
       </c>
       <c r="B308" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C308" s="37"/>
-    </row>
-    <row r="309" spans="1:4">
-      <c r="A309" s="16"/>
-      <c r="B309" s="16"/>
-      <c r="C309" s="37"/>
-    </row>
-    <row r="310" spans="1:4">
-      <c r="A310" s="16"/>
-      <c r="B310" s="16"/>
-      <c r="C310" s="37"/>
-    </row>
-    <row r="311" spans="1:4">
-      <c r="A311" s="16"/>
-      <c r="B311" s="16"/>
-      <c r="C311" s="37"/>
-    </row>
-    <row r="312" spans="1:4">
-      <c r="A312" s="16"/>
-      <c r="B312" s="16"/>
-      <c r="C312" s="37"/>
-    </row>
-    <row r="322" spans="1:4">
-      <c r="A322" t="s">
+      <c r="C308" s="37" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A309" s="16" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B309" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C309" s="37" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A310" s="16" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B310" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C310" s="37" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A311" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="B311" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C311" s="37" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A312" s="16" t="s">
+        <v>2496</v>
+      </c>
+      <c r="B312" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C312" s="37" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A313" s="16" t="s">
+        <v>2497</v>
+      </c>
+      <c r="B313" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C313" s="37" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A314" s="16" t="s">
+        <v>2498</v>
+      </c>
+      <c r="B314" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C314" s="37" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A315" s="16" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B315" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C315" s="37" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A316" s="16" t="s">
+        <v>2493</v>
+      </c>
+      <c r="B316" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C316" s="37" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A317" s="16" t="s">
+        <v>2500</v>
+      </c>
+      <c r="B317" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C317" s="37" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A318" s="16" t="s">
+        <v>2501</v>
+      </c>
+      <c r="B318" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C318" s="37" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A319" s="16" t="s">
+        <v>2502</v>
+      </c>
+      <c r="B319" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C319" s="37" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A320" s="16" t="s">
+        <v>2503</v>
+      </c>
+      <c r="B320" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C320" s="37" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A321" s="16" t="s">
+        <v>2504</v>
+      </c>
+      <c r="B321" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C321" s="37" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A322" s="16" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B322" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C322" s="37" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A323" s="16" t="s">
+        <v>2506</v>
+      </c>
+      <c r="B323" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C323" s="37" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A324" s="16" t="s">
+        <v>2507</v>
+      </c>
+      <c r="B324" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C324" s="37" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A325" s="16" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B325" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C325" s="37" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A326" s="16" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B326" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C326" s="37" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A327" s="16" t="s">
+        <v>2510</v>
+      </c>
+      <c r="B327" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C327" s="37" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A328" s="16" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B328" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C328" s="37" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A329" s="16" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B329" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C329" s="37" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A330" s="16" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B330" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C330" s="37" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A331" s="16" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B331" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C331" s="37" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A332" s="16" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B332" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C332" s="37" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A333" s="16" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B333" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C333" s="37" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A334" s="16" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B334" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C334" s="37" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A335" s="16" t="s">
+        <v>2518</v>
+      </c>
+      <c r="B335" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C335" s="37" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A336" s="16" t="s">
+        <v>2519</v>
+      </c>
+      <c r="B336" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C336" s="37" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A337" s="16" t="s">
+        <v>2520</v>
+      </c>
+      <c r="B337" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C337" s="37" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A338" s="16" t="s">
+        <v>2521</v>
+      </c>
+      <c r="B338" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C338" s="37" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A339" s="16" t="s">
+        <v>2522</v>
+      </c>
+      <c r="B339" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C339" s="37" t="s">
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A340" s="16" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B340" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C340" s="37" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A341" s="16" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B341" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C341" s="37" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A342" s="16" t="s">
+        <v>2525</v>
+      </c>
+      <c r="B342" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C342" s="37" t="s">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A343" s="16" t="s">
+        <v>2526</v>
+      </c>
+      <c r="B343" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C343" s="37" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A344" s="16"/>
+      <c r="B344" s="16"/>
+      <c r="C344" s="37"/>
+    </row>
+    <row r="345" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A345" s="16"/>
+      <c r="B345" s="16"/>
+      <c r="C345" s="37"/>
+    </row>
+    <row r="346" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A346" s="16"/>
+      <c r="B346" s="16"/>
+      <c r="C346" s="37"/>
+    </row>
+    <row r="347" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A347" s="16"/>
+      <c r="B347" s="16"/>
+      <c r="C347" s="37"/>
+    </row>
+    <row r="348" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A348" s="16"/>
+      <c r="B348" s="16"/>
+      <c r="C348" s="37"/>
+    </row>
+    <row r="349" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A349" s="16"/>
+      <c r="B349" s="16"/>
+      <c r="C349" s="37"/>
+    </row>
+    <row r="350" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A350" s="16"/>
+      <c r="B350" s="16"/>
+      <c r="C350" s="37"/>
+    </row>
+    <row r="351" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A351" s="16"/>
+      <c r="B351" s="16"/>
+      <c r="C351" s="37"/>
+    </row>
+    <row r="352" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A352" s="16"/>
+      <c r="B352" s="16"/>
+      <c r="C352" s="37"/>
+    </row>
+    <row r="353" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A353" s="16"/>
+      <c r="B353" s="16"/>
+      <c r="C353" s="37"/>
+    </row>
+    <row r="354" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A354" s="16"/>
+      <c r="B354" s="16"/>
+      <c r="C354" s="37"/>
+    </row>
+    <row r="355" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A355" s="16"/>
+      <c r="B355" s="16"/>
+      <c r="C355" s="37"/>
+    </row>
+    <row r="356" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A356" s="16"/>
+      <c r="B356" s="16"/>
+      <c r="C356" s="37"/>
+    </row>
+    <row r="357" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A357" s="16"/>
+      <c r="B357" s="16"/>
+      <c r="C357" s="37"/>
+    </row>
+    <row r="358" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A358" s="16"/>
+      <c r="B358" s="16"/>
+      <c r="C358" s="37"/>
+    </row>
+    <row r="359" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A359" s="16"/>
+      <c r="B359" s="16"/>
+      <c r="C359" s="37"/>
+    </row>
+    <row r="360" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A360" s="16"/>
+      <c r="B360" s="16"/>
+      <c r="C360" s="37"/>
+    </row>
+    <row r="361" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A361" s="16"/>
+      <c r="B361" s="16"/>
+      <c r="C361" s="37"/>
+    </row>
+    <row r="362" spans="1:4">
+      <c r="A362" s="16"/>
+      <c r="B362" s="16"/>
+      <c r="C362" s="37"/>
+    </row>
+    <row r="363" spans="1:4">
+      <c r="A363" s="16"/>
+      <c r="B363" s="16"/>
+      <c r="C363" s="37"/>
+    </row>
+    <row r="364" spans="1:4">
+      <c r="A364" s="16" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B364" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C364" s="37" t="s">
+        <v>2534</v>
+      </c>
+      <c r="D364" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4">
+      <c r="A365" s="16" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B365" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C365" s="37" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4">
+      <c r="A366" s="16" t="s">
+        <v>2419</v>
+      </c>
+      <c r="B366" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C366" s="37"/>
+    </row>
+    <row r="367" spans="1:4">
+      <c r="A367" s="16" t="s">
+        <v>2383</v>
+      </c>
+      <c r="B367" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C367" s="37"/>
+    </row>
+    <row r="368" spans="1:4">
+      <c r="A368" s="16"/>
+      <c r="B368" s="16"/>
+      <c r="C368" s="37"/>
+    </row>
+    <row r="369" spans="1:4">
+      <c r="A369" s="16"/>
+      <c r="B369" s="16"/>
+      <c r="C369" s="37"/>
+    </row>
+    <row r="370" spans="1:4">
+      <c r="A370" s="16"/>
+      <c r="B370" s="16"/>
+      <c r="C370" s="37"/>
+    </row>
+    <row r="371" spans="1:4">
+      <c r="A371" s="16"/>
+      <c r="B371" s="16"/>
+      <c r="C371" s="37"/>
+    </row>
+    <row r="381" spans="1:4">
+      <c r="A381" t="s">
         <v>1230</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B381" t="s">
         <v>1217</v>
       </c>
-      <c r="C322" s="22" t="s">
+      <c r="C381" s="22" t="s">
         <v>1218</v>
       </c>
-      <c r="D322" t="str">
-        <f>"line along "&amp;B322&amp;" of "&amp;C322</f>
+      <c r="D381" t="str">
+        <f>"line along "&amp;B381&amp;" of "&amp;C381</f>
         <v>line along proximal-distal of lateral side' some talus</v>
       </c>
     </row>
-    <row r="323" spans="1:4">
-      <c r="A323" t="s">
+    <row r="382" spans="1:4">
+      <c r="A382" t="s">
         <v>1216</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B382" t="s">
         <v>1217</v>
       </c>
-      <c r="C323" t="s">
+      <c r="C382" t="s">
         <v>1219</v>
       </c>
-      <c r="D323" t="str">
-        <f>"line along "&amp;B323&amp;" of "&amp;C323</f>
+      <c r="D382" t="str">
+        <f>"line along "&amp;B382&amp;" of "&amp;C382</f>
         <v>line along proximal-distal of pes</v>
       </c>
     </row>
-    <row r="324" spans="1:4">
-      <c r="A324" t="s">
+    <row r="383" spans="1:4">
+      <c r="A383" t="s">
         <v>1220</v>
       </c>
     </row>
-    <row r="325" spans="1:4">
-      <c r="A325" t="s">
+    <row r="384" spans="1:4">
+      <c r="A384" t="s">
         <v>1221</v>
       </c>
     </row>
-    <row r="326" spans="1:4">
-      <c r="A326" t="s">
+    <row r="385" spans="1:1">
+      <c r="A385" t="s">
         <v>1222</v>
       </c>
     </row>
-    <row r="327" spans="1:4">
-      <c r="A327" t="s">
+    <row r="386" spans="1:1">
+      <c r="A386" t="s">
         <v>1223</v>
       </c>
     </row>
-    <row r="328" spans="1:4">
-      <c r="A328" t="s">
+    <row r="387" spans="1:1">
+      <c r="A387" t="s">
         <v>1224</v>
       </c>
     </row>
-    <row r="329" spans="1:4">
-      <c r="A329" t="s">
+    <row r="388" spans="1:1">
+      <c r="A388" t="s">
         <v>1225</v>
       </c>
     </row>
-    <row r="330" spans="1:4">
-      <c r="A330" t="s">
+    <row r="389" spans="1:1">
+      <c r="A389" t="s">
         <v>1226</v>
       </c>
     </row>
-    <row r="331" spans="1:4">
-      <c r="A331" t="s">
+    <row r="390" spans="1:1">
+      <c r="A390" t="s">
         <v>1227</v>
       </c>
     </row>
-    <row r="332" spans="1:4">
-      <c r="A332" t="s">
+    <row r="391" spans="1:1">
+      <c r="A391" t="s">
         <v>1228</v>
       </c>
     </row>
-    <row r="333" spans="1:4">
-      <c r="A333" t="s">
+    <row r="392" spans="1:1">
+      <c r="A392" t="s">
         <v>1229</v>
       </c>
     </row>
-    <row r="334" spans="1:4">
-      <c r="A334" t="s">
+    <row r="393" spans="1:1">
+      <c r="A393" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="341" spans="1:1">
-      <c r="A341" s="1" t="s">
+    <row r="400" spans="1:1">
+      <c r="A400" s="1" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="342" spans="1:1">
-      <c r="A342" s="1" t="s">
+    <row r="401" spans="1:1">
+      <c r="A401" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="343" spans="1:1">
-      <c r="A343" s="1" t="s">
+    <row r="402" spans="1:1">
+      <c r="A402" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="344" spans="1:1">
-      <c r="A344" s="1" t="s">
+    <row r="403" spans="1:1">
+      <c r="A403" s="1" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="345" spans="1:1">
-      <c r="A345" s="1" t="s">
+    <row r="404" spans="1:1">
+      <c r="A404" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="346" spans="1:1">
-      <c r="A346" s="1" t="s">
+    <row r="405" spans="1:1">
+      <c r="A405" s="1" t="s">
         <v>630</v>
       </c>
     </row>
@@ -27129,10 +27996,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -27491,10 +28358,10 @@
         <v>1908</v>
       </c>
       <c r="C43" t="s">
-        <v>2150</v>
+        <v>2450</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>2151</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -27502,10 +28369,10 @@
         <v>1909</v>
       </c>
       <c r="C44" t="s">
-        <v>2150</v>
+        <v>2450</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>2329</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -27532,35 +28399,35 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>2321</v>
+        <v>2316</v>
       </c>
       <c r="C47" t="s">
-        <v>2322</v>
+        <v>2317</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>2323</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>2324</v>
+        <v>2319</v>
       </c>
       <c r="C48" t="s">
-        <v>2325</v>
+        <v>2320</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>2326</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>2327</v>
+        <v>2322</v>
       </c>
       <c r="C49" t="s">
-        <v>2328</v>
+        <v>2323</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>2330</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -27579,10 +28446,10 @@
         <v>1956</v>
       </c>
       <c r="C51" t="s">
-        <v>2333</v>
+        <v>2448</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>2334</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -27590,10 +28457,10 @@
         <v>1957</v>
       </c>
       <c r="C52" t="s">
-        <v>2335</v>
+        <v>2449</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>2336</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -27612,10 +28479,10 @@
         <v>1991</v>
       </c>
       <c r="C54" t="s">
-        <v>2338</v>
+        <v>2446</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>2339</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -27623,10 +28490,10 @@
         <v>1992</v>
       </c>
       <c r="C55" t="s">
-        <v>2337</v>
+        <v>2447</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>2340</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -27656,10 +28523,10 @@
         <v>2027</v>
       </c>
       <c r="C58" t="s">
-        <v>2331</v>
+        <v>2445</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>2332</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -27667,10 +28534,10 @@
         <v>2028</v>
       </c>
       <c r="C59" t="s">
-        <v>2341</v>
+        <v>2444</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>2342</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -27689,10 +28556,10 @@
         <v>2058</v>
       </c>
       <c r="C61" t="s">
-        <v>2343</v>
+        <v>2332</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>2345</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -27700,10 +28567,10 @@
         <v>2059</v>
       </c>
       <c r="C62" t="s">
-        <v>2344</v>
+        <v>2333</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>2346</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -27733,10 +28600,10 @@
         <v>2092</v>
       </c>
       <c r="C65" t="s">
-        <v>2348</v>
+        <v>2337</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>2349</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -27744,10 +28611,10 @@
         <v>2093</v>
       </c>
       <c r="C66" t="s">
-        <v>2347</v>
+        <v>2336</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>2350</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -27755,109 +28622,109 @@
         <v>2121</v>
       </c>
       <c r="C67" t="s">
-        <v>2352</v>
+        <v>2341</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>2351</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>2387</v>
+        <v>2375</v>
       </c>
       <c r="C68" t="s">
-        <v>2399</v>
+        <v>2386</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>2419</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>2400</v>
+        <v>2387</v>
       </c>
       <c r="C69" t="s">
-        <v>2408</v>
+        <v>2395</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>2420</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>2401</v>
+        <v>2388</v>
       </c>
       <c r="C70" t="s">
-        <v>2409</v>
+        <v>2396</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>2421</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>2388</v>
+        <v>2438</v>
       </c>
       <c r="C71" t="s">
-        <v>2412</v>
+        <v>2442</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>2423</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>2402</v>
+        <v>2439</v>
       </c>
       <c r="C72" t="s">
-        <v>2410</v>
+        <v>2443</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>2424</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>2403</v>
+        <v>2440</v>
       </c>
       <c r="C73" t="s">
-        <v>2411</v>
+        <v>2451</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>2422</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>2389</v>
+        <v>2441</v>
       </c>
       <c r="C74" t="s">
-        <v>2415</v>
+        <v>2452</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>2425</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>2404</v>
+        <v>2376</v>
       </c>
       <c r="C75" t="s">
-        <v>2413</v>
+        <v>2399</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>2426</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>2405</v>
+        <v>2389</v>
       </c>
       <c r="C76" t="s">
-        <v>2414</v>
+        <v>2397</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>2427</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -27865,32 +28732,208 @@
         <v>2390</v>
       </c>
       <c r="C77" t="s">
-        <v>2416</v>
+        <v>2398</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>2428</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>2406</v>
+        <v>2453</v>
       </c>
       <c r="C78" t="s">
-        <v>2417</v>
+        <v>2457</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>2429</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>2407</v>
+        <v>2454</v>
       </c>
       <c r="C79" t="s">
-        <v>2418</v>
+        <v>2460</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>2430</v>
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>2456</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2458</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2402</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>2391</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>2392</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2401</v>
+      </c>
+      <c r="D84" s="22" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>2469</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D85" s="22" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>2378</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2403</v>
+      </c>
+      <c r="D89" s="22" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>2393</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D90" s="22" t="s">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>2394</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2405</v>
+      </c>
+      <c r="D91" s="22" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>2481</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>2483</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2487</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>2492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added incisor 3-6 traits
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ECAAC0-FC58-4F65-A0F4-670EC7E60510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294FBFAB-384C-4928-806E-F858AC9C142B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5041" uniqueCount="2535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5293" uniqueCount="2647">
   <si>
     <t>Status</t>
   </si>
@@ -7454,9 +7454,6 @@
     <t>Lower primary incisor 1 anterior-posterior diameter at base</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 1')</t>
-  </si>
-  <si>
     <t>line along anterior-posterior axis of upper secondary canine tooth</t>
   </si>
   <si>
@@ -7782,6 +7779,345 @@
   </si>
   <si>
     <t>anterior-posterior axis' and ('part of' some 'premolar tooth' 'part of' some ('anatomical row' and ('has member' some 'alveolar ridge')))</t>
+  </si>
+  <si>
+    <t>Incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 3 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 3 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>Upper incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>Lower incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 3 crown height</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 3')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 3')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'central incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 3')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower third secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper third secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper third primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower third primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>Incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 4 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 4 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>Upper incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>Lower incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 4 crown height</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 4')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 4')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 4')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper fourth secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper fourth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower fourth secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower fourth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>Incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 5 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 5 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>Upper incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>Lower incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 5 crown height</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 5')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 5')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 5')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper fifth secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper fifth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower fifth secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower fifth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>Incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 6 anterior-posterior diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 6 medial-lateral diameter at base</t>
+  </si>
+  <si>
+    <t>Incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>Upper incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>Lower incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>Upper primary incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>Lower secondary incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>Lower primary incisor 6 crown height</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 6')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 6')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 6')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper sixth secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'upper sixth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower sixth secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>('part of' some 'tooth crown') and ('part of' some 'lower sixth primary incisor tooth')</t>
   </si>
 </sst>
 </file>
@@ -22994,11 +23330,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D405"/>
+  <dimension ref="A1:D472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C365" sqref="C365"/>
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D422" sqref="D422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -26999,7 +27335,7 @@
         <v>2209</v>
       </c>
       <c r="D284" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -27013,7 +27349,7 @@
         <v>2210</v>
       </c>
       <c r="D285" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -27027,7 +27363,7 @@
         <v>2211</v>
       </c>
       <c r="D286" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -27041,7 +27377,7 @@
         <v>2212</v>
       </c>
       <c r="D287" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -27248,7 +27584,7 @@
         <v>112</v>
       </c>
       <c r="C302" s="37" t="s">
-        <v>2425</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -27259,7 +27595,7 @@
         <v>112</v>
       </c>
       <c r="C303" s="37" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="16.899999999999999" customHeight="1">
@@ -27270,7 +27606,7 @@
         <v>112</v>
       </c>
       <c r="C304" s="37" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="16.899999999999999" customHeight="1">
@@ -27281,7 +27617,7 @@
         <v>112</v>
       </c>
       <c r="C305" s="37" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="16.899999999999999" customHeight="1">
@@ -27292,7 +27628,7 @@
         <v>112</v>
       </c>
       <c r="C306" s="37" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="16.899999999999999" customHeight="1">
@@ -27303,7 +27639,7 @@
         <v>112</v>
       </c>
       <c r="C307" s="37" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="16.899999999999999" customHeight="1">
@@ -27314,669 +27650,1508 @@
         <v>112</v>
       </c>
       <c r="C308" s="37" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A309" s="16" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="B309" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C309" s="37" t="s">
-        <v>2425</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A310" s="16" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="B310" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C310" s="37" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A311" s="16" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="B311" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C311" s="37" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A312" s="16" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="B312" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C312" s="37" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A313" s="16" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B313" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C313" s="37" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A314" s="16" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="B314" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C314" s="37" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A315" s="16" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
       <c r="B315" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C315" s="37" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A316" s="16" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="B316" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C316" s="37" t="s">
-        <v>2425</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A317" s="16" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B317" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C317" s="37" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A318" s="16" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="B318" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C318" s="37" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A319" s="16" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="B319" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C319" s="37" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A320" s="16" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="B320" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C320" s="37" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A321" s="16" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="B321" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C321" s="37" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A322" s="16" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="B322" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C322" s="37" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A323" s="16" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="B323" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C323" s="37" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A324" s="16" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="B324" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C324" s="37" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A325" s="16" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="B325" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C325" s="37" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A326" s="16" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="B326" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C326" s="37" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A327" s="16" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="B327" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C327" s="37" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A328" s="16" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="B328" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C328" s="37" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A329" s="16" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B329" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C329" s="37" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A330" s="16" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="B330" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C330" s="37" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="331" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A331" s="16" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="B331" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C331" s="37" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A332" s="16" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="B332" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C332" s="37" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="333" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A333" s="16" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="B333" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C333" s="37" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A334" s="16" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="B334" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C334" s="37" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="335" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A335" s="16" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="B335" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C335" s="37" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="336" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A336" s="16" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="B336" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C336" s="37" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A337" s="16" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B337" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C337" s="37" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A338" s="16" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B338" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C338" s="37" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A339" s="16" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B339" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C339" s="37" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A340" s="16" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B340" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C340" s="37" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="341" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A341" s="16" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="B341" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C341" s="37" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A342" s="16" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="B342" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C342" s="37" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A343" s="16" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="B343" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C343" s="37" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A344" s="16"/>
-      <c r="B344" s="16"/>
-      <c r="C344" s="37"/>
+      <c r="A344" s="16" t="s">
+        <v>2534</v>
+      </c>
+      <c r="B344" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C344" s="37" t="s">
+        <v>2555</v>
+      </c>
     </row>
     <row r="345" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A345" s="16"/>
-      <c r="B345" s="16"/>
-      <c r="C345" s="37"/>
+      <c r="A345" s="16" t="s">
+        <v>2535</v>
+      </c>
+      <c r="B345" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C345" s="37" t="s">
+        <v>2558</v>
+      </c>
     </row>
     <row r="346" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A346" s="16"/>
-      <c r="B346" s="16"/>
-      <c r="C346" s="37"/>
+      <c r="A346" s="16" t="s">
+        <v>2536</v>
+      </c>
+      <c r="B346" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C346" s="37" t="s">
+        <v>2556</v>
+      </c>
     </row>
     <row r="347" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A347" s="16"/>
-      <c r="B347" s="16"/>
-      <c r="C347" s="37"/>
+      <c r="A347" s="16" t="s">
+        <v>2537</v>
+      </c>
+      <c r="B347" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C347" s="37" t="s">
+        <v>2560</v>
+      </c>
     </row>
     <row r="348" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A348" s="16"/>
-      <c r="B348" s="16"/>
-      <c r="C348" s="37"/>
+      <c r="A348" s="16" t="s">
+        <v>2538</v>
+      </c>
+      <c r="B348" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C348" s="37" t="s">
+        <v>2561</v>
+      </c>
     </row>
     <row r="349" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A349" s="16"/>
-      <c r="B349" s="16"/>
-      <c r="C349" s="37"/>
+      <c r="A349" s="16" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B349" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C349" s="37" t="s">
+        <v>2559</v>
+      </c>
     </row>
     <row r="350" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A350" s="16"/>
-      <c r="B350" s="16"/>
-      <c r="C350" s="37"/>
+      <c r="A350" s="16" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B350" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C350" s="37" t="s">
+        <v>2562</v>
+      </c>
     </row>
     <row r="351" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A351" s="16"/>
-      <c r="B351" s="16"/>
-      <c r="C351" s="37"/>
+      <c r="A351" s="16" t="s">
+        <v>2541</v>
+      </c>
+      <c r="B351" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C351" s="37" t="s">
+        <v>2555</v>
+      </c>
     </row>
     <row r="352" spans="1:3" ht="16.899999999999999" customHeight="1">
-      <c r="A352" s="16"/>
-      <c r="B352" s="16"/>
-      <c r="C352" s="37"/>
-    </row>
-    <row r="353" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A353" s="16"/>
-      <c r="B353" s="16"/>
-      <c r="C353" s="37"/>
-    </row>
-    <row r="354" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A354" s="16"/>
-      <c r="B354" s="16"/>
-      <c r="C354" s="37"/>
-    </row>
-    <row r="355" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A355" s="16"/>
-      <c r="B355" s="16"/>
-      <c r="C355" s="37"/>
-    </row>
-    <row r="356" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A356" s="16"/>
-      <c r="B356" s="16"/>
-      <c r="C356" s="37"/>
-    </row>
-    <row r="357" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A357" s="16"/>
-      <c r="B357" s="16"/>
-      <c r="C357" s="37"/>
-    </row>
-    <row r="358" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A358" s="16"/>
-      <c r="B358" s="16"/>
-      <c r="C358" s="37"/>
-    </row>
-    <row r="359" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A359" s="16"/>
-      <c r="B359" s="16"/>
-      <c r="C359" s="37"/>
-    </row>
-    <row r="360" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A360" s="16"/>
-      <c r="B360" s="16"/>
-      <c r="C360" s="37"/>
-    </row>
-    <row r="361" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A361" s="16"/>
-      <c r="B361" s="16"/>
-      <c r="C361" s="37"/>
-    </row>
-    <row r="362" spans="1:4">
-      <c r="A362" s="16"/>
-      <c r="B362" s="16"/>
-      <c r="C362" s="37"/>
-    </row>
-    <row r="363" spans="1:4">
-      <c r="A363" s="16"/>
-      <c r="B363" s="16"/>
-      <c r="C363" s="37"/>
-    </row>
-    <row r="364" spans="1:4">
+      <c r="A352" s="16" t="s">
+        <v>2542</v>
+      </c>
+      <c r="B352" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C352" s="37" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A353" s="16" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B353" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C353" s="37" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A354" s="16" t="s">
+        <v>2544</v>
+      </c>
+      <c r="B354" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C354" s="37" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A355" s="16" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B355" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C355" s="37" t="s">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A356" s="16" t="s">
+        <v>2546</v>
+      </c>
+      <c r="B356" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C356" s="37" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A357" s="16" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B357" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C357" s="37" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A358" s="16" t="s">
+        <v>2548</v>
+      </c>
+      <c r="B358" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C358" s="37" t="s">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A359" s="16" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B359" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C359" s="37" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A360" s="16" t="s">
+        <v>2550</v>
+      </c>
+      <c r="B360" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C360" s="37" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A361" s="16" t="s">
+        <v>2551</v>
+      </c>
+      <c r="B361" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C361" s="37" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A362" s="16" t="s">
+        <v>2552</v>
+      </c>
+      <c r="B362" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C362" s="37" t="s">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A363" s="16" t="s">
+        <v>2553</v>
+      </c>
+      <c r="B363" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C363" s="37" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A364" s="16" t="s">
-        <v>2417</v>
+        <v>2554</v>
       </c>
       <c r="B364" s="16" t="s">
-        <v>112</v>
+        <v>2140</v>
       </c>
       <c r="C364" s="37" t="s">
-        <v>2533</v>
-      </c>
-      <c r="D364" t="s">
-        <v>2380</v>
-      </c>
-    </row>
-    <row r="365" spans="1:4">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A365" s="16" t="s">
-        <v>2381</v>
+        <v>2563</v>
       </c>
       <c r="B365" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C365" s="37" t="s">
-        <v>2534</v>
-      </c>
-    </row>
-    <row r="366" spans="1:4">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A366" s="16" t="s">
-        <v>2418</v>
+        <v>2564</v>
       </c>
       <c r="B366" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C366" s="37"/>
-    </row>
-    <row r="367" spans="1:4">
+      <c r="C366" s="37" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A367" s="16" t="s">
-        <v>2382</v>
+        <v>2565</v>
       </c>
       <c r="B367" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C367" s="37"/>
-    </row>
-    <row r="368" spans="1:4">
-      <c r="A368" s="16"/>
-      <c r="B368" s="16"/>
-      <c r="C368" s="37"/>
-    </row>
-    <row r="369" spans="1:4">
-      <c r="A369" s="16"/>
-      <c r="B369" s="16"/>
-      <c r="C369" s="37"/>
-    </row>
-    <row r="370" spans="1:4">
-      <c r="A370" s="16"/>
-      <c r="B370" s="16"/>
-      <c r="C370" s="37"/>
-    </row>
-    <row r="371" spans="1:4">
-      <c r="A371" s="16"/>
-      <c r="B371" s="16"/>
-      <c r="C371" s="37"/>
-    </row>
-    <row r="381" spans="1:4">
-      <c r="A381" t="s">
+      <c r="C367" s="37" t="s">
+        <v>2586</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A368" s="16" t="s">
+        <v>2566</v>
+      </c>
+      <c r="B368" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C368" s="37" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A369" s="16" t="s">
+        <v>2567</v>
+      </c>
+      <c r="B369" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C369" s="37" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A370" s="16" t="s">
+        <v>2568</v>
+      </c>
+      <c r="B370" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C370" s="37" t="s">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A371" s="16" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B371" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C371" s="37" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A372" s="16" t="s">
+        <v>2570</v>
+      </c>
+      <c r="B372" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C372" s="37" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A373" s="16" t="s">
+        <v>2571</v>
+      </c>
+      <c r="B373" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C373" s="37" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A374" s="16" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B374" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C374" s="37" t="s">
+        <v>2586</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A375" s="16" t="s">
+        <v>2573</v>
+      </c>
+      <c r="B375" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C375" s="37" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A376" s="16" t="s">
+        <v>2574</v>
+      </c>
+      <c r="B376" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C376" s="37" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A377" s="16" t="s">
+        <v>2575</v>
+      </c>
+      <c r="B377" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C377" s="37" t="s">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A378" s="16" t="s">
+        <v>2576</v>
+      </c>
+      <c r="B378" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C378" s="37" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A379" s="16" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B379" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C379" s="37" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A380" s="16" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B380" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C380" s="37" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A381" s="16" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B381" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C381" s="37" t="s">
+        <v>2586</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A382" s="16" t="s">
+        <v>2580</v>
+      </c>
+      <c r="B382" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C382" s="37" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A383" s="16" t="s">
+        <v>2581</v>
+      </c>
+      <c r="B383" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C383" s="37" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A384" s="16" t="s">
+        <v>2582</v>
+      </c>
+      <c r="B384" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C384" s="37" t="s">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A385" s="16" t="s">
+        <v>2583</v>
+      </c>
+      <c r="B385" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C385" s="37" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A386" s="16" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B386" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C386" s="37" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A387" s="16" t="s">
+        <v>2592</v>
+      </c>
+      <c r="B387" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C387" s="37" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A388" s="16" t="s">
+        <v>2593</v>
+      </c>
+      <c r="B388" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C388" s="37" t="s">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A389" s="16" t="s">
+        <v>2594</v>
+      </c>
+      <c r="B389" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C389" s="37" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A390" s="16" t="s">
+        <v>2595</v>
+      </c>
+      <c r="B390" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C390" s="37" t="s">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A391" s="16" t="s">
+        <v>2596</v>
+      </c>
+      <c r="B391" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C391" s="37" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A392" s="16" t="s">
+        <v>2597</v>
+      </c>
+      <c r="B392" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C392" s="37" t="s">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A393" s="16" t="s">
+        <v>2598</v>
+      </c>
+      <c r="B393" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C393" s="37" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A394" s="16" t="s">
+        <v>2599</v>
+      </c>
+      <c r="B394" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C394" s="37" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A395" s="16" t="s">
+        <v>2600</v>
+      </c>
+      <c r="B395" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C395" s="37" t="s">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A396" s="16" t="s">
+        <v>2601</v>
+      </c>
+      <c r="B396" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C396" s="37" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A397" s="16" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B397" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C397" s="37" t="s">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A398" s="16" t="s">
+        <v>2603</v>
+      </c>
+      <c r="B398" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C398" s="37" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A399" s="16" t="s">
+        <v>2604</v>
+      </c>
+      <c r="B399" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C399" s="37" t="s">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A400" s="16" t="s">
+        <v>2605</v>
+      </c>
+      <c r="B400" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C400" s="37" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A401" s="16" t="s">
+        <v>2606</v>
+      </c>
+      <c r="B401" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C401" s="37" t="s">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A402" s="16" t="s">
+        <v>2607</v>
+      </c>
+      <c r="B402" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C402" s="37" t="s">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A403" s="16" t="s">
+        <v>2608</v>
+      </c>
+      <c r="B403" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C403" s="37" t="s">
+        <v>2615</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A404" s="16" t="s">
+        <v>2609</v>
+      </c>
+      <c r="B404" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C404" s="37" t="s">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A405" s="16" t="s">
+        <v>2610</v>
+      </c>
+      <c r="B405" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C405" s="37" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A406" s="16" t="s">
+        <v>2611</v>
+      </c>
+      <c r="B406" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C406" s="37" t="s">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A407" s="16" t="s">
+        <v>2619</v>
+      </c>
+      <c r="B407" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C407" s="37" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A408" s="16" t="s">
+        <v>2620</v>
+      </c>
+      <c r="B408" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C408" s="37" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A409" s="16" t="s">
+        <v>2621</v>
+      </c>
+      <c r="B409" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C409" s="37" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A410" s="16" t="s">
+        <v>2622</v>
+      </c>
+      <c r="B410" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C410" s="37" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A411" s="16" t="s">
+        <v>2623</v>
+      </c>
+      <c r="B411" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C411" s="37" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A412" s="16" t="s">
+        <v>2624</v>
+      </c>
+      <c r="B412" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C412" s="37" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A413" s="16" t="s">
+        <v>2625</v>
+      </c>
+      <c r="B413" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C413" s="37" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A414" s="16" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B414" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C414" s="37" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A415" s="16" t="s">
+        <v>2627</v>
+      </c>
+      <c r="B415" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C415" s="37" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="A416" s="16" t="s">
+        <v>2628</v>
+      </c>
+      <c r="B416" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C416" s="37" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A417" s="16" t="s">
+        <v>2629</v>
+      </c>
+      <c r="B417" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C417" s="37" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A418" s="16" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B418" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C418" s="37" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A419" s="16" t="s">
+        <v>2631</v>
+      </c>
+      <c r="B419" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C419" s="37" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A420" s="16" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B420" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C420" s="37" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A421" s="16" t="s">
+        <v>2633</v>
+      </c>
+      <c r="B421" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C421" s="37" t="s">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A422" s="16" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B422" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C422" s="37" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A423" s="16" t="s">
+        <v>2635</v>
+      </c>
+      <c r="B423" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C423" s="37" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A424" s="16" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B424" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C424" s="37" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A425" s="16" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B425" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C425" s="37" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A426" s="16" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B426" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C426" s="37" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A427" s="16" t="s">
+        <v>2639</v>
+      </c>
+      <c r="B427" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C427" s="37" t="s">
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A428" s="16"/>
+      <c r="B428" s="16"/>
+      <c r="C428" s="37"/>
+    </row>
+    <row r="429" spans="1:4">
+      <c r="A429" s="16"/>
+      <c r="B429" s="16"/>
+      <c r="C429" s="37"/>
+    </row>
+    <row r="430" spans="1:4">
+      <c r="A430" s="16"/>
+      <c r="B430" s="16"/>
+      <c r="C430" s="37"/>
+    </row>
+    <row r="431" spans="1:4">
+      <c r="A431" s="16" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B431" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C431" s="37" t="s">
+        <v>2532</v>
+      </c>
+      <c r="D431" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4">
+      <c r="A432" s="16" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B432" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C432" s="37" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4">
+      <c r="A433" s="16" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B433" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C433" s="37"/>
+    </row>
+    <row r="434" spans="1:4">
+      <c r="A434" s="16" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B434" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C434" s="37"/>
+    </row>
+    <row r="435" spans="1:4">
+      <c r="A435" s="16"/>
+      <c r="B435" s="16"/>
+      <c r="C435" s="37"/>
+    </row>
+    <row r="436" spans="1:4">
+      <c r="A436" s="16"/>
+      <c r="B436" s="16"/>
+      <c r="C436" s="37"/>
+    </row>
+    <row r="437" spans="1:4">
+      <c r="A437" s="16"/>
+      <c r="B437" s="16"/>
+      <c r="C437" s="37"/>
+    </row>
+    <row r="438" spans="1:4">
+      <c r="A438" s="16"/>
+      <c r="B438" s="16"/>
+      <c r="C438" s="37"/>
+    </row>
+    <row r="448" spans="1:4">
+      <c r="A448" t="s">
         <v>1230</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B448" t="s">
         <v>1217</v>
       </c>
-      <c r="C381" s="22" t="s">
+      <c r="C448" s="22" t="s">
         <v>1218</v>
       </c>
-      <c r="D381" t="str">
-        <f>"line along "&amp;B381&amp;" of "&amp;C381</f>
+      <c r="D448" t="str">
+        <f>"line along "&amp;B448&amp;" of "&amp;C448</f>
         <v>line along proximal-distal of lateral side' some talus</v>
       </c>
     </row>
-    <row r="382" spans="1:4">
-      <c r="A382" t="s">
+    <row r="449" spans="1:4">
+      <c r="A449" t="s">
         <v>1216</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B449" t="s">
         <v>1217</v>
       </c>
-      <c r="C382" t="s">
+      <c r="C449" t="s">
         <v>1219</v>
       </c>
-      <c r="D382" t="str">
-        <f>"line along "&amp;B382&amp;" of "&amp;C382</f>
+      <c r="D449" t="str">
+        <f>"line along "&amp;B449&amp;" of "&amp;C449</f>
         <v>line along proximal-distal of pes</v>
       </c>
     </row>
-    <row r="383" spans="1:4">
-      <c r="A383" t="s">
+    <row r="450" spans="1:4">
+      <c r="A450" t="s">
         <v>1220</v>
       </c>
     </row>
-    <row r="384" spans="1:4">
-      <c r="A384" t="s">
+    <row r="451" spans="1:4">
+      <c r="A451" t="s">
         <v>1221</v>
       </c>
     </row>
-    <row r="385" spans="1:1">
-      <c r="A385" t="s">
+    <row r="452" spans="1:4">
+      <c r="A452" t="s">
         <v>1222</v>
       </c>
     </row>
-    <row r="386" spans="1:1">
-      <c r="A386" t="s">
+    <row r="453" spans="1:4">
+      <c r="A453" t="s">
         <v>1223</v>
       </c>
     </row>
-    <row r="387" spans="1:1">
-      <c r="A387" t="s">
+    <row r="454" spans="1:4">
+      <c r="A454" t="s">
         <v>1224</v>
       </c>
     </row>
-    <row r="388" spans="1:1">
-      <c r="A388" t="s">
+    <row r="455" spans="1:4">
+      <c r="A455" t="s">
         <v>1225</v>
       </c>
     </row>
-    <row r="389" spans="1:1">
-      <c r="A389" t="s">
+    <row r="456" spans="1:4">
+      <c r="A456" t="s">
         <v>1226</v>
       </c>
     </row>
-    <row r="390" spans="1:1">
-      <c r="A390" t="s">
+    <row r="457" spans="1:4">
+      <c r="A457" t="s">
         <v>1227</v>
       </c>
     </row>
-    <row r="391" spans="1:1">
-      <c r="A391" t="s">
+    <row r="458" spans="1:4">
+      <c r="A458" t="s">
         <v>1228</v>
       </c>
     </row>
-    <row r="392" spans="1:1">
-      <c r="A392" t="s">
+    <row r="459" spans="1:4">
+      <c r="A459" t="s">
         <v>1229</v>
       </c>
     </row>
-    <row r="393" spans="1:1">
-      <c r="A393" t="s">
+    <row r="460" spans="1:4">
+      <c r="A460" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="400" spans="1:1">
-      <c r="A400" s="1" t="s">
+    <row r="467" spans="1:1">
+      <c r="A467" s="1" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="401" spans="1:1">
-      <c r="A401" s="1" t="s">
+    <row r="468" spans="1:1">
+      <c r="A468" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="402" spans="1:1">
-      <c r="A402" s="1" t="s">
+    <row r="469" spans="1:1">
+      <c r="A469" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
-    <row r="403" spans="1:1">
-      <c r="A403" s="1" t="s">
+    <row r="470" spans="1:1">
+      <c r="A470" s="1" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="404" spans="1:1">
-      <c r="A404" s="1" t="s">
+    <row r="471" spans="1:1">
+      <c r="A471" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="405" spans="1:1">
-      <c r="A405" s="1" t="s">
+    <row r="472" spans="1:1">
+      <c r="A472" s="1" t="s">
         <v>630</v>
       </c>
     </row>
@@ -27992,8 +29167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -28352,7 +29527,7 @@
         <v>1908</v>
       </c>
       <c r="C43" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>2146</v>
@@ -28363,7 +29538,7 @@
         <v>1909</v>
       </c>
       <c r="C44" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>2324</v>
@@ -28440,7 +29615,7 @@
         <v>1956</v>
       </c>
       <c r="C51" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>2327</v>
@@ -28451,7 +29626,7 @@
         <v>1957</v>
       </c>
       <c r="C52" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>2328</v>
@@ -28473,7 +29648,7 @@
         <v>1991</v>
       </c>
       <c r="C54" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>2329</v>
@@ -28484,7 +29659,7 @@
         <v>1992</v>
       </c>
       <c r="C55" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>2330</v>
@@ -28517,7 +29692,7 @@
         <v>2027</v>
       </c>
       <c r="C58" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="D58" s="22" t="s">
         <v>2326</v>
@@ -28528,7 +29703,7 @@
         <v>2028</v>
       </c>
       <c r="C59" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>2331</v>
@@ -28657,46 +29832,46 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="C71" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="C72" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="C73" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="C74" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -28734,46 +29909,46 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="C78" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="C79" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="C80" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="C81" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -28811,46 +29986,46 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C85" t="s">
         <v>2468</v>
       </c>
-      <c r="C85" t="s">
-        <v>2469</v>
-      </c>
       <c r="D85" s="22" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="C86" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="C87" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="C88" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -28888,46 +30063,46 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="C92" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="C93" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="C94" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="C95" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added premolar and molar row length axis patterns
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294FBFAB-384C-4928-806E-F858AC9C142B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A963617F-4028-4BA3-91C6-E9EA8500D7AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5293" uniqueCount="2647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5342" uniqueCount="2678">
   <si>
     <t>Status</t>
   </si>
@@ -7775,12 +7775,6 @@
     <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral primary incisor tooth')</t>
   </si>
   <si>
-    <t>anterior-posterior axis' and ('part of' some ('premolar tooth' 'part of' some 'tooth row'))</t>
-  </si>
-  <si>
-    <t>anterior-posterior axis' and ('part of' some 'premolar tooth' 'part of' some ('anatomical row' and ('has member' some 'alveolar ridge')))</t>
-  </si>
-  <si>
     <t>Incisor 3 anterior-posterior diameter at base</t>
   </si>
   <si>
@@ -8118,6 +8112,105 @@
   </si>
   <si>
     <t>('part of' some 'tooth crown') and ('part of' some 'lower sixth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>('part of' some ('premolar tooth' 'part of' some 'tooth row'))</t>
+  </si>
+  <si>
+    <t>('part of' some 'premolar tooth' 'part of' some ('anatomical row' and ('has member' some 'alveolar ridge')))</t>
+  </si>
+  <si>
+    <t>('part of' some ('molar tooth' 'part of' some 'tooth row'))</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of premolar tooth row at alveoli</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of molar tooth row</t>
+  </si>
+  <si>
+    <t>('part of' some 'molar tooth' 'part of' some ('anatomical row' and ('has member' some 'alveolar ridge')))</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of molar tooth row at alveoli</t>
+  </si>
+  <si>
+    <t>Length of upper premolar tooth row</t>
+  </si>
+  <si>
+    <t>Length of upper molar tooth row</t>
+  </si>
+  <si>
+    <t>Length of upper molar row at alveoli</t>
+  </si>
+  <si>
+    <t>Length of upper premolar row at alveoli</t>
+  </si>
+  <si>
+    <t>Length of lower premolar tooth row</t>
+  </si>
+  <si>
+    <t>Length of lower premolar row at alveoli</t>
+  </si>
+  <si>
+    <t>Length of lower molar row at alveoli</t>
+  </si>
+  <si>
+    <t>('part of' some ('premolar tooth' 'part of' some 'maxillary tooth row'))</t>
+  </si>
+  <si>
+    <t>('part of' some ('molar tooth' 'part of' some 'maxillary tooth row'))</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar tooth row</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper premolar tooth row at alveoli</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar tooth row at alveoli</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper molar tooth row</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper molar tooth row at alveoli</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower molar tooth row at alveoli</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower premolar tooth row</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower molar tooth row</t>
+  </si>
+  <si>
+    <t>Length of lower molar tooth row</t>
+  </si>
+  <si>
+    <t>Premolar 5 length</t>
+  </si>
+  <si>
+    <t>Upper premolar 5 length</t>
+  </si>
+  <si>
+    <t>Lower premolar 5 length</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 5 length</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 5 length</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 5 length</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 5 length</t>
+  </si>
+  <si>
+    <t>Length of whole tooth row</t>
   </si>
 </sst>
 </file>
@@ -8895,9 +8988,9 @@
   <dimension ref="A1:AD500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I244" sqref="I244"/>
+      <selection pane="bottomLeft" activeCell="H262" sqref="H262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16400,6 +16493,9 @@
     </row>
     <row r="232" spans="1:21">
       <c r="A232" s="39"/>
+      <c r="C232" t="s">
+        <v>2113</v>
+      </c>
       <c r="E232" s="1" t="s">
         <v>343</v>
       </c>
@@ -16425,6 +16521,9 @@
     </row>
     <row r="233" spans="1:21">
       <c r="A233" s="39"/>
+      <c r="C233" t="s">
+        <v>2113</v>
+      </c>
       <c r="E233" s="1" t="s">
         <v>343</v>
       </c>
@@ -16450,12 +16549,18 @@
     </row>
     <row r="234" spans="1:21">
       <c r="A234" s="39"/>
+      <c r="C234" t="s">
+        <v>2113</v>
+      </c>
       <c r="H234" s="34" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="235" spans="1:21">
       <c r="A235" s="39"/>
+      <c r="C235" t="s">
+        <v>2113</v>
+      </c>
       <c r="E235" s="1" t="s">
         <v>343</v>
       </c>
@@ -16481,6 +16586,9 @@
     </row>
     <row r="236" spans="1:21">
       <c r="A236" s="39"/>
+      <c r="C236" t="s">
+        <v>2113</v>
+      </c>
       <c r="E236" s="1" t="s">
         <v>343</v>
       </c>
@@ -16710,6 +16818,9 @@
     </row>
     <row r="244" spans="1:21">
       <c r="A244" s="39"/>
+      <c r="C244" s="16" t="s">
+        <v>2113</v>
+      </c>
       <c r="H244" s="19" t="s">
         <v>1030</v>
       </c>
@@ -16723,7 +16834,9 @@
     <row r="245" spans="1:21">
       <c r="A245" s="39"/>
       <c r="B245" s="21"/>
-      <c r="C245" s="21"/>
+      <c r="C245" s="16" t="s">
+        <v>2113</v>
+      </c>
       <c r="H245" s="19" t="s">
         <v>1033</v>
       </c>
@@ -16737,7 +16850,9 @@
     <row r="246" spans="1:21">
       <c r="A246" s="39"/>
       <c r="B246" s="21"/>
-      <c r="C246" s="21"/>
+      <c r="C246" s="16" t="s">
+        <v>2113</v>
+      </c>
       <c r="H246" s="19" t="s">
         <v>1036</v>
       </c>
@@ -16751,7 +16866,9 @@
     <row r="247" spans="1:21">
       <c r="A247" s="39"/>
       <c r="B247" s="21"/>
-      <c r="C247" s="21"/>
+      <c r="C247" s="16" t="s">
+        <v>2113</v>
+      </c>
       <c r="H247" s="19" t="s">
         <v>1037</v>
       </c>
@@ -17244,7 +17361,9 @@
     <row r="268" spans="1:21">
       <c r="A268" s="39"/>
       <c r="B268" s="21"/>
-      <c r="C268" s="21"/>
+      <c r="C268" t="s">
+        <v>2113</v>
+      </c>
       <c r="H268" s="19" t="s">
         <v>1038</v>
       </c>
@@ -17257,6 +17376,9 @@
     </row>
     <row r="269" spans="1:21">
       <c r="A269" s="39"/>
+      <c r="C269" t="s">
+        <v>2113</v>
+      </c>
       <c r="H269" s="19" t="s">
         <v>1039</v>
       </c>
@@ -23330,11 +23452,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D472"/>
+  <dimension ref="A1:D469"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D422" sqref="D422"/>
+      <pane ySplit="1" topLeftCell="A425" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A437" sqref="A437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -27186,7 +27308,7 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>2083</v>
+        <v>2670</v>
       </c>
       <c r="B274" t="s">
         <v>112</v>
@@ -27200,7 +27322,7 @@
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>2084</v>
+        <v>2671</v>
       </c>
       <c r="B275" t="s">
         <v>112</v>
@@ -27214,7 +27336,7 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>2085</v>
+        <v>2672</v>
       </c>
       <c r="B276" t="s">
         <v>112</v>
@@ -27228,7 +27350,7 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>2086</v>
+        <v>2673</v>
       </c>
       <c r="B277" t="s">
         <v>112</v>
@@ -27242,7 +27364,7 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>2087</v>
+        <v>2674</v>
       </c>
       <c r="B278" t="s">
         <v>112</v>
@@ -27256,7 +27378,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>2088</v>
+        <v>2675</v>
       </c>
       <c r="B279" t="s">
         <v>112</v>
@@ -27270,7 +27392,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>2089</v>
+        <v>2676</v>
       </c>
       <c r="B280" t="s">
         <v>112</v>
@@ -27584,7 +27706,7 @@
         <v>112</v>
       </c>
       <c r="C302" s="37" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -27661,7 +27783,7 @@
         <v>108</v>
       </c>
       <c r="C309" s="37" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="16.899999999999999" customHeight="1">
@@ -27738,7 +27860,7 @@
         <v>2140</v>
       </c>
       <c r="C316" s="37" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="16.899999999999999" customHeight="1">
@@ -28040,1118 +28162,1213 @@
     </row>
     <row r="344" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A344" s="16" t="s">
-        <v>2534</v>
+        <v>2532</v>
       </c>
       <c r="B344" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C344" s="37" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="345" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A345" s="16" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
       <c r="B345" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C345" s="37" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A346" s="16" t="s">
-        <v>2536</v>
+        <v>2534</v>
       </c>
       <c r="B346" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C346" s="37" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="347" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A347" s="16" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="B347" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C347" s="37" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="348" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A348" s="16" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="B348" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C348" s="37" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A349" s="16" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="B349" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C349" s="37" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A350" s="16" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="B350" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C350" s="37" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="351" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A351" s="16" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="B351" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C351" s="37" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="352" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A352" s="16" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
       <c r="B352" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C352" s="37" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="353" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A353" s="16" t="s">
-        <v>2543</v>
+        <v>2541</v>
       </c>
       <c r="B353" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C353" s="37" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A354" s="16" t="s">
-        <v>2544</v>
+        <v>2542</v>
       </c>
       <c r="B354" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C354" s="37" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="355" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A355" s="16" t="s">
-        <v>2545</v>
+        <v>2543</v>
       </c>
       <c r="B355" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C355" s="37" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="356" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A356" s="16" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
       <c r="B356" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C356" s="37" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A357" s="16" t="s">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="B357" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C357" s="37" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A358" s="16" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="B358" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C358" s="37" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A359" s="16" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="B359" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C359" s="37" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A360" s="16" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="B360" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C360" s="37" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A361" s="16" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="B361" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C361" s="37" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A362" s="16" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="B362" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C362" s="37" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="363" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A363" s="16" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="B363" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C363" s="37" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="364" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A364" s="16" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
       <c r="B364" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C364" s="37" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="365" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A365" s="16" t="s">
-        <v>2563</v>
+        <v>2561</v>
       </c>
       <c r="B365" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C365" s="37" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="366" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A366" s="16" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="B366" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C366" s="37" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="367" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A367" s="16" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="B367" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C367" s="37" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A368" s="16" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="B368" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C368" s="37" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="369" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A369" s="16" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="B369" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C369" s="37" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="370" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A370" s="16" t="s">
-        <v>2568</v>
+        <v>2566</v>
       </c>
       <c r="B370" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C370" s="37" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="371" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A371" s="16" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
       <c r="B371" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C371" s="37" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A372" s="16" t="s">
-        <v>2570</v>
+        <v>2568</v>
       </c>
       <c r="B372" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C372" s="37" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A373" s="16" t="s">
-        <v>2571</v>
+        <v>2569</v>
       </c>
       <c r="B373" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C373" s="37" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A374" s="16" t="s">
-        <v>2572</v>
+        <v>2570</v>
       </c>
       <c r="B374" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C374" s="37" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="375" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A375" s="16" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="B375" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C375" s="37" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="376" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A376" s="16" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="B376" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C376" s="37" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="377" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A377" s="16" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="B377" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C377" s="37" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="378" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A378" s="16" t="s">
-        <v>2576</v>
+        <v>2574</v>
       </c>
       <c r="B378" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C378" s="37" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="379" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A379" s="16" t="s">
-        <v>2577</v>
+        <v>2575</v>
       </c>
       <c r="B379" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C379" s="37" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="380" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A380" s="16" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="B380" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C380" s="37" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="381" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A381" s="16" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
       <c r="B381" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C381" s="37" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="382" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A382" s="16" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="B382" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C382" s="37" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="383" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A383" s="16" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
       <c r="B383" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C383" s="37" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="384" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A384" s="16" t="s">
-        <v>2582</v>
+        <v>2580</v>
       </c>
       <c r="B384" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C384" s="37" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A385" s="16" t="s">
-        <v>2583</v>
+        <v>2581</v>
       </c>
       <c r="B385" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C385" s="37" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="386" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A386" s="16" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
       <c r="B386" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C386" s="37" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="387" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A387" s="16" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
       <c r="B387" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C387" s="37" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="388" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A388" s="16" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
       <c r="B388" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C388" s="37" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="389" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A389" s="16" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
       <c r="B389" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C389" s="37" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="390" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A390" s="16" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
       <c r="B390" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C390" s="37" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="391" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A391" s="16" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="B391" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C391" s="37" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="392" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A392" s="16" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="B392" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C392" s="37" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="393" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A393" s="16" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="B393" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C393" s="37" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="394" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A394" s="16" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="B394" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C394" s="37" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="395" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A395" s="16" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="B395" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C395" s="37" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="396" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A396" s="16" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="B396" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C396" s="37" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="397" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A397" s="16" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="B397" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C397" s="37" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="398" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A398" s="16" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="B398" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C398" s="37" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="399" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A399" s="16" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="B399" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C399" s="37" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="400" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A400" s="16" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="B400" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C400" s="37" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="401" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A401" s="16" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
       <c r="B401" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C401" s="37" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="402" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A402" s="16" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
       <c r="B402" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C402" s="37" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A403" s="16" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
       <c r="B403" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C403" s="37" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A404" s="16" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="B404" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C404" s="37" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A405" s="16" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="B405" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C405" s="37" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="406" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A406" s="16" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="B406" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C406" s="37" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A407" s="16" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
       <c r="B407" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C407" s="37" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A408" s="16" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="B408" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C408" s="37" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A409" s="16" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="B409" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C409" s="37" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="410" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A410" s="16" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="B410" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C410" s="37" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A411" s="16" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="B411" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C411" s="37" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A412" s="16" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="B412" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C412" s="37" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A413" s="16" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="B413" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C413" s="37" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A414" s="16" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
       <c r="B414" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C414" s="37" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A415" s="16" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="B415" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C415" s="37" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A416" s="16" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="B416" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C416" s="37" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A417" s="16" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="B417" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C417" s="37" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A418" s="16" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
       <c r="B418" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C418" s="37" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="419" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A419" s="16" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="B419" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C419" s="37" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="420" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A420" s="16" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="B420" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C420" s="37" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="421" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A421" s="16" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="B421" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C421" s="37" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="422" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A422" s="16" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
       <c r="B422" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C422" s="37" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="423" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A423" s="16" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="B423" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C423" s="37" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A424" s="16" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="B424" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C424" s="37" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="425" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A425" s="16" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="B425" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C425" s="37" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="426" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A426" s="16" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
       <c r="B426" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C426" s="37" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="427" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A427" s="16" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="B427" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C427" s="37" t="s">
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4">
+      <c r="A428" s="16" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B428" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C428" s="37" t="s">
+        <v>2645</v>
+      </c>
+      <c r="D428" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4">
+      <c r="A429" s="16" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B429" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C429" s="37" t="s">
         <v>2646</v>
       </c>
-    </row>
-    <row r="428" spans="1:4" ht="16.899999999999999" customHeight="1">
-      <c r="A428" s="16"/>
-      <c r="B428" s="16"/>
-      <c r="C428" s="37"/>
-    </row>
-    <row r="429" spans="1:4">
-      <c r="A429" s="16"/>
-      <c r="B429" s="16"/>
-      <c r="C429" s="37"/>
+      <c r="D429" t="s">
+        <v>2648</v>
+      </c>
     </row>
     <row r="430" spans="1:4">
-      <c r="A430" s="16"/>
-      <c r="B430" s="16"/>
-      <c r="C430" s="37"/>
+      <c r="A430" s="16" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B430" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C430" s="37" t="s">
+        <v>2647</v>
+      </c>
+      <c r="D430" t="s">
+        <v>2649</v>
+      </c>
     </row>
     <row r="431" spans="1:4">
       <c r="A431" s="16" t="s">
-        <v>2417</v>
+        <v>2382</v>
       </c>
       <c r="B431" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C431" s="37" t="s">
-        <v>2532</v>
+        <v>2650</v>
       </c>
       <c r="D431" t="s">
-        <v>2380</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="432" spans="1:4">
       <c r="A432" s="16" t="s">
-        <v>2381</v>
+        <v>2652</v>
       </c>
       <c r="B432" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C432" s="37" t="s">
-        <v>2533</v>
+        <v>2659</v>
+      </c>
+      <c r="D432" t="s">
+        <v>2661</v>
       </c>
     </row>
     <row r="433" spans="1:4">
       <c r="A433" s="16" t="s">
-        <v>2418</v>
+        <v>2655</v>
       </c>
       <c r="B433" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C433" s="37"/>
+      <c r="C433" s="32" t="s">
+        <v>2646</v>
+      </c>
+      <c r="D433" t="s">
+        <v>2662</v>
+      </c>
     </row>
     <row r="434" spans="1:4">
       <c r="A434" s="16" t="s">
-        <v>2382</v>
+        <v>2653</v>
       </c>
       <c r="B434" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C434" s="37"/>
+      <c r="C434" s="37" t="s">
+        <v>2660</v>
+      </c>
+      <c r="D434" t="s">
+        <v>2664</v>
+      </c>
     </row>
     <row r="435" spans="1:4">
-      <c r="A435" s="16"/>
-      <c r="B435" s="16"/>
-      <c r="C435" s="37"/>
+      <c r="A435" s="16" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B435" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C435" s="32" t="s">
+        <v>2650</v>
+      </c>
+      <c r="D435" t="s">
+        <v>2665</v>
+      </c>
     </row>
     <row r="436" spans="1:4">
-      <c r="A436" s="16"/>
-      <c r="B436" s="16"/>
-      <c r="C436" s="37"/>
+      <c r="A436" s="16" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B436" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C436" s="37" t="s">
+        <v>2645</v>
+      </c>
+      <c r="D436" t="s">
+        <v>2667</v>
+      </c>
     </row>
     <row r="437" spans="1:4">
-      <c r="A437" s="16"/>
-      <c r="B437" s="16"/>
-      <c r="C437" s="37"/>
+      <c r="A437" s="16" t="s">
+        <v>2657</v>
+      </c>
+      <c r="B437" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C437" s="32" t="s">
+        <v>2646</v>
+      </c>
+      <c r="D437" t="s">
+        <v>2663</v>
+      </c>
     </row>
     <row r="438" spans="1:4">
-      <c r="A438" s="16"/>
-      <c r="B438" s="16"/>
-      <c r="C438" s="37"/>
+      <c r="A438" s="16" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B438" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C438" s="37" t="s">
+        <v>2647</v>
+      </c>
+      <c r="D438" t="s">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4">
+      <c r="A439" s="16" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B439" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C439" s="32" t="s">
+        <v>2650</v>
+      </c>
+      <c r="D439" t="s">
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4">
+      <c r="A440" s="16" t="s">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4">
+      <c r="A445" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C445" s="22" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D445" t="str">
+        <f>"line along "&amp;B445&amp;" of "&amp;C445</f>
+        <v>line along proximal-distal of lateral side' some talus</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4">
+      <c r="A446" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B446" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C446" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D446" t="str">
+        <f>"line along "&amp;B446&amp;" of "&amp;C446</f>
+        <v>line along proximal-distal of pes</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4">
+      <c r="A447" t="s">
+        <v>1220</v>
+      </c>
     </row>
     <row r="448" spans="1:4">
       <c r="A448" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B448" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C448" s="22" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D448" t="str">
-        <f>"line along "&amp;B448&amp;" of "&amp;C448</f>
-        <v>line along proximal-distal of lateral side' some talus</v>
-      </c>
-    </row>
-    <row r="449" spans="1:4">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B449" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C449" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D449" t="str">
-        <f>"line along "&amp;B449&amp;" of "&amp;C449</f>
-        <v>line along proximal-distal of pes</v>
-      </c>
-    </row>
-    <row r="450" spans="1:4">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="451" spans="1:4">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="452" spans="1:4">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="453" spans="1:4">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="454" spans="1:4">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="455" spans="1:4">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="456" spans="1:4">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="457" spans="1:4">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="458" spans="1:4">
-      <c r="A458" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="459" spans="1:4">
-      <c r="A459" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="460" spans="1:4">
-      <c r="A460" t="s">
         <v>537</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1">
+      <c r="A464" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1">
+      <c r="A465" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1">
+      <c r="A466" s="1" t="s">
+        <v>1130</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" s="1" t="s">
-        <v>620</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" s="1" t="s">
-        <v>623</v>
+        <v>629</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" s="1" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="470" spans="1:1">
-      <c r="A470" s="1" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="471" spans="1:1">
-      <c r="A471" s="1" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="472" spans="1:1">
-      <c r="A472" s="1" t="s">
         <v>630</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added premolar 3 height patterns
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADD7335-5493-4A8B-998A-BF6AD66A0713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C1F1B3-B22C-492D-95F2-0B9064B1CA1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -92,7 +92,7 @@
     check these?</t>
       </text>
     </comment>
-    <comment ref="C308" authorId="1" shapeId="0" xr:uid="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
+    <comment ref="C309" authorId="1" shapeId="0" xr:uid="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5352" uniqueCount="2685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5379" uniqueCount="2705">
   <si>
     <t>Status</t>
   </si>
@@ -8232,6 +8232,66 @@
   </si>
   <si>
     <t>Premolar 3 crown height</t>
+  </si>
+  <si>
+    <t>Upper premolar 3 crown height</t>
+  </si>
+  <si>
+    <t>Lower premolar 3 crown height</t>
+  </si>
+  <si>
+    <t>Upper secondary premolar 3 height</t>
+  </si>
+  <si>
+    <t>Upper primary premolar 3 height</t>
+  </si>
+  <si>
+    <t>Lower secondary premolar 3 height</t>
+  </si>
+  <si>
+    <t>Lower primary premolar 3 height</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'premolar 3')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower premolar 3')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper premolar 3')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper third secondary premolar tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and  ('part of' some 'upper third primary premolar tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower third secondary premolar tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower third primary premolar tooth')</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of premolar 3</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper premolar 3</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower premolar 3</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper third secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower third secondary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower third primary premolar tooth</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper third primary premolar tooth</t>
   </si>
 </sst>
 </file>
@@ -8800,7 +8860,7 @@
   <threadedComment ref="C151" dT="2021-04-21T23:28:43.22" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{0D4CF0A9-8CA0-4BED-8E0F-2717916146F3}">
     <text>check these?</text>
   </threadedComment>
-  <threadedComment ref="C308" dT="2021-04-23T17:10:42.70" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
+  <threadedComment ref="C309" dT="2021-04-23T17:10:42.70" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
     <text>Not sure if this needs a term other than 'occlusal surface'?</text>
   </threadedComment>
 </ThreadedComments>
@@ -23510,11 +23570,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
-  <dimension ref="A1:D475"/>
+  <dimension ref="A1:D476"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A254" sqref="A254"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D260" sqref="D260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -27074,2364 +27134,2457 @@
       <c r="A253" t="s">
         <v>2684</v>
       </c>
+      <c r="B253" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C253" s="22" t="s">
+        <v>2691</v>
+      </c>
+      <c r="D253" t="s">
+        <v>2698</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B254" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C254" s="22" t="s">
+        <v>2693</v>
+      </c>
+      <c r="D254" t="s">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B255" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C255" s="22" t="s">
+        <v>2692</v>
+      </c>
+      <c r="D255" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B256" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C256" s="22" t="s">
+        <v>2694</v>
+      </c>
+      <c r="D256" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" t="s">
+        <v>2688</v>
+      </c>
+      <c r="B257" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C257" s="22" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D257" t="s">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B258" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C258" s="22" t="s">
+        <v>2696</v>
+      </c>
+      <c r="D258" t="s">
+        <v>2702</v>
+      </c>
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>2050</v>
+        <v>2690</v>
       </c>
       <c r="B259" t="s">
-        <v>108</v>
-      </c>
-      <c r="C259" t="s">
-        <v>2192</v>
+        <v>2140</v>
+      </c>
+      <c r="C259" s="22" t="s">
+        <v>2697</v>
       </c>
       <c r="D259" t="s">
-        <v>2062</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B260" t="s">
         <v>108</v>
       </c>
       <c r="C260" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="D260" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B261" t="s">
         <v>108</v>
       </c>
       <c r="C261" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="D261" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B262" t="s">
         <v>108</v>
       </c>
       <c r="C262" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="D262" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B263" t="s">
         <v>108</v>
       </c>
       <c r="C263" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="D263" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B264" t="s">
         <v>108</v>
       </c>
       <c r="C264" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="D264" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="B265" t="s">
         <v>108</v>
       </c>
       <c r="C265" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="D265" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>2069</v>
+        <v>2056</v>
       </c>
       <c r="B266" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C266" t="s">
-        <v>2192</v>
+        <v>2198</v>
       </c>
       <c r="D266" t="s">
-        <v>2076</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B267" t="s">
         <v>112</v>
       </c>
       <c r="C267" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="D267" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="B268" t="s">
         <v>112</v>
       </c>
       <c r="C268" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="D268" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B269" t="s">
         <v>112</v>
       </c>
       <c r="C269" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="D269" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="B270" t="s">
         <v>112</v>
       </c>
       <c r="C270" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="D270" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="B271" t="s">
         <v>112</v>
       </c>
       <c r="C271" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="D271" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B272" t="s">
         <v>112</v>
       </c>
       <c r="C272" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="D272" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>2083</v>
+        <v>2075</v>
       </c>
       <c r="B273" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C273" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="D273" t="s">
-        <v>2099</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B274" t="s">
         <v>108</v>
       </c>
       <c r="C274" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="D274" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B275" t="s">
         <v>108</v>
       </c>
       <c r="C275" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="D275" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B276" t="s">
         <v>108</v>
       </c>
       <c r="C276" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="D276" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="B277" t="s">
         <v>108</v>
       </c>
       <c r="C277" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="D277" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B278" t="s">
         <v>108</v>
       </c>
       <c r="C278" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="D278" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B279" t="s">
         <v>108</v>
       </c>
       <c r="C279" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="D279" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>2670</v>
+        <v>2089</v>
       </c>
       <c r="B280" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C280" t="s">
-        <v>2199</v>
+        <v>2205</v>
       </c>
       <c r="D280" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="B281" t="s">
         <v>112</v>
       </c>
       <c r="C281" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="D281" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="B282" t="s">
         <v>112</v>
       </c>
       <c r="C282" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="D282" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
       <c r="B283" t="s">
         <v>112</v>
       </c>
       <c r="C283" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="D283" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="B284" t="s">
         <v>112</v>
       </c>
       <c r="C284" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="D284" t="s">
-        <v>2109</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="B285" t="s">
         <v>112</v>
       </c>
       <c r="C285" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="D285" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="B286" t="s">
         <v>112</v>
       </c>
       <c r="C286" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="D286" t="s">
-        <v>2110</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="287" spans="1:4">
-      <c r="A287" s="31" t="s">
-        <v>2114</v>
+      <c r="A287" t="s">
+        <v>2676</v>
       </c>
       <c r="B287" t="s">
         <v>112</v>
       </c>
-      <c r="C287" s="16" t="s">
-        <v>2206</v>
+      <c r="C287" t="s">
+        <v>2205</v>
       </c>
       <c r="D287" t="s">
-        <v>2122</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="31" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="B288" t="s">
         <v>112</v>
       </c>
       <c r="C288" s="16" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="D288" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="289" spans="1:4">
       <c r="A289" s="31" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="B289" t="s">
         <v>112</v>
       </c>
       <c r="C289" s="16" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="D289" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="31" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="B290" t="s">
         <v>112</v>
       </c>
       <c r="C290" s="16" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="D290" t="s">
-        <v>2425</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="31" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="B291" t="s">
         <v>112</v>
       </c>
       <c r="C291" s="16" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="D291" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="31" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="B292" t="s">
         <v>112</v>
       </c>
       <c r="C292" s="16" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="D292" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="31" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="B293" t="s">
         <v>112</v>
       </c>
       <c r="C293" s="16" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="D293" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="31" t="s">
-        <v>2125</v>
+        <v>2120</v>
       </c>
       <c r="B294" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C294" s="16" t="s">
-        <v>2206</v>
+        <v>2212</v>
       </c>
       <c r="D294" t="s">
-        <v>2132</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="31" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="B295" t="s">
         <v>108</v>
       </c>
       <c r="C295" s="16" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="D295" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="296" spans="1:4">
       <c r="A296" s="31" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="B296" t="s">
         <v>108</v>
       </c>
       <c r="C296" s="16" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="D296" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="297" spans="1:4">
       <c r="A297" s="31" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="B297" t="s">
         <v>108</v>
       </c>
-      <c r="C297" t="s">
-        <v>2209</v>
+      <c r="C297" s="16" t="s">
+        <v>2208</v>
       </c>
       <c r="D297" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="298" spans="1:4">
       <c r="A298" s="31" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="B298" t="s">
         <v>108</v>
       </c>
       <c r="C298" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="D298" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="31" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="B299" t="s">
         <v>108</v>
       </c>
       <c r="C299" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="D299" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="31" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="B300" t="s">
         <v>108</v>
       </c>
       <c r="C300" t="s">
+        <v>2211</v>
+      </c>
+      <c r="D300" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301" s="31" t="s">
+        <v>2131</v>
+      </c>
+      <c r="B301" t="s">
+        <v>108</v>
+      </c>
+      <c r="C301" t="s">
         <v>2212</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D301" t="s">
         <v>2138</v>
-      </c>
-    </row>
-    <row r="301" spans="1:4">
-      <c r="A301" s="16" t="s">
-        <v>2139</v>
-      </c>
-      <c r="B301" s="16" t="s">
-        <v>2140</v>
-      </c>
-      <c r="C301" s="32" t="s">
-        <v>2221</v>
-      </c>
-      <c r="D301" t="s">
-        <v>2213</v>
       </c>
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="16" t="s">
-        <v>2214</v>
+        <v>2139</v>
       </c>
       <c r="B302" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C302" s="32" t="s">
-        <v>2220</v>
+        <v>2221</v>
       </c>
       <c r="D302" t="s">
-        <v>2227</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="16" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="B303" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C303" s="32" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="D303" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="16" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="B304" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C304" s="32" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="D304" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="305" spans="1:4">
       <c r="A305" s="16" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="B305" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C305" s="32" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="D305" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="306" spans="1:4">
       <c r="A306" s="16" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="B306" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C306" s="32" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="D306" t="s">
-        <v>2230</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="307" spans="1:4">
       <c r="A307" s="16" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="B307" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C307" s="32" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="D307" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="308" spans="1:4">
       <c r="A308" s="16" t="s">
-        <v>2372</v>
+        <v>2219</v>
       </c>
       <c r="B308" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C308" s="37" t="s">
-        <v>2555</v>
+        <v>2140</v>
+      </c>
+      <c r="C308" s="32" t="s">
+        <v>2226</v>
+      </c>
+      <c r="D308" t="s">
+        <v>2232</v>
       </c>
     </row>
     <row r="309" spans="1:4">
       <c r="A309" s="16" t="s">
-        <v>2419</v>
+        <v>2372</v>
       </c>
       <c r="B309" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C309" s="37" t="s">
-        <v>2429</v>
-      </c>
-    </row>
-    <row r="310" spans="1:4" ht="16.899999999999999" customHeight="1">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
       <c r="A310" s="16" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="B310" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C310" s="37" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A311" s="16" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="B311" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C311" s="37" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A312" s="16" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="B312" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C312" s="37" t="s">
-        <v>2434</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A313" s="16" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="B313" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C313" s="37" t="s">
-        <v>2432</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A314" s="16" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="B314" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C314" s="37" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A315" s="16" t="s">
-        <v>2435</v>
+        <v>2424</v>
       </c>
       <c r="B315" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C315" s="37" t="s">
-        <v>2555</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A316" s="16" t="s">
-        <v>2492</v>
+        <v>2435</v>
       </c>
       <c r="B316" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C316" s="37" t="s">
-        <v>2429</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A317" s="16" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="B317" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C317" s="37" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A318" s="16" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="B318" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C318" s="37" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A319" s="16" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="B319" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C319" s="37" t="s">
-        <v>2434</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A320" s="16" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B320" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C320" s="37" t="s">
-        <v>2432</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A321" s="16" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="B321" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C321" s="37" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A322" s="16" t="s">
-        <v>2491</v>
+        <v>2497</v>
       </c>
       <c r="B322" s="16" t="s">
-        <v>2140</v>
+        <v>108</v>
       </c>
       <c r="C322" s="37" t="s">
-        <v>2555</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A323" s="16" t="s">
-        <v>2498</v>
+        <v>2491</v>
       </c>
       <c r="B323" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C323" s="37" t="s">
-        <v>2429</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A324" s="16" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="B324" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C324" s="37" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A325" s="16" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
       <c r="B325" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C325" s="37" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A326" s="16" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="B326" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C326" s="37" t="s">
-        <v>2434</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A327" s="16" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="B327" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C327" s="37" t="s">
-        <v>2432</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A328" s="16" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="B328" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C328" s="37" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A329" s="16" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="B329" s="16" t="s">
-        <v>112</v>
+        <v>2140</v>
       </c>
       <c r="C329" s="37" t="s">
-        <v>2525</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A330" s="16" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="B330" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C330" s="37" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="331" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A331" s="16" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="B331" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C331" s="37" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A332" s="16" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="B332" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C332" s="37" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="333" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A333" s="16" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="B333" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C333" s="37" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A334" s="16" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
       <c r="B334" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C334" s="37" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="335" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A335" s="16" t="s">
-        <v>2510</v>
+        <v>2509</v>
       </c>
       <c r="B335" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C335" s="37" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="336" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A336" s="16" t="s">
-        <v>2511</v>
+        <v>2510</v>
       </c>
       <c r="B336" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C336" s="37" t="s">
-        <v>2525</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A337" s="16" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="B337" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C337" s="37" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A338" s="16" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="B338" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C338" s="37" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A339" s="16" t="s">
-        <v>2514</v>
+        <v>2513</v>
       </c>
       <c r="B339" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C339" s="37" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A340" s="16" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="B340" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C340" s="37" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="341" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A341" s="16" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="B341" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C341" s="37" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A342" s="16" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="B342" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C342" s="37" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A343" s="16" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="B343" s="16" t="s">
-        <v>2140</v>
+        <v>108</v>
       </c>
       <c r="C343" s="37" t="s">
-        <v>2525</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A344" s="16" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B344" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C344" s="37" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="345" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A345" s="16" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B345" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C345" s="37" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A346" s="16" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B346" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C346" s="37" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="347" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A347" s="16" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B347" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C347" s="37" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
     </row>
     <row r="348" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A348" s="16" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="B348" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C348" s="37" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A349" s="16" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="B349" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C349" s="37" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A350" s="16" t="s">
-        <v>2532</v>
+        <v>2524</v>
       </c>
       <c r="B350" s="16" t="s">
-        <v>112</v>
+        <v>2140</v>
       </c>
       <c r="C350" s="37" t="s">
-        <v>2553</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="351" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A351" s="16" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="B351" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C351" s="37" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="352" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A352" s="16" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="B352" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C352" s="37" t="s">
-        <v>2554</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="353" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A353" s="16" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="B353" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C353" s="37" t="s">
-        <v>2558</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A354" s="16" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="B354" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C354" s="37" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="355" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A355" s="16" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="B355" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C355" s="37" t="s">
-        <v>2557</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="356" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A356" s="16" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="B356" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C356" s="37" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A357" s="16" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="B357" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C357" s="37" t="s">
-        <v>2553</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A358" s="16" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="B358" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C358" s="37" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A359" s="16" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="B359" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C359" s="37" t="s">
-        <v>2554</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A360" s="16" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="B360" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C360" s="37" t="s">
-        <v>2558</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A361" s="16" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="B361" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C361" s="37" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A362" s="16" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="B362" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C362" s="37" t="s">
-        <v>2557</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="363" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A363" s="16" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="B363" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C363" s="37" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="364" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A364" s="16" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="B364" s="16" t="s">
-        <v>2140</v>
+        <v>108</v>
       </c>
       <c r="C364" s="37" t="s">
-        <v>2553</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="365" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A365" s="16" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="B365" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C365" s="37" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="366" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A366" s="16" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="B366" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C366" s="37" t="s">
-        <v>2554</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="367" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A367" s="16" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="B367" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C367" s="37" t="s">
-        <v>2558</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A368" s="16" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="B368" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C368" s="37" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="369" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A369" s="16" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="B369" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C369" s="37" t="s">
-        <v>2557</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="370" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A370" s="16" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="B370" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C370" s="37" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="371" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A371" s="16" t="s">
-        <v>2561</v>
+        <v>2552</v>
       </c>
       <c r="B371" s="16" t="s">
-        <v>112</v>
+        <v>2140</v>
       </c>
       <c r="C371" s="37" t="s">
-        <v>2582</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A372" s="16" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="B372" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C372" s="37" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A373" s="16" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="B373" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C373" s="37" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A374" s="16" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="B374" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C374" s="37" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="375" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A375" s="16" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="B375" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C375" s="37" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="376" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A376" s="16" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="B376" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C376" s="37" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="377" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A377" s="16" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="B377" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C377" s="37" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="378" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A378" s="16" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="B378" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C378" s="37" t="s">
-        <v>2582</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="379" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A379" s="16" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="B379" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C379" s="37" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="380" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A380" s="16" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="B380" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C380" s="37" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="381" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A381" s="16" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="B381" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C381" s="37" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="382" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A382" s="16" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="B382" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C382" s="37" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="383" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A383" s="16" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="B383" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C383" s="37" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="384" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A384" s="16" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="B384" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C384" s="37" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A385" s="16" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="B385" s="16" t="s">
-        <v>2140</v>
+        <v>108</v>
       </c>
       <c r="C385" s="37" t="s">
-        <v>2582</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="386" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A386" s="16" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="B386" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C386" s="37" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="387" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A387" s="16" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="B387" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C387" s="37" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="388" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A388" s="16" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="B388" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C388" s="37" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="389" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A389" s="16" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="B389" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C389" s="37" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="390" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A390" s="16" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="B390" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C390" s="37" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="391" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A391" s="16" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="B391" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C391" s="37" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="392" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A392" s="16" t="s">
-        <v>2589</v>
+        <v>2581</v>
       </c>
       <c r="B392" s="16" t="s">
-        <v>112</v>
+        <v>2140</v>
       </c>
       <c r="C392" s="37" t="s">
-        <v>2610</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="393" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A393" s="16" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="B393" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C393" s="37" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="394" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A394" s="16" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="B394" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C394" s="37" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="395" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A395" s="16" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="B395" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C395" s="37" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="396" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A396" s="16" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="B396" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C396" s="37" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="397" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A397" s="16" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="B397" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C397" s="37" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="398" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A398" s="16" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="B398" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C398" s="37" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="399" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A399" s="16" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="B399" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C399" s="37" t="s">
-        <v>2610</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="400" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A400" s="16" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="B400" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C400" s="37" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="401" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A401" s="16" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="B401" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C401" s="37" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="402" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A402" s="16" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="B402" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C402" s="37" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A403" s="16" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="B403" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C403" s="37" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A404" s="16" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="B404" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C404" s="37" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A405" s="16" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B405" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C405" s="37" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="406" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A406" s="16" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="B406" s="16" t="s">
-        <v>2140</v>
+        <v>108</v>
       </c>
       <c r="C406" s="37" t="s">
-        <v>2610</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A407" s="16" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="B407" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C407" s="37" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A408" s="16" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="B408" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C408" s="37" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A409" s="16" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="B409" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C409" s="37" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="410" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A410" s="16" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="B410" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C410" s="37" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A411" s="16" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="B411" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C411" s="37" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A412" s="16" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="B412" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C412" s="37" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A413" s="16" t="s">
-        <v>2617</v>
+        <v>2609</v>
       </c>
       <c r="B413" s="16" t="s">
-        <v>112</v>
+        <v>2140</v>
       </c>
       <c r="C413" s="37" t="s">
-        <v>2638</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A414" s="16" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="B414" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C414" s="37" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A415" s="16" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="B415" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C415" s="37" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A416" s="16" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="B416" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C416" s="37" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A417" s="16" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="B417" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C417" s="37" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A418" s="16" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="B418" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C418" s="37" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A419" s="16" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="B419" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C419" s="37" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A420" s="16" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="B420" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C420" s="37" t="s">
-        <v>2638</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="421" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A421" s="16" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="B421" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C421" s="37" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A422" s="16" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="B422" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C422" s="37" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A423" s="16" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="B423" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C423" s="37" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A424" s="16" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="B424" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C424" s="37" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A425" s="16" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="B425" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C425" s="37" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A426" s="16" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="B426" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C426" s="37" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A427" s="16" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="B427" s="16" t="s">
-        <v>2140</v>
+        <v>108</v>
       </c>
       <c r="C427" s="37" t="s">
-        <v>2638</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A428" s="16" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="B428" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C428" s="37" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A429" s="16" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="B429" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C429" s="37" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A430" s="16" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="B430" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C430" s="37" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A431" s="16" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="B431" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C431" s="37" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="432" spans="1:3" ht="16.899999999999999" customHeight="1">
       <c r="A432" s="16" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="B432" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C432" s="37" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="433" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A433" s="16" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="B433" s="16" t="s">
         <v>2140</v>
       </c>
       <c r="C433" s="37" t="s">
+        <v>2643</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" ht="16.899999999999999" customHeight="1">
+      <c r="A434" s="16" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B434" s="16" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C434" s="37" t="s">
         <v>2644</v>
-      </c>
-    </row>
-    <row r="434" spans="1:4">
-      <c r="A434" s="16" t="s">
-        <v>2417</v>
-      </c>
-      <c r="B434" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C434" s="37" t="s">
-        <v>2645</v>
-      </c>
-      <c r="D434" t="s">
-        <v>2380</v>
       </c>
     </row>
     <row r="435" spans="1:4">
       <c r="A435" s="16" t="s">
-        <v>2381</v>
+        <v>2417</v>
       </c>
       <c r="B435" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C435" s="37" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="D435" t="s">
-        <v>2648</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="436" spans="1:4">
       <c r="A436" s="16" t="s">
-        <v>2418</v>
+        <v>2381</v>
       </c>
       <c r="B436" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C436" s="37" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="D436" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="437" spans="1:4">
       <c r="A437" s="16" t="s">
-        <v>2382</v>
+        <v>2418</v>
       </c>
       <c r="B437" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C437" s="37" t="s">
-        <v>2650</v>
+        <v>2647</v>
       </c>
       <c r="D437" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="438" spans="1:4">
       <c r="A438" s="16" t="s">
-        <v>2652</v>
+        <v>2382</v>
       </c>
       <c r="B438" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C438" s="37" t="s">
-        <v>2659</v>
+        <v>2650</v>
       </c>
       <c r="D438" t="s">
-        <v>2661</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="439" spans="1:4">
       <c r="A439" s="16" t="s">
-        <v>2655</v>
+        <v>2652</v>
       </c>
       <c r="B439" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C439" s="32" t="s">
-        <v>2646</v>
+      <c r="C439" s="37" t="s">
+        <v>2659</v>
       </c>
       <c r="D439" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="440" spans="1:4">
       <c r="A440" s="16" t="s">
-        <v>2653</v>
+        <v>2655</v>
       </c>
       <c r="B440" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C440" s="37" t="s">
-        <v>2660</v>
+      <c r="C440" s="32" t="s">
+        <v>2646</v>
       </c>
       <c r="D440" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="441" spans="1:4">
       <c r="A441" s="16" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="B441" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C441" s="32" t="s">
-        <v>2650</v>
+      <c r="C441" s="37" t="s">
+        <v>2660</v>
       </c>
       <c r="D441" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="442" spans="1:4">
       <c r="A442" s="16" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
       <c r="B442" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C442" s="37" t="s">
-        <v>2645</v>
+      <c r="C442" s="32" t="s">
+        <v>2650</v>
       </c>
       <c r="D442" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="443" spans="1:4">
       <c r="A443" s="16" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
       <c r="B443" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C443" s="32" t="s">
-        <v>2646</v>
+      <c r="C443" s="37" t="s">
+        <v>2645</v>
       </c>
       <c r="D443" t="s">
-        <v>2663</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="444" spans="1:4">
       <c r="A444" s="16" t="s">
-        <v>2669</v>
+        <v>2657</v>
       </c>
       <c r="B444" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C444" s="37" t="s">
-        <v>2647</v>
+      <c r="C444" s="32" t="s">
+        <v>2646</v>
       </c>
       <c r="D444" t="s">
-        <v>2668</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="445" spans="1:4">
       <c r="A445" s="16" t="s">
-        <v>2658</v>
+        <v>2669</v>
       </c>
       <c r="B445" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C445" s="32" t="s">
-        <v>2650</v>
+      <c r="C445" s="37" t="s">
+        <v>2647</v>
       </c>
       <c r="D445" t="s">
-        <v>2666</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="446" spans="1:4">
       <c r="A446" s="16" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B446" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C446" s="32" t="s">
+        <v>2650</v>
+      </c>
+      <c r="D446" t="s">
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4">
+      <c r="A447" s="16" t="s">
         <v>2677</v>
-      </c>
-    </row>
-    <row r="451" spans="1:4">
-      <c r="A451" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B451" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C451" s="22" t="s">
-        <v>1218</v>
-      </c>
-      <c r="D451" t="str">
-        <f>"line along "&amp;B451&amp;" of "&amp;C451</f>
-        <v>line along proximal-distal of lateral side' some talus</v>
       </c>
     </row>
     <row r="452" spans="1:4">
       <c r="A452" t="s">
-        <v>1216</v>
+        <v>1230</v>
       </c>
       <c r="B452" t="s">
         <v>1217</v>
       </c>
-      <c r="C452" t="s">
-        <v>1219</v>
+      <c r="C452" s="22" t="s">
+        <v>1218</v>
       </c>
       <c r="D452" t="str">
         <f>"line along "&amp;B452&amp;" of "&amp;C452</f>
-        <v>line along proximal-distal of pes</v>
+        <v>line along proximal-distal of lateral side' some talus</v>
       </c>
     </row>
     <row r="453" spans="1:4">
       <c r="A453" t="s">
-        <v>1220</v>
+        <v>1216</v>
+      </c>
+      <c r="B453" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C453" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D453" t="str">
+        <f>"line along "&amp;B453&amp;" of "&amp;C453</f>
+        <v>line along proximal-distal of pes</v>
       </c>
     </row>
     <row r="454" spans="1:4">
       <c r="A454" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="455" spans="1:4">
       <c r="A455" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="456" spans="1:4">
       <c r="A456" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="457" spans="1:4">
       <c r="A457" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="458" spans="1:4">
       <c r="A458" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="459" spans="1:4">
       <c r="A459" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="460" spans="1:4">
       <c r="A460" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="461" spans="1:4">
       <c r="A461" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="462" spans="1:4">
       <c r="A462" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="463" spans="1:4">
       <c r="A463" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4">
+      <c r="A464" t="s">
         <v>537</v>
-      </c>
-    </row>
-    <row r="470" spans="1:1">
-      <c r="A470" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" s="1" t="s">
-        <v>1130</v>
+        <v>623</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" s="1" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" s="1" t="s">
-        <v>629</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1">
+      <c r="A476" s="1" t="s">
         <v>630</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added remaining incisor axis pattern names
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC90F0-80F5-473E-A04C-7AC47B2C9C01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3533C57-752F-47AD-9D38-9186BBE22AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6980" uniqueCount="2753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7106" uniqueCount="2816">
   <si>
     <t>Status</t>
   </si>
@@ -8436,6 +8436,195 @@
   </si>
   <si>
     <t>line along upper-lower axis of lower primary incisor 3</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of incisor 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of incisor 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper incisor 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower incisor 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper incisor 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower incisor 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper secondary incisor 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper secondary incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper primary incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower secondary incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower primary incisor 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper secondary incisor 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper primary incisor 5</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower secondary incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper primary incisor 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower secondary incisor 4</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower primary incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper secondary incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper primary incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower secondary incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower primary incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper secondary incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper primary incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower secondary incisor 4</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower primary incisor 4</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower primary incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper secondary incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper primary incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower secondary incisor 5</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower primary incisor 5</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of incisor 6</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper incisor 6</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower incisor 6</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper secondary incisor 6</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of upper primary incisor 6</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower secondary incisor 6</t>
+  </si>
+  <si>
+    <t>line along anterior-posterior axis of lower primary incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper secondary incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of upper primary incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower secondary incisor 6</t>
+  </si>
+  <si>
+    <t>line along medial-lateral axis of lower primary incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper secondary incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper primary incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower secondary incisor 6</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower primary incisor 6</t>
   </si>
 </sst>
 </file>
@@ -23716,9 +23905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
   <dimension ref="A1:D472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D368" sqref="D368"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D431" sqref="D431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -28894,8 +29083,11 @@
       <c r="C368" s="37" t="s">
         <v>2567</v>
       </c>
-    </row>
-    <row r="369" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D368" t="s">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A369" s="16" t="s">
         <v>2547</v>
       </c>
@@ -28905,8 +29097,11 @@
       <c r="C369" s="37" t="s">
         <v>2568</v>
       </c>
-    </row>
-    <row r="370" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D369" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A370" s="16" t="s">
         <v>2548</v>
       </c>
@@ -28916,8 +29111,11 @@
       <c r="C370" s="37" t="s">
         <v>2569</v>
       </c>
-    </row>
-    <row r="371" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D370" t="s">
+        <v>2761</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A371" s="16" t="s">
         <v>2549</v>
       </c>
@@ -28927,8 +29125,11 @@
       <c r="C371" s="37" t="s">
         <v>2570</v>
       </c>
-    </row>
-    <row r="372" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D371" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A372" s="16" t="s">
         <v>2550</v>
       </c>
@@ -28938,8 +29139,11 @@
       <c r="C372" s="37" t="s">
         <v>2571</v>
       </c>
-    </row>
-    <row r="373" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D372" t="s">
+        <v>2770</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A373" s="16" t="s">
         <v>2551</v>
       </c>
@@ -28949,8 +29153,11 @@
       <c r="C373" s="37" t="s">
         <v>2572</v>
       </c>
-    </row>
-    <row r="374" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D373" t="s">
+        <v>2771</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A374" s="16" t="s">
         <v>2552</v>
       </c>
@@ -28960,8 +29167,11 @@
       <c r="C374" s="37" t="s">
         <v>2573</v>
       </c>
-    </row>
-    <row r="375" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D374" t="s">
+        <v>2772</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A375" s="16" t="s">
         <v>2553</v>
       </c>
@@ -28971,8 +29181,11 @@
       <c r="C375" s="37" t="s">
         <v>2567</v>
       </c>
-    </row>
-    <row r="376" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D375" t="s">
+        <v>2773</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A376" s="16" t="s">
         <v>2554</v>
       </c>
@@ -28982,8 +29195,11 @@
       <c r="C376" s="37" t="s">
         <v>2568</v>
       </c>
-    </row>
-    <row r="377" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D376" t="s">
+        <v>2774</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A377" s="16" t="s">
         <v>2555</v>
       </c>
@@ -28993,8 +29209,11 @@
       <c r="C377" s="37" t="s">
         <v>2569</v>
       </c>
-    </row>
-    <row r="378" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D377" t="s">
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A378" s="16" t="s">
         <v>2556</v>
       </c>
@@ -29004,8 +29223,11 @@
       <c r="C378" s="37" t="s">
         <v>2570</v>
       </c>
-    </row>
-    <row r="379" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D378" t="s">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A379" s="16" t="s">
         <v>2557</v>
       </c>
@@ -29015,8 +29237,11 @@
       <c r="C379" s="37" t="s">
         <v>2571</v>
       </c>
-    </row>
-    <row r="380" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D379" t="s">
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A380" s="16" t="s">
         <v>2558</v>
       </c>
@@ -29026,8 +29251,11 @@
       <c r="C380" s="37" t="s">
         <v>2572</v>
       </c>
-    </row>
-    <row r="381" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D380" t="s">
+        <v>2778</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A381" s="16" t="s">
         <v>2559</v>
       </c>
@@ -29037,8 +29265,11 @@
       <c r="C381" s="37" t="s">
         <v>2573</v>
       </c>
-    </row>
-    <row r="382" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D381" t="s">
+        <v>2779</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A382" s="16" t="s">
         <v>2560</v>
       </c>
@@ -29048,8 +29279,11 @@
       <c r="C382" s="37" t="s">
         <v>2567</v>
       </c>
-    </row>
-    <row r="383" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D382" t="s">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A383" s="16" t="s">
         <v>2561</v>
       </c>
@@ -29059,8 +29293,11 @@
       <c r="C383" s="37" t="s">
         <v>2568</v>
       </c>
-    </row>
-    <row r="384" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D383" t="s">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A384" s="16" t="s">
         <v>2562</v>
       </c>
@@ -29070,8 +29307,11 @@
       <c r="C384" s="37" t="s">
         <v>2569</v>
       </c>
-    </row>
-    <row r="385" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D384" t="s">
+        <v>2782</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A385" s="16" t="s">
         <v>2563</v>
       </c>
@@ -29081,8 +29321,11 @@
       <c r="C385" s="37" t="s">
         <v>2570</v>
       </c>
-    </row>
-    <row r="386" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D385" t="s">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A386" s="16" t="s">
         <v>2564</v>
       </c>
@@ -29092,8 +29335,11 @@
       <c r="C386" s="37" t="s">
         <v>2571</v>
       </c>
-    </row>
-    <row r="387" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D386" t="s">
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A387" s="16" t="s">
         <v>2565</v>
       </c>
@@ -29103,8 +29349,11 @@
       <c r="C387" s="37" t="s">
         <v>2572</v>
       </c>
-    </row>
-    <row r="388" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D387" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A388" s="16" t="s">
         <v>2566</v>
       </c>
@@ -29114,8 +29363,11 @@
       <c r="C388" s="37" t="s">
         <v>2573</v>
       </c>
-    </row>
-    <row r="389" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D388" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A389" s="16" t="s">
         <v>2574</v>
       </c>
@@ -29125,8 +29377,11 @@
       <c r="C389" s="37" t="s">
         <v>2595</v>
       </c>
-    </row>
-    <row r="390" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D389" t="s">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A390" s="16" t="s">
         <v>2575</v>
       </c>
@@ -29136,8 +29391,11 @@
       <c r="C390" s="37" t="s">
         <v>2596</v>
       </c>
-    </row>
-    <row r="391" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D390" t="s">
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A391" s="16" t="s">
         <v>2576</v>
       </c>
@@ -29147,8 +29405,11 @@
       <c r="C391" s="37" t="s">
         <v>2597</v>
       </c>
-    </row>
-    <row r="392" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D391" t="s">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A392" s="16" t="s">
         <v>2577</v>
       </c>
@@ -29158,8 +29419,11 @@
       <c r="C392" s="37" t="s">
         <v>2598</v>
       </c>
-    </row>
-    <row r="393" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D392" t="s">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A393" s="16" t="s">
         <v>2578</v>
       </c>
@@ -29169,8 +29433,11 @@
       <c r="C393" s="37" t="s">
         <v>2599</v>
       </c>
-    </row>
-    <row r="394" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D393" t="s">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A394" s="16" t="s">
         <v>2579</v>
       </c>
@@ -29180,8 +29447,11 @@
       <c r="C394" s="37" t="s">
         <v>2600</v>
       </c>
-    </row>
-    <row r="395" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D394" t="s">
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A395" s="16" t="s">
         <v>2580</v>
       </c>
@@ -29191,8 +29461,11 @@
       <c r="C395" s="37" t="s">
         <v>2601</v>
       </c>
-    </row>
-    <row r="396" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D395" t="s">
+        <v>2766</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A396" s="16" t="s">
         <v>2581</v>
       </c>
@@ -29202,8 +29475,11 @@
       <c r="C396" s="37" t="s">
         <v>2595</v>
       </c>
-    </row>
-    <row r="397" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D396" t="s">
+        <v>2755</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A397" s="16" t="s">
         <v>2582</v>
       </c>
@@ -29213,8 +29489,11 @@
       <c r="C397" s="37" t="s">
         <v>2596</v>
       </c>
-    </row>
-    <row r="398" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D397" t="s">
+        <v>2759</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A398" s="16" t="s">
         <v>2583</v>
       </c>
@@ -29224,8 +29503,11 @@
       <c r="C398" s="37" t="s">
         <v>2597</v>
       </c>
-    </row>
-    <row r="399" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D398" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A399" s="16" t="s">
         <v>2584</v>
       </c>
@@ -29235,8 +29517,11 @@
       <c r="C399" s="37" t="s">
         <v>2598</v>
       </c>
-    </row>
-    <row r="400" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D399" t="s">
+        <v>2767</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A400" s="16" t="s">
         <v>2585</v>
       </c>
@@ -29246,8 +29531,11 @@
       <c r="C400" s="37" t="s">
         <v>2599</v>
       </c>
-    </row>
-    <row r="401" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D400" t="s">
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A401" s="16" t="s">
         <v>2586</v>
       </c>
@@ -29257,8 +29545,11 @@
       <c r="C401" s="37" t="s">
         <v>2600</v>
       </c>
-    </row>
-    <row r="402" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D401" t="s">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A402" s="16" t="s">
         <v>2587</v>
       </c>
@@ -29268,8 +29559,11 @@
       <c r="C402" s="37" t="s">
         <v>2601</v>
       </c>
-    </row>
-    <row r="403" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D402" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A403" s="16" t="s">
         <v>2588</v>
       </c>
@@ -29279,8 +29573,11 @@
       <c r="C403" s="37" t="s">
         <v>2595</v>
       </c>
-    </row>
-    <row r="404" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D403" t="s">
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A404" s="16" t="s">
         <v>2589</v>
       </c>
@@ -29290,8 +29587,11 @@
       <c r="C404" s="37" t="s">
         <v>2596</v>
       </c>
-    </row>
-    <row r="405" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D404" t="s">
+        <v>2789</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A405" s="16" t="s">
         <v>2590</v>
       </c>
@@ -29301,8 +29601,11 @@
       <c r="C405" s="37" t="s">
         <v>2597</v>
       </c>
-    </row>
-    <row r="406" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D405" t="s">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A406" s="16" t="s">
         <v>2591</v>
       </c>
@@ -29312,8 +29615,11 @@
       <c r="C406" s="37" t="s">
         <v>2598</v>
       </c>
-    </row>
-    <row r="407" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D406" t="s">
+        <v>2791</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A407" s="16" t="s">
         <v>2592</v>
       </c>
@@ -29323,8 +29629,11 @@
       <c r="C407" s="37" t="s">
         <v>2599</v>
       </c>
-    </row>
-    <row r="408" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D407" t="s">
+        <v>2792</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A408" s="16" t="s">
         <v>2593</v>
       </c>
@@ -29334,8 +29643,11 @@
       <c r="C408" s="37" t="s">
         <v>2600</v>
       </c>
-    </row>
-    <row r="409" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D408" t="s">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A409" s="16" t="s">
         <v>2594</v>
       </c>
@@ -29345,8 +29657,11 @@
       <c r="C409" s="37" t="s">
         <v>2601</v>
       </c>
-    </row>
-    <row r="410" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D409" t="s">
+        <v>2794</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A410" s="16" t="s">
         <v>2602</v>
       </c>
@@ -29356,8 +29671,11 @@
       <c r="C410" s="37" t="s">
         <v>2623</v>
       </c>
-    </row>
-    <row r="411" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D410" t="s">
+        <v>2795</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A411" s="16" t="s">
         <v>2603</v>
       </c>
@@ -29367,8 +29685,11 @@
       <c r="C411" s="37" t="s">
         <v>2624</v>
       </c>
-    </row>
-    <row r="412" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D411" t="s">
+        <v>2796</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A412" s="16" t="s">
         <v>2604</v>
       </c>
@@ -29378,8 +29699,11 @@
       <c r="C412" s="37" t="s">
         <v>2625</v>
       </c>
-    </row>
-    <row r="413" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D412" t="s">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A413" s="16" t="s">
         <v>2605</v>
       </c>
@@ -29389,8 +29713,11 @@
       <c r="C413" s="37" t="s">
         <v>2626</v>
       </c>
-    </row>
-    <row r="414" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D413" t="s">
+        <v>2798</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A414" s="16" t="s">
         <v>2606</v>
       </c>
@@ -29400,8 +29727,11 @@
       <c r="C414" s="37" t="s">
         <v>2627</v>
       </c>
-    </row>
-    <row r="415" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D414" t="s">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A415" s="16" t="s">
         <v>2607</v>
       </c>
@@ -29411,8 +29741,11 @@
       <c r="C415" s="37" t="s">
         <v>2628</v>
       </c>
-    </row>
-    <row r="416" spans="1:3" ht="16.899999999999999" customHeight="1">
+      <c r="D415" t="s">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A416" s="16" t="s">
         <v>2608</v>
       </c>
@@ -29421,6 +29754,9 @@
       </c>
       <c r="C416" s="37" t="s">
         <v>2629</v>
+      </c>
+      <c r="D416" t="s">
+        <v>2801</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="16.899999999999999" customHeight="1">
@@ -29433,6 +29769,9 @@
       <c r="C417" s="37" t="s">
         <v>2623</v>
       </c>
+      <c r="D417" t="s">
+        <v>2802</v>
+      </c>
     </row>
     <row r="418" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A418" s="16" t="s">
@@ -29444,6 +29783,9 @@
       <c r="C418" s="37" t="s">
         <v>2624</v>
       </c>
+      <c r="D418" t="s">
+        <v>2803</v>
+      </c>
     </row>
     <row r="419" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A419" s="16" t="s">
@@ -29455,6 +29797,9 @@
       <c r="C419" s="37" t="s">
         <v>2625</v>
       </c>
+      <c r="D419" t="s">
+        <v>2804</v>
+      </c>
     </row>
     <row r="420" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A420" s="16" t="s">
@@ -29466,6 +29811,9 @@
       <c r="C420" s="37" t="s">
         <v>2626</v>
       </c>
+      <c r="D420" t="s">
+        <v>2805</v>
+      </c>
     </row>
     <row r="421" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A421" s="16" t="s">
@@ -29477,6 +29825,9 @@
       <c r="C421" s="37" t="s">
         <v>2627</v>
       </c>
+      <c r="D421" t="s">
+        <v>2806</v>
+      </c>
     </row>
     <row r="422" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A422" s="16" t="s">
@@ -29488,6 +29839,9 @@
       <c r="C422" s="37" t="s">
         <v>2628</v>
       </c>
+      <c r="D422" t="s">
+        <v>2807</v>
+      </c>
     </row>
     <row r="423" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A423" s="16" t="s">
@@ -29499,6 +29853,9 @@
       <c r="C423" s="37" t="s">
         <v>2629</v>
       </c>
+      <c r="D423" t="s">
+        <v>2808</v>
+      </c>
     </row>
     <row r="424" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A424" s="16" t="s">
@@ -29510,6 +29867,9 @@
       <c r="C424" s="37" t="s">
         <v>2623</v>
       </c>
+      <c r="D424" t="s">
+        <v>2809</v>
+      </c>
     </row>
     <row r="425" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A425" s="16" t="s">
@@ -29521,6 +29881,9 @@
       <c r="C425" s="37" t="s">
         <v>2624</v>
       </c>
+      <c r="D425" t="s">
+        <v>2810</v>
+      </c>
     </row>
     <row r="426" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A426" s="16" t="s">
@@ -29532,6 +29895,9 @@
       <c r="C426" s="37" t="s">
         <v>2625</v>
       </c>
+      <c r="D426" t="s">
+        <v>2811</v>
+      </c>
     </row>
     <row r="427" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A427" s="16" t="s">
@@ -29543,6 +29909,9 @@
       <c r="C427" s="37" t="s">
         <v>2626</v>
       </c>
+      <c r="D427" t="s">
+        <v>2812</v>
+      </c>
     </row>
     <row r="428" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A428" s="16" t="s">
@@ -29554,6 +29923,9 @@
       <c r="C428" s="37" t="s">
         <v>2627</v>
       </c>
+      <c r="D428" t="s">
+        <v>2813</v>
+      </c>
     </row>
     <row r="429" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A429" s="16" t="s">
@@ -29565,6 +29937,9 @@
       <c r="C429" s="37" t="s">
         <v>2628</v>
       </c>
+      <c r="D429" t="s">
+        <v>2814</v>
+      </c>
     </row>
     <row r="430" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A430" s="16" t="s">
@@ -29575,6 +29950,9 @@
       </c>
       <c r="C430" s="37" t="s">
         <v>2629</v>
+      </c>
+      <c r="D430" t="s">
+        <v>2815</v>
       </c>
     </row>
     <row r="431" spans="1:4">

</xml_diff>

<commit_message>
Added molar height structure terms, fixed incisor structure terms
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94094DA5-739A-4A88-8A9F-D1251E385400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E99C7EB-2B0B-4436-8ECB-E0D048C8EF83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
   <sheets>
     <sheet name="To Dos" sheetId="4" r:id="rId1"/>
@@ -79,28 +79,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={763FEFB1-51CA-4FC1-A6F7-E523DCC18069}</author>
-  </authors>
-  <commentList>
-    <comment ref="C305" authorId="0" shapeId="0" xr:uid="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Not sure if this needs a term other than 'occlusal surface'?
-Reply:
-    change to just 'tooth crown'</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5483" uniqueCount="2816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5486" uniqueCount="2816">
   <si>
     <t>Status</t>
   </si>
@@ -6753,27 +6733,6 @@
     <t>'occlusal surface' and ('part of' some 'lower deciduous premolar 5')</t>
   </si>
   <si>
-    <t>'occlusal surface' and ('part of' some 'canine tooth')</t>
-  </si>
-  <si>
-    <t>'occlusal surface' and ('part of' some 'upper canine 1')</t>
-  </si>
-  <si>
-    <t>'occlusal surface' and ('part of' some 'lower canine tooth')</t>
-  </si>
-  <si>
-    <t>'occlusal surface' and ('part of' some 'upper secondary canine tooth')</t>
-  </si>
-  <si>
-    <t>'occlusal surface' and ('part of' some 'upper primary canine tooth')</t>
-  </si>
-  <si>
-    <t>'occlusal surface' and ('part of' some 'lower secondary canine tooth')</t>
-  </si>
-  <si>
-    <t>'occlusal surface' and ('part of' some 'lower primary canine tooth')</t>
-  </si>
-  <si>
     <t>line along upper-lower axis of canine tooth</t>
   </si>
   <si>
@@ -6795,27 +6754,6 @@
     <t>Lower primary canine crown height</t>
   </si>
   <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown' ) and ('part of' some 'upper canine 1')</t>
-  </si>
-  <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown') and ('part of' some 'canine tooth')</t>
-  </si>
-  <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown' ) and ('part of' some 'lower canine tooth')</t>
-  </si>
-  <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown' ) and ('part of' some 'upper secondary canine tooth')</t>
-  </si>
-  <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown' ) and ('part of' some 'upper primary canine tooth')</t>
-  </si>
-  <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown' ) and ('part of' some 'lower secondary canine tooth')</t>
-  </si>
-  <si>
-    <t>occlusal surface' and ('part of' some 'tooth crown' ) and ('part of' some 'lower primary canine tooth')</t>
-  </si>
-  <si>
     <t>line along upper-lower axis of upper canine tooth</t>
   </si>
   <si>
@@ -6876,21 +6814,6 @@
     <t>Lower primary molar 2 crown height</t>
   </si>
   <si>
-    <t>molar tooth 2</t>
-  </si>
-  <si>
-    <t>upper second secondary molar tooth</t>
-  </si>
-  <si>
-    <t>upper second primary molar tooth</t>
-  </si>
-  <si>
-    <t>lower second secondary molar tooth</t>
-  </si>
-  <si>
-    <t>lower second primary molar tooth</t>
-  </si>
-  <si>
     <t>upper molar 1-2 length</t>
   </si>
   <si>
@@ -7230,12 +7153,6 @@
     <t>line along upper-lower axis of lower molar 1</t>
   </si>
   <si>
-    <t>linotalong upper-lower axis second molar too</t>
-  </si>
-  <si>
-    <t>linrialong upper-lower axis second molar too</t>
-  </si>
-  <si>
     <t>line along upper-lower axis of upper first primary molar tooth</t>
   </si>
   <si>
@@ -7419,24 +7336,6 @@
     <t>line along anterior-posterior axis of lower primary canine tooth</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper central incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower central incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper central secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower central secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower central primary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper central primary incisor tooth')</t>
-  </si>
-  <si>
     <t>Incisor 1 medial-lateral diameter at base</t>
   </si>
   <si>
@@ -7704,27 +7603,6 @@
     <t>Lower primary incisor 2 crown height</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lateral incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper lateral incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper lateral secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper lateral primary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower lateral primary incisor tooth')</t>
-  </si>
-  <si>
     <t>Incisor 3 anterior-posterior diameter at base</t>
   </si>
   <si>
@@ -7788,30 +7666,6 @@
     <t>Lower primary incisor 3 crown height</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 3')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 3')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'central incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 3')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower third secondary incisor tooth') </t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper third secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper third primary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower third primary incisor tooth')</t>
-  </si>
-  <si>
     <t>Incisor 4 anterior-posterior diameter at base</t>
   </si>
   <si>
@@ -7875,27 +7729,6 @@
     <t>Lower primary incisor 4 crown height</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 4')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 4')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 4')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper fourth secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper fourth primary incisor tooth')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower fourth secondary incisor tooth') </t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower fourth primary incisor tooth')</t>
-  </si>
-  <si>
     <t>Incisor 5 anterior-posterior diameter at base</t>
   </si>
   <si>
@@ -7959,27 +7792,6 @@
     <t>Lower primary incisor 5 crown height</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 5')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 5')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 5')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper fifth secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper fifth primary incisor tooth')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower fifth secondary incisor tooth') </t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower fifth primary incisor tooth')</t>
-  </si>
-  <si>
     <t>Incisor 6 anterior-posterior diameter at base</t>
   </si>
   <si>
@@ -8043,27 +7855,6 @@
     <t>Lower primary incisor 6 crown height</t>
   </si>
   <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'incisor 6')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper incisor 6')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower incisor 6')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper sixth secondary incisor tooth')</t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'upper sixth primary incisor tooth')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">('part of' some 'tooth crown') and ('part of' some 'lower sixth secondary incisor tooth') </t>
-  </si>
-  <si>
-    <t>('part of' some 'tooth crown') and ('part of' some 'lower sixth primary incisor tooth')</t>
-  </si>
-  <si>
     <t>('part of' some ('premolar tooth' 'part of' some 'tooth row'))</t>
   </si>
   <si>
@@ -8620,6 +8411,195 @@
   </si>
   <si>
     <t>line along upper-lower axis of lower primary incisor 6</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'central incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper central incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower central incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper central secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper central primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower central secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower central primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lateral incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper lateral incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower lateral incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper lateral secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper lateral primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower lateral secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower lateral primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'incisor 3')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper incisor 3')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower incisor 3')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper third secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper third primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooth crown' and ('part of' some 'lower third secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower third primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'incisor 4')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper incisor 4')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower incisor 4')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper fourth secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper fourth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooth crown' and ('part of' some 'lower fourth secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower fourth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'incisor 5')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper incisor 5')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower incisor 5')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper fifth secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper fifth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooth crown' and ('part of' some 'lower fifth secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower fifth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'incisor 6')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper incisor 6')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower incisor 6')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper sixth secondary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper sixth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooth crown' and ('part of' some 'lower sixth secondary incisor tooth') </t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower sixth primary incisor tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower primary canine tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'canine tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper canine 1')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower canine tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper secondary canine tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper primary canine tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower secondary canine tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'molar tooth 2')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper molar 2')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower molar 2')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper second secondary molar tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower second primary molar tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'lower second secondary molar tooth')</t>
+  </si>
+  <si>
+    <t>tooth crown' and ('part of' some 'upper second primary molar tooth')</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of molar tooth 2</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper molar 2</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower molar 2</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of lower second secondary molar tooth</t>
+  </si>
+  <si>
+    <t>line along upper-lower axis of upper second primary molar tooth</t>
+  </si>
+  <si>
+    <t>line allong upper-lower axis of lower second primary molar tooth</t>
   </si>
 </sst>
 </file>
@@ -9186,17 +9166,6 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C305" dT="2021-04-23T17:10:42.70" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
-    <text>Not sure if this needs a term other than 'occlusal surface'?</text>
-  </threadedComment>
-  <threadedComment ref="C305" dT="2021-04-29T22:12:22.98" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{CFF7EBC8-2D5C-4795-8AED-B91B03DCC54D}" parentId="{763FEFB1-51CA-4FC1-A6F7-E523DCC18069}">
-    <text>change to just 'tooth crown'</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581405C8-F852-7340-B9C9-201B714E3AD5}">
   <dimension ref="A1:D25"/>
@@ -9387,7 +9356,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="B25" t="s">
-        <v>2365</v>
+        <v>2344</v>
       </c>
     </row>
   </sheetData>
@@ -9399,10 +9368,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A27AA15-0A87-AC4A-A35D-D4FB3D2ACF67}">
   <dimension ref="A1:AD500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H263" sqref="H263"/>
+      <selection pane="bottomLeft" activeCell="H267" sqref="H267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16333,7 +16302,7 @@
     <row r="212" spans="1:21">
       <c r="A212" s="39"/>
       <c r="C212" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>15</v>
@@ -16366,7 +16335,7 @@
     <row r="213" spans="1:21" s="16" customFormat="1">
       <c r="A213" s="39"/>
       <c r="C213" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E213" s="18" t="s">
         <v>343</v>
@@ -16401,7 +16370,7 @@
     <row r="214" spans="1:21" s="16" customFormat="1">
       <c r="A214" s="39"/>
       <c r="C214" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E214" s="30" t="s">
         <v>15</v>
@@ -16434,7 +16403,7 @@
     <row r="215" spans="1:21" s="16" customFormat="1">
       <c r="A215" s="39"/>
       <c r="C215" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E215" s="18" t="s">
         <v>343</v>
@@ -16469,7 +16438,7 @@
     <row r="216" spans="1:21" s="16" customFormat="1">
       <c r="A216" s="39"/>
       <c r="C216" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E216" s="18" t="s">
         <v>343</v>
@@ -16497,7 +16466,7 @@
     <row r="217" spans="1:21" s="16" customFormat="1">
       <c r="A217" s="39"/>
       <c r="C217" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E217" s="18" t="s">
         <v>343</v>
@@ -16525,7 +16494,7 @@
     <row r="218" spans="1:21" s="16" customFormat="1">
       <c r="A218" s="39"/>
       <c r="C218" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E218" s="18" t="s">
         <v>343</v>
@@ -16553,7 +16522,7 @@
     <row r="219" spans="1:21" s="16" customFormat="1">
       <c r="A219" s="39"/>
       <c r="C219" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E219" s="18" t="s">
         <v>343</v>
@@ -16581,7 +16550,7 @@
     <row r="220" spans="1:21" s="16" customFormat="1">
       <c r="A220" s="39"/>
       <c r="C220" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E220" s="18" t="s">
         <v>343</v>
@@ -16609,7 +16578,7 @@
     <row r="221" spans="1:21" s="16" customFormat="1">
       <c r="A221" s="39"/>
       <c r="C221" s="17" t="s">
-        <v>2243</v>
+        <v>2224</v>
       </c>
       <c r="E221" s="18" t="s">
         <v>343</v>
@@ -23562,76 +23531,76 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>2239</v>
+        <v>2220</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>2240</v>
+        <v>2221</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>2252</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>2241</v>
+        <v>2222</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>2242</v>
+        <v>2223</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>2253</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>2245</v>
+        <v>2226</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>2248</v>
+        <v>2229</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>2282</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>2244</v>
+        <v>2225</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>2249</v>
+        <v>2230</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>2283</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>2246</v>
+        <v>2227</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>2250</v>
+        <v>2231</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>2284</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>2247</v>
+        <v>2228</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>2251</v>
+        <v>2232</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>2285</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>2256</v>
+        <v>2237</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>2254</v>
+        <v>2235</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>2133</v>
@@ -23639,76 +23608,76 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>2257</v>
+        <v>2238</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>2255</v>
+        <v>2236</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>2252</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>2258</v>
+        <v>2239</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>2263</v>
+        <v>2244</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>2253</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>2259</v>
+        <v>2240</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>2264</v>
+        <v>2245</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>2282</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>2260</v>
+        <v>2241</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>2265</v>
+        <v>2246</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>2283</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>2261</v>
+        <v>2242</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>2266</v>
+        <v>2247</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>2284</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>2262</v>
+        <v>2243</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>2267</v>
+        <v>2248</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>2285</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>2663</v>
+        <v>2600</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>2666</v>
+        <v>2603</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>2133</v>
@@ -23716,134 +23685,134 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>2664</v>
+        <v>2601</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>2667</v>
+        <v>2604</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>2252</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>2665</v>
+        <v>2602</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>2668</v>
+        <v>2605</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>2253</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>2268</v>
+        <v>2249</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>2254</v>
+        <v>2235</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>2269</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>2270</v>
+        <v>2251</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>2255</v>
+        <v>2236</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>2276</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>2271</v>
+        <v>2252</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>2263</v>
+        <v>2244</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>2277</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>2272</v>
+        <v>2253</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>2264</v>
+        <v>2245</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>2278</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>2273</v>
+        <v>2254</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>2265</v>
+        <v>2246</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>2279</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>2274</v>
+        <v>2255</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>2266</v>
+        <v>2247</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>2280</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>2275</v>
+        <v>2256</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>2267</v>
+        <v>2248</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>2281</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>2286</v>
+        <v>2267</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>2337</v>
+        <v>2318</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>2289</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="38" t="s">
-        <v>2287</v>
+        <v>2268</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>2338</v>
+        <v>2319</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>2290</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>2288</v>
+        <v>2269</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>2339</v>
+        <v>2320</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>2291</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -23852,24 +23821,24 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="31" t="s">
-        <v>2292</v>
+        <v>2273</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>2293</v>
+        <v>2274</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>2294</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="22" t="s">
-        <v>2336</v>
+        <v>2317</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>2295</v>
+        <v>2276</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>2296</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -23877,20 +23846,20 @@
         <v>1013</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>2359</v>
+        <v>2338</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>2360</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>2369</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>2370</v>
+        <v>2349</v>
       </c>
     </row>
   </sheetData>
@@ -23900,11 +23869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01658F34-4982-8840-AF22-6E6480DB069B}">
   <dimension ref="A1:D472"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
@@ -26117,100 +26086,100 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>2220</v>
+        <v>2206</v>
       </c>
       <c r="B151" t="s">
         <v>2130</v>
       </c>
-      <c r="C151" s="32" t="s">
-        <v>2343</v>
+      <c r="C151" s="37" t="s">
+        <v>2324</v>
       </c>
       <c r="D151" s="37" t="s">
-        <v>2349</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>2221</v>
+        <v>2207</v>
       </c>
       <c r="B152" t="s">
         <v>2130</v>
       </c>
-      <c r="C152" s="32" t="s">
-        <v>2342</v>
+      <c r="C152" s="37" t="s">
+        <v>2323</v>
       </c>
       <c r="D152" t="s">
-        <v>2350</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>2222</v>
+        <v>2208</v>
       </c>
       <c r="B153" t="s">
         <v>2130</v>
       </c>
-      <c r="C153" s="32" t="s">
-        <v>2344</v>
+      <c r="C153" s="37" t="s">
+        <v>2325</v>
       </c>
       <c r="D153" t="s">
-        <v>2351</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>2223</v>
+        <v>2209</v>
       </c>
       <c r="B154" t="s">
         <v>2130</v>
       </c>
-      <c r="C154" s="32" t="s">
-        <v>2345</v>
+      <c r="C154" s="37" t="s">
+        <v>2326</v>
       </c>
       <c r="D154" t="s">
-        <v>2355</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>2224</v>
+        <v>2210</v>
       </c>
       <c r="B155" t="s">
         <v>2130</v>
       </c>
-      <c r="C155" s="32" t="s">
-        <v>2346</v>
+      <c r="C155" s="37" t="s">
+        <v>2327</v>
       </c>
       <c r="D155" t="s">
-        <v>2354</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>2225</v>
+        <v>2211</v>
       </c>
       <c r="B156" t="s">
         <v>2130</v>
       </c>
-      <c r="C156" s="32" t="s">
-        <v>2347</v>
+      <c r="C156" s="37" t="s">
+        <v>2328</v>
       </c>
       <c r="D156" t="s">
-        <v>2356</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>2226</v>
+        <v>2212</v>
       </c>
       <c r="B157" t="s">
         <v>2130</v>
       </c>
-      <c r="C157" s="32" t="s">
-        <v>2348</v>
+      <c r="C157" s="37" t="s">
+        <v>2329</v>
       </c>
       <c r="D157" t="s">
-        <v>2357</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -26411,91 +26380,100 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>2227</v>
+        <v>2213</v>
       </c>
       <c r="B172" t="s">
         <v>2130</v>
       </c>
-      <c r="C172" s="32" t="s">
-        <v>2234</v>
+      <c r="C172" s="37" t="s">
+        <v>2802</v>
+      </c>
+      <c r="D172" t="s">
+        <v>2809</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>2229</v>
+        <v>2215</v>
       </c>
       <c r="B173" t="s">
         <v>2130</v>
       </c>
-      <c r="C173" s="32" t="s">
-        <v>1870</v>
+      <c r="C173" s="37" t="s">
+        <v>2803</v>
+      </c>
+      <c r="D173" t="s">
+        <v>2810</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>2228</v>
+        <v>2214</v>
       </c>
       <c r="B174" t="s">
         <v>2130</v>
       </c>
-      <c r="C174" s="32" t="s">
-        <v>1873</v>
+      <c r="C174" s="37" t="s">
+        <v>2804</v>
+      </c>
+      <c r="D174" t="s">
+        <v>2811</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>2230</v>
+        <v>2216</v>
       </c>
       <c r="B175" t="s">
         <v>2130</v>
       </c>
-      <c r="C175" s="32" t="s">
-        <v>2235</v>
+      <c r="C175" s="37" t="s">
+        <v>2805</v>
       </c>
       <c r="D175" t="s">
-        <v>2352</v>
+        <v>2812</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>2231</v>
+        <v>2217</v>
       </c>
       <c r="B176" t="s">
         <v>2130</v>
       </c>
-      <c r="C176" s="32" t="s">
-        <v>2236</v>
+      <c r="C176" s="37" t="s">
+        <v>2808</v>
       </c>
       <c r="D176" t="s">
-        <v>2353</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>2232</v>
+        <v>2218</v>
       </c>
       <c r="B177" t="s">
         <v>2130</v>
       </c>
-      <c r="C177" s="32" t="s">
-        <v>2237</v>
+      <c r="C177" s="37" t="s">
+        <v>2807</v>
       </c>
       <c r="D177" t="s">
-        <v>2352</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>2233</v>
+        <v>2219</v>
       </c>
       <c r="B178" t="s">
         <v>2130</v>
       </c>
-      <c r="C178" s="32" t="s">
-        <v>2238</v>
+      <c r="C178" s="37" t="s">
+        <v>2806</v>
       </c>
       <c r="D178" t="s">
-        <v>2353</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -26570,13 +26548,13 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>2340</v>
+        <v>2321</v>
       </c>
       <c r="B184" t="s">
         <v>108</v>
       </c>
       <c r="C184" s="22" t="s">
-        <v>2341</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -26735,72 +26713,72 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>2297</v>
+        <v>2278</v>
       </c>
       <c r="B201" t="s">
         <v>112</v>
       </c>
       <c r="C201" s="22" t="s">
-        <v>2302</v>
+        <v>2283</v>
       </c>
       <c r="D201" t="s">
-        <v>2330</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>2298</v>
+        <v>2279</v>
       </c>
       <c r="B202" t="s">
         <v>112</v>
       </c>
       <c r="C202" s="22" t="s">
-        <v>2328</v>
+        <v>2309</v>
       </c>
       <c r="D202" t="s">
-        <v>2331</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>2299</v>
+        <v>2280</v>
       </c>
       <c r="B203" t="s">
         <v>112</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>2329</v>
+        <v>2310</v>
       </c>
       <c r="D203" t="s">
-        <v>2332</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>2300</v>
+        <v>2281</v>
       </c>
       <c r="B204" t="s">
         <v>108</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>2302</v>
+        <v>2283</v>
       </c>
       <c r="D204" t="s">
-        <v>2333</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>2301</v>
+        <v>2282</v>
       </c>
       <c r="B205" t="s">
         <v>108</v>
       </c>
       <c r="C205" s="22" t="s">
-        <v>2328</v>
+        <v>2309</v>
       </c>
       <c r="D205" t="s">
-        <v>2334</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -26811,10 +26789,10 @@
         <v>108</v>
       </c>
       <c r="C206" s="22" t="s">
-        <v>2329</v>
+        <v>2310</v>
       </c>
       <c r="D206" t="s">
-        <v>2335</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -27407,100 +27385,100 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>2669</v>
+        <v>2606</v>
       </c>
       <c r="B249" t="s">
         <v>2130</v>
       </c>
       <c r="C249" s="22" t="s">
-        <v>2676</v>
+        <v>2613</v>
       </c>
       <c r="D249" t="s">
-        <v>2683</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>2670</v>
+        <v>2607</v>
       </c>
       <c r="B250" t="s">
         <v>2130</v>
       </c>
       <c r="C250" s="22" t="s">
-        <v>2678</v>
+        <v>2615</v>
       </c>
       <c r="D250" t="s">
-        <v>2684</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>2671</v>
+        <v>2608</v>
       </c>
       <c r="B251" t="s">
         <v>2130</v>
       </c>
       <c r="C251" s="22" t="s">
-        <v>2677</v>
+        <v>2614</v>
       </c>
       <c r="D251" t="s">
-        <v>2685</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>2672</v>
+        <v>2609</v>
       </c>
       <c r="B252" t="s">
         <v>2130</v>
       </c>
       <c r="C252" s="22" t="s">
-        <v>2679</v>
+        <v>2616</v>
       </c>
       <c r="D252" t="s">
-        <v>2686</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>2673</v>
+        <v>2610</v>
       </c>
       <c r="B253" t="s">
         <v>2130</v>
       </c>
       <c r="C253" s="22" t="s">
-        <v>2680</v>
+        <v>2617</v>
       </c>
       <c r="D253" t="s">
-        <v>2689</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>2674</v>
+        <v>2611</v>
       </c>
       <c r="B254" t="s">
         <v>2130</v>
       </c>
       <c r="C254" s="22" t="s">
-        <v>2681</v>
+        <v>2618</v>
       </c>
       <c r="D254" t="s">
-        <v>2687</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>2675</v>
+        <v>2612</v>
       </c>
       <c r="B255" t="s">
         <v>2130</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>2682</v>
+        <v>2619</v>
       </c>
       <c r="D255" t="s">
-        <v>2688</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -27799,7 +27777,7 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>2655</v>
+        <v>2592</v>
       </c>
       <c r="B277" t="s">
         <v>112</v>
@@ -27813,7 +27791,7 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>2656</v>
+        <v>2593</v>
       </c>
       <c r="B278" t="s">
         <v>112</v>
@@ -27827,7 +27805,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>2657</v>
+        <v>2594</v>
       </c>
       <c r="B279" t="s">
         <v>112</v>
@@ -27841,7 +27819,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>2658</v>
+        <v>2595</v>
       </c>
       <c r="B280" t="s">
         <v>112</v>
@@ -27855,7 +27833,7 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>2659</v>
+        <v>2596</v>
       </c>
       <c r="B281" t="s">
         <v>112</v>
@@ -27869,7 +27847,7 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>2660</v>
+        <v>2597</v>
       </c>
       <c r="B282" t="s">
         <v>112</v>
@@ -27883,7 +27861,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>2661</v>
+        <v>2598</v>
       </c>
       <c r="B283" t="s">
         <v>112</v>
@@ -27896,196 +27874,196 @@
       </c>
     </row>
     <row r="284" spans="1:4">
-      <c r="A284" s="31" t="s">
+      <c r="A284" s="16" t="s">
         <v>2104</v>
       </c>
       <c r="B284" t="s">
         <v>112</v>
       </c>
-      <c r="C284" s="16" t="s">
-        <v>2193</v>
+      <c r="C284" s="37" t="s">
+        <v>2796</v>
       </c>
       <c r="D284" t="s">
         <v>2112</v>
       </c>
     </row>
     <row r="285" spans="1:4">
-      <c r="A285" s="31" t="s">
+      <c r="A285" s="16" t="s">
         <v>2105</v>
       </c>
       <c r="B285" t="s">
         <v>112</v>
       </c>
-      <c r="C285" s="16" t="s">
-        <v>2194</v>
+      <c r="C285" s="37" t="s">
+        <v>2797</v>
       </c>
       <c r="D285" t="s">
         <v>2113</v>
       </c>
     </row>
     <row r="286" spans="1:4">
-      <c r="A286" s="31" t="s">
+      <c r="A286" s="16" t="s">
         <v>2106</v>
       </c>
       <c r="B286" t="s">
         <v>112</v>
       </c>
-      <c r="C286" s="16" t="s">
-        <v>2195</v>
+      <c r="C286" s="37" t="s">
+        <v>2798</v>
       </c>
       <c r="D286" t="s">
         <v>2114</v>
       </c>
     </row>
     <row r="287" spans="1:4">
-      <c r="A287" s="31" t="s">
+      <c r="A287" s="16" t="s">
         <v>2107</v>
       </c>
       <c r="B287" t="s">
         <v>112</v>
       </c>
-      <c r="C287" s="16" t="s">
-        <v>2196</v>
+      <c r="C287" s="37" t="s">
+        <v>2799</v>
       </c>
       <c r="D287" t="s">
-        <v>2411</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="288" spans="1:4">
-      <c r="A288" s="31" t="s">
+      <c r="A288" s="16" t="s">
         <v>2108</v>
       </c>
       <c r="B288" t="s">
         <v>112</v>
       </c>
-      <c r="C288" s="16" t="s">
-        <v>2197</v>
+      <c r="C288" s="37" t="s">
+        <v>2800</v>
       </c>
       <c r="D288" t="s">
-        <v>2412</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="289" spans="1:4">
-      <c r="A289" s="31" t="s">
+      <c r="A289" s="16" t="s">
         <v>2109</v>
       </c>
       <c r="B289" t="s">
         <v>112</v>
       </c>
-      <c r="C289" s="16" t="s">
-        <v>2198</v>
+      <c r="C289" s="37" t="s">
+        <v>2801</v>
       </c>
       <c r="D289" t="s">
-        <v>2413</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="290" spans="1:4">
-      <c r="A290" s="31" t="s">
+      <c r="A290" s="16" t="s">
         <v>2110</v>
       </c>
       <c r="B290" t="s">
         <v>112</v>
       </c>
-      <c r="C290" s="16" t="s">
-        <v>2199</v>
+      <c r="C290" s="37" t="s">
+        <v>2795</v>
       </c>
       <c r="D290" t="s">
-        <v>2414</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="291" spans="1:4">
-      <c r="A291" s="31" t="s">
+      <c r="A291" s="16" t="s">
         <v>2115</v>
       </c>
       <c r="B291" t="s">
         <v>108</v>
       </c>
-      <c r="C291" s="16" t="s">
-        <v>2193</v>
+      <c r="C291" s="37" t="s">
+        <v>2796</v>
       </c>
       <c r="D291" t="s">
         <v>2122</v>
       </c>
     </row>
     <row r="292" spans="1:4">
-      <c r="A292" s="31" t="s">
+      <c r="A292" s="16" t="s">
         <v>2116</v>
       </c>
       <c r="B292" t="s">
         <v>108</v>
       </c>
-      <c r="C292" s="16" t="s">
-        <v>2194</v>
+      <c r="C292" s="37" t="s">
+        <v>2797</v>
       </c>
       <c r="D292" t="s">
         <v>2123</v>
       </c>
     </row>
     <row r="293" spans="1:4">
-      <c r="A293" s="31" t="s">
+      <c r="A293" s="16" t="s">
         <v>2117</v>
       </c>
       <c r="B293" t="s">
         <v>108</v>
       </c>
-      <c r="C293" s="16" t="s">
-        <v>2195</v>
+      <c r="C293" s="37" t="s">
+        <v>2798</v>
       </c>
       <c r="D293" t="s">
         <v>2124</v>
       </c>
     </row>
     <row r="294" spans="1:4">
-      <c r="A294" s="31" t="s">
+      <c r="A294" s="16" t="s">
         <v>2118</v>
       </c>
       <c r="B294" t="s">
         <v>108</v>
       </c>
-      <c r="C294" t="s">
-        <v>2196</v>
+      <c r="C294" s="37" t="s">
+        <v>2799</v>
       </c>
       <c r="D294" t="s">
         <v>2125</v>
       </c>
     </row>
     <row r="295" spans="1:4">
-      <c r="A295" s="31" t="s">
+      <c r="A295" s="16" t="s">
         <v>2119</v>
       </c>
       <c r="B295" t="s">
         <v>108</v>
       </c>
-      <c r="C295" t="s">
-        <v>2197</v>
+      <c r="C295" s="37" t="s">
+        <v>2800</v>
       </c>
       <c r="D295" t="s">
         <v>2126</v>
       </c>
     </row>
     <row r="296" spans="1:4">
-      <c r="A296" s="31" t="s">
+      <c r="A296" s="16" t="s">
         <v>2120</v>
       </c>
       <c r="B296" t="s">
         <v>108</v>
       </c>
-      <c r="C296" t="s">
-        <v>2198</v>
+      <c r="C296" s="37" t="s">
+        <v>2801</v>
       </c>
       <c r="D296" t="s">
         <v>2127</v>
       </c>
     </row>
     <row r="297" spans="1:4">
-      <c r="A297" s="31" t="s">
+      <c r="A297" s="16" t="s">
         <v>2121</v>
       </c>
       <c r="B297" t="s">
         <v>108</v>
       </c>
-      <c r="C297" t="s">
-        <v>2199</v>
+      <c r="C297" s="37" t="s">
+        <v>2795</v>
       </c>
       <c r="D297" t="s">
         <v>2128</v>
@@ -28098,2032 +28076,2032 @@
       <c r="B298" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C298" s="32" t="s">
-        <v>2208</v>
+      <c r="C298" s="37" t="s">
+        <v>2796</v>
       </c>
       <c r="D298" t="s">
-        <v>2200</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="16" t="s">
-        <v>2201</v>
+        <v>2194</v>
       </c>
       <c r="B299" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C299" s="32" t="s">
-        <v>2207</v>
+      <c r="C299" s="37" t="s">
+        <v>2797</v>
       </c>
       <c r="D299" t="s">
-        <v>2214</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="16" t="s">
-        <v>2202</v>
+        <v>2195</v>
       </c>
       <c r="B300" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C300" s="32" t="s">
-        <v>2209</v>
+      <c r="C300" s="37" t="s">
+        <v>2798</v>
       </c>
       <c r="D300" t="s">
-        <v>2215</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="16" t="s">
-        <v>2203</v>
+        <v>2196</v>
       </c>
       <c r="B301" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C301" s="32" t="s">
-        <v>2210</v>
+      <c r="C301" s="37" t="s">
+        <v>2799</v>
       </c>
       <c r="D301" t="s">
-        <v>2216</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="16" t="s">
-        <v>2204</v>
+        <v>2197</v>
       </c>
       <c r="B302" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C302" s="32" t="s">
-        <v>2211</v>
+      <c r="C302" s="37" t="s">
+        <v>2800</v>
       </c>
       <c r="D302" t="s">
-        <v>2218</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="16" t="s">
-        <v>2205</v>
+        <v>2198</v>
       </c>
       <c r="B303" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C303" s="32" t="s">
-        <v>2212</v>
+      <c r="C303" s="37" t="s">
+        <v>2801</v>
       </c>
       <c r="D303" t="s">
-        <v>2217</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="16" t="s">
-        <v>2206</v>
+        <v>2199</v>
       </c>
       <c r="B304" s="16" t="s">
         <v>2130</v>
       </c>
-      <c r="C304" s="32" t="s">
-        <v>2213</v>
+      <c r="C304" s="37" t="s">
+        <v>2795</v>
       </c>
       <c r="D304" t="s">
-        <v>2219</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="305" spans="1:4">
       <c r="A305" s="16" t="s">
-        <v>2358</v>
+        <v>2337</v>
       </c>
       <c r="B305" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C305" s="37" t="s">
-        <v>2540</v>
+        <v>2753</v>
       </c>
       <c r="D305" t="s">
-        <v>2690</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="306" spans="1:4">
       <c r="A306" s="16" t="s">
-        <v>2405</v>
+        <v>2384</v>
       </c>
       <c r="B306" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C306" s="37" t="s">
-        <v>2415</v>
+        <v>2754</v>
       </c>
       <c r="D306" t="s">
-        <v>2693</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A307" s="16" t="s">
-        <v>2406</v>
+        <v>2385</v>
       </c>
       <c r="B307" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C307" s="37" t="s">
-        <v>2416</v>
+        <v>2755</v>
       </c>
       <c r="D307" t="s">
-        <v>2694</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A308" s="16" t="s">
-        <v>2407</v>
+        <v>2386</v>
       </c>
       <c r="B308" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C308" s="37" t="s">
-        <v>2417</v>
+        <v>2756</v>
       </c>
       <c r="D308" t="s">
-        <v>2699</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A309" s="16" t="s">
-        <v>2408</v>
+        <v>2387</v>
       </c>
       <c r="B309" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C309" s="37" t="s">
-        <v>2420</v>
+        <v>2757</v>
       </c>
       <c r="D309" t="s">
-        <v>2700</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A310" s="16" t="s">
-        <v>2409</v>
+        <v>2388</v>
       </c>
       <c r="B310" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C310" s="37" t="s">
-        <v>2418</v>
+        <v>2758</v>
       </c>
       <c r="D310" t="s">
-        <v>2701</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A311" s="16" t="s">
-        <v>2410</v>
+        <v>2389</v>
       </c>
       <c r="B311" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C311" s="37" t="s">
-        <v>2419</v>
+        <v>2759</v>
       </c>
       <c r="D311" t="s">
-        <v>2702</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A312" s="16" t="s">
-        <v>2421</v>
+        <v>2394</v>
       </c>
       <c r="B312" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C312" s="37" t="s">
-        <v>2540</v>
+        <v>2753</v>
       </c>
       <c r="D312" t="s">
-        <v>2691</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A313" s="16" t="s">
-        <v>2477</v>
+        <v>2450</v>
       </c>
       <c r="B313" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C313" s="37" t="s">
-        <v>2415</v>
+        <v>2754</v>
       </c>
       <c r="D313" t="s">
-        <v>2695</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A314" s="16" t="s">
-        <v>2478</v>
+        <v>2451</v>
       </c>
       <c r="B314" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C314" s="37" t="s">
-        <v>2416</v>
+        <v>2755</v>
       </c>
       <c r="D314" t="s">
-        <v>2696</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A315" s="16" t="s">
-        <v>2479</v>
+        <v>2452</v>
       </c>
       <c r="B315" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C315" s="37" t="s">
-        <v>2417</v>
+        <v>2756</v>
       </c>
       <c r="D315" t="s">
-        <v>2703</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A316" s="16" t="s">
-        <v>2480</v>
+        <v>2453</v>
       </c>
       <c r="B316" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C316" s="37" t="s">
-        <v>2420</v>
+        <v>2757</v>
       </c>
       <c r="D316" t="s">
-        <v>2704</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A317" s="16" t="s">
-        <v>2481</v>
+        <v>2454</v>
       </c>
       <c r="B317" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C317" s="37" t="s">
-        <v>2418</v>
+        <v>2758</v>
       </c>
       <c r="D317" t="s">
-        <v>2705</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A318" s="16" t="s">
-        <v>2482</v>
+        <v>2455</v>
       </c>
       <c r="B318" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C318" s="37" t="s">
-        <v>2419</v>
+        <v>2759</v>
       </c>
       <c r="D318" t="s">
-        <v>2706</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A319" s="16" t="s">
-        <v>2476</v>
+        <v>2449</v>
       </c>
       <c r="B319" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C319" s="37" t="s">
-        <v>2540</v>
+        <v>2753</v>
       </c>
       <c r="D319" t="s">
-        <v>2707</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A320" s="16" t="s">
-        <v>2483</v>
+        <v>2456</v>
       </c>
       <c r="B320" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C320" s="37" t="s">
-        <v>2415</v>
+        <v>2754</v>
       </c>
       <c r="D320" t="s">
-        <v>2708</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A321" s="16" t="s">
-        <v>2484</v>
+        <v>2457</v>
       </c>
       <c r="B321" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C321" s="37" t="s">
-        <v>2416</v>
+        <v>2755</v>
       </c>
       <c r="D321" t="s">
-        <v>2709</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A322" s="16" t="s">
-        <v>2485</v>
+        <v>2458</v>
       </c>
       <c r="B322" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C322" s="37" t="s">
-        <v>2417</v>
+        <v>2756</v>
       </c>
       <c r="D322" t="s">
-        <v>2710</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A323" s="16" t="s">
-        <v>2486</v>
+        <v>2459</v>
       </c>
       <c r="B323" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C323" s="37" t="s">
-        <v>2420</v>
+        <v>2757</v>
       </c>
       <c r="D323" t="s">
-        <v>2711</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A324" s="16" t="s">
-        <v>2487</v>
+        <v>2460</v>
       </c>
       <c r="B324" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C324" s="37" t="s">
-        <v>2418</v>
+        <v>2758</v>
       </c>
       <c r="D324" t="s">
-        <v>2712</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="325" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A325" s="16" t="s">
-        <v>2488</v>
+        <v>2461</v>
       </c>
       <c r="B325" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C325" s="37" t="s">
-        <v>2419</v>
+        <v>2759</v>
       </c>
       <c r="D325" t="s">
-        <v>2713</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="326" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A326" s="16" t="s">
-        <v>2489</v>
+        <v>2462</v>
       </c>
       <c r="B326" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C326" s="37" t="s">
-        <v>2510</v>
+        <v>2760</v>
       </c>
       <c r="D326" t="s">
-        <v>2692</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A327" s="16" t="s">
-        <v>2490</v>
+        <v>2463</v>
       </c>
       <c r="B327" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C327" s="37" t="s">
-        <v>2511</v>
+        <v>2761</v>
       </c>
       <c r="D327" t="s">
-        <v>2697</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A328" s="16" t="s">
-        <v>2491</v>
+        <v>2464</v>
       </c>
       <c r="B328" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C328" s="37" t="s">
-        <v>2512</v>
+        <v>2762</v>
       </c>
       <c r="D328" t="s">
-        <v>2698</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A329" s="16" t="s">
-        <v>2492</v>
+        <v>2465</v>
       </c>
       <c r="B329" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C329" s="37" t="s">
-        <v>2513</v>
+        <v>2763</v>
       </c>
       <c r="D329" t="s">
-        <v>2714</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A330" s="16" t="s">
-        <v>2493</v>
+        <v>2466</v>
       </c>
       <c r="B330" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C330" s="37" t="s">
-        <v>2514</v>
+        <v>2764</v>
       </c>
       <c r="D330" t="s">
-        <v>2715</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A331" s="16" t="s">
-        <v>2494</v>
+        <v>2467</v>
       </c>
       <c r="B331" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C331" s="37" t="s">
-        <v>2515</v>
+        <v>2765</v>
       </c>
       <c r="D331" t="s">
-        <v>2716</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A332" s="16" t="s">
-        <v>2495</v>
+        <v>2468</v>
       </c>
       <c r="B332" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C332" s="37" t="s">
-        <v>2516</v>
+        <v>2766</v>
       </c>
       <c r="D332" t="s">
-        <v>2717</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A333" s="16" t="s">
-        <v>2496</v>
+        <v>2469</v>
       </c>
       <c r="B333" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C333" s="37" t="s">
-        <v>2510</v>
+        <v>2760</v>
       </c>
       <c r="D333" t="s">
-        <v>2718</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A334" s="16" t="s">
-        <v>2497</v>
+        <v>2470</v>
       </c>
       <c r="B334" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C334" s="37" t="s">
-        <v>2511</v>
+        <v>2761</v>
       </c>
       <c r="D334" t="s">
-        <v>2719</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A335" s="16" t="s">
-        <v>2498</v>
+        <v>2471</v>
       </c>
       <c r="B335" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C335" s="37" t="s">
-        <v>2512</v>
+        <v>2762</v>
       </c>
       <c r="D335" t="s">
-        <v>2720</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A336" s="16" t="s">
-        <v>2499</v>
+        <v>2472</v>
       </c>
       <c r="B336" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C336" s="37" t="s">
-        <v>2513</v>
+        <v>2763</v>
       </c>
       <c r="D336" t="s">
-        <v>2721</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A337" s="16" t="s">
-        <v>2500</v>
+        <v>2473</v>
       </c>
       <c r="B337" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C337" s="37" t="s">
-        <v>2514</v>
+        <v>2764</v>
       </c>
       <c r="D337" t="s">
-        <v>2722</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A338" s="16" t="s">
-        <v>2501</v>
+        <v>2474</v>
       </c>
       <c r="B338" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C338" s="37" t="s">
-        <v>2515</v>
+        <v>2765</v>
       </c>
       <c r="D338" t="s">
-        <v>2723</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A339" s="16" t="s">
-        <v>2502</v>
+        <v>2475</v>
       </c>
       <c r="B339" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C339" s="37" t="s">
-        <v>2516</v>
+        <v>2766</v>
       </c>
       <c r="D339" t="s">
-        <v>2724</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A340" s="16" t="s">
-        <v>2503</v>
+        <v>2476</v>
       </c>
       <c r="B340" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C340" s="37" t="s">
-        <v>2510</v>
+        <v>2760</v>
       </c>
       <c r="D340" t="s">
-        <v>2725</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A341" s="16" t="s">
-        <v>2504</v>
+        <v>2477</v>
       </c>
       <c r="B341" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C341" s="37" t="s">
-        <v>2511</v>
+        <v>2761</v>
       </c>
       <c r="D341" t="s">
-        <v>2726</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A342" s="16" t="s">
-        <v>2505</v>
+        <v>2478</v>
       </c>
       <c r="B342" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C342" s="37" t="s">
-        <v>2512</v>
+        <v>2762</v>
       </c>
       <c r="D342" t="s">
-        <v>2727</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A343" s="16" t="s">
-        <v>2506</v>
+        <v>2479</v>
       </c>
       <c r="B343" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C343" s="37" t="s">
-        <v>2513</v>
+        <v>2763</v>
       </c>
       <c r="D343" t="s">
-        <v>2728</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A344" s="16" t="s">
-        <v>2507</v>
+        <v>2480</v>
       </c>
       <c r="B344" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C344" s="37" t="s">
-        <v>2514</v>
+        <v>2764</v>
       </c>
       <c r="D344" t="s">
-        <v>2729</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A345" s="16" t="s">
-        <v>2508</v>
+        <v>2481</v>
       </c>
       <c r="B345" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C345" s="37" t="s">
-        <v>2515</v>
+        <v>2765</v>
       </c>
       <c r="D345" t="s">
-        <v>2730</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A346" s="16" t="s">
-        <v>2509</v>
+        <v>2482</v>
       </c>
       <c r="B346" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C346" s="37" t="s">
-        <v>2516</v>
+        <v>2766</v>
       </c>
       <c r="D346" t="s">
-        <v>2731</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A347" s="16" t="s">
-        <v>2517</v>
+        <v>2483</v>
       </c>
       <c r="B347" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C347" s="37" t="s">
-        <v>2538</v>
+        <v>2767</v>
       </c>
       <c r="D347" t="s">
-        <v>2732</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A348" s="16" t="s">
-        <v>2518</v>
+        <v>2484</v>
       </c>
       <c r="B348" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C348" s="37" t="s">
-        <v>2541</v>
+        <v>2768</v>
       </c>
       <c r="D348" t="s">
-        <v>2733</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="349" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A349" s="16" t="s">
-        <v>2519</v>
+        <v>2485</v>
       </c>
       <c r="B349" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C349" s="37" t="s">
-        <v>2539</v>
+        <v>2769</v>
       </c>
       <c r="D349" t="s">
-        <v>2734</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A350" s="16" t="s">
-        <v>2520</v>
+        <v>2486</v>
       </c>
       <c r="B350" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C350" s="37" t="s">
-        <v>2543</v>
+        <v>2770</v>
       </c>
       <c r="D350" t="s">
-        <v>2735</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A351" s="16" t="s">
-        <v>2521</v>
+        <v>2487</v>
       </c>
       <c r="B351" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C351" s="37" t="s">
-        <v>2544</v>
+        <v>2771</v>
       </c>
       <c r="D351" t="s">
-        <v>2736</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A352" s="16" t="s">
-        <v>2522</v>
+        <v>2488</v>
       </c>
       <c r="B352" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C352" s="37" t="s">
-        <v>2542</v>
+        <v>2772</v>
       </c>
       <c r="D352" t="s">
-        <v>2737</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A353" s="16" t="s">
-        <v>2523</v>
+        <v>2489</v>
       </c>
       <c r="B353" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C353" s="37" t="s">
-        <v>2545</v>
+        <v>2773</v>
       </c>
       <c r="D353" t="s">
-        <v>2738</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A354" s="16" t="s">
-        <v>2524</v>
+        <v>2490</v>
       </c>
       <c r="B354" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C354" s="37" t="s">
-        <v>2538</v>
+        <v>2767</v>
       </c>
       <c r="D354" t="s">
-        <v>2739</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A355" s="16" t="s">
-        <v>2525</v>
+        <v>2491</v>
       </c>
       <c r="B355" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C355" s="37" t="s">
-        <v>2541</v>
+        <v>2768</v>
       </c>
       <c r="D355" t="s">
-        <v>2740</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="356" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A356" s="16" t="s">
-        <v>2526</v>
+        <v>2492</v>
       </c>
       <c r="B356" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C356" s="37" t="s">
-        <v>2539</v>
+        <v>2769</v>
       </c>
       <c r="D356" t="s">
-        <v>2741</v>
+        <v>2678</v>
       </c>
     </row>
     <row r="357" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A357" s="16" t="s">
-        <v>2527</v>
+        <v>2493</v>
       </c>
       <c r="B357" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C357" s="37" t="s">
-        <v>2543</v>
+        <v>2770</v>
       </c>
       <c r="D357" t="s">
-        <v>2742</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A358" s="16" t="s">
-        <v>2528</v>
+        <v>2494</v>
       </c>
       <c r="B358" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C358" s="37" t="s">
-        <v>2544</v>
+        <v>2771</v>
       </c>
       <c r="D358" t="s">
-        <v>2743</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="359" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A359" s="16" t="s">
-        <v>2529</v>
+        <v>2495</v>
       </c>
       <c r="B359" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C359" s="37" t="s">
-        <v>2542</v>
+        <v>2772</v>
       </c>
       <c r="D359" t="s">
-        <v>2744</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="360" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A360" s="16" t="s">
-        <v>2530</v>
+        <v>2496</v>
       </c>
       <c r="B360" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C360" s="37" t="s">
-        <v>2545</v>
+        <v>2773</v>
       </c>
       <c r="D360" t="s">
-        <v>2745</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="361" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A361" s="16" t="s">
-        <v>2531</v>
+        <v>2497</v>
       </c>
       <c r="B361" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C361" s="37" t="s">
-        <v>2538</v>
+        <v>2767</v>
       </c>
       <c r="D361" t="s">
-        <v>2746</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A362" s="16" t="s">
-        <v>2532</v>
+        <v>2498</v>
       </c>
       <c r="B362" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C362" s="37" t="s">
-        <v>2541</v>
+        <v>2768</v>
       </c>
       <c r="D362" t="s">
-        <v>2747</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A363" s="16" t="s">
-        <v>2533</v>
+        <v>2499</v>
       </c>
       <c r="B363" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C363" s="37" t="s">
-        <v>2539</v>
+        <v>2769</v>
       </c>
       <c r="D363" t="s">
-        <v>2748</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="364" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A364" s="16" t="s">
-        <v>2534</v>
+        <v>2500</v>
       </c>
       <c r="B364" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C364" s="37" t="s">
-        <v>2543</v>
+        <v>2770</v>
       </c>
       <c r="D364" t="s">
-        <v>2749</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A365" s="16" t="s">
-        <v>2535</v>
+        <v>2501</v>
       </c>
       <c r="B365" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C365" s="37" t="s">
-        <v>2544</v>
+        <v>2771</v>
       </c>
       <c r="D365" t="s">
-        <v>2750</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A366" s="16" t="s">
-        <v>2536</v>
+        <v>2502</v>
       </c>
       <c r="B366" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C366" s="37" t="s">
-        <v>2542</v>
+        <v>2772</v>
       </c>
       <c r="D366" t="s">
-        <v>2751</v>
+        <v>2688</v>
       </c>
     </row>
     <row r="367" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A367" s="16" t="s">
-        <v>2537</v>
+        <v>2503</v>
       </c>
       <c r="B367" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C367" s="37" t="s">
-        <v>2545</v>
+        <v>2773</v>
       </c>
       <c r="D367" t="s">
-        <v>2752</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A368" s="16" t="s">
-        <v>2546</v>
+        <v>2504</v>
       </c>
       <c r="B368" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C368" s="37" t="s">
-        <v>2567</v>
+        <v>2774</v>
       </c>
       <c r="D368" t="s">
-        <v>2753</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="369" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A369" s="16" t="s">
-        <v>2547</v>
+        <v>2505</v>
       </c>
       <c r="B369" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C369" s="37" t="s">
-        <v>2568</v>
+        <v>2775</v>
       </c>
       <c r="D369" t="s">
-        <v>2756</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="370" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A370" s="16" t="s">
-        <v>2548</v>
+        <v>2506</v>
       </c>
       <c r="B370" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C370" s="37" t="s">
-        <v>2569</v>
+        <v>2776</v>
       </c>
       <c r="D370" t="s">
-        <v>2761</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="371" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A371" s="16" t="s">
-        <v>2549</v>
+        <v>2507</v>
       </c>
       <c r="B371" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C371" s="37" t="s">
-        <v>2570</v>
+        <v>2777</v>
       </c>
       <c r="D371" t="s">
-        <v>2762</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="372" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A372" s="16" t="s">
-        <v>2550</v>
+        <v>2508</v>
       </c>
       <c r="B372" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C372" s="37" t="s">
-        <v>2571</v>
+        <v>2778</v>
       </c>
       <c r="D372" t="s">
-        <v>2770</v>
+        <v>2707</v>
       </c>
     </row>
     <row r="373" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A373" s="16" t="s">
-        <v>2551</v>
+        <v>2509</v>
       </c>
       <c r="B373" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C373" s="37" t="s">
-        <v>2572</v>
+        <v>2779</v>
       </c>
       <c r="D373" t="s">
-        <v>2771</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="374" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A374" s="16" t="s">
-        <v>2552</v>
+        <v>2510</v>
       </c>
       <c r="B374" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C374" s="37" t="s">
-        <v>2573</v>
+        <v>2780</v>
       </c>
       <c r="D374" t="s">
-        <v>2772</v>
+        <v>2709</v>
       </c>
     </row>
     <row r="375" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A375" s="16" t="s">
-        <v>2553</v>
+        <v>2511</v>
       </c>
       <c r="B375" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C375" s="37" t="s">
-        <v>2567</v>
+        <v>2774</v>
       </c>
       <c r="D375" t="s">
-        <v>2773</v>
+        <v>2710</v>
       </c>
     </row>
     <row r="376" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A376" s="16" t="s">
-        <v>2554</v>
+        <v>2512</v>
       </c>
       <c r="B376" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C376" s="37" t="s">
-        <v>2568</v>
+        <v>2775</v>
       </c>
       <c r="D376" t="s">
-        <v>2774</v>
+        <v>2711</v>
       </c>
     </row>
     <row r="377" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A377" s="16" t="s">
-        <v>2555</v>
+        <v>2513</v>
       </c>
       <c r="B377" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C377" s="37" t="s">
-        <v>2569</v>
+        <v>2776</v>
       </c>
       <c r="D377" t="s">
-        <v>2775</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="378" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A378" s="16" t="s">
-        <v>2556</v>
+        <v>2514</v>
       </c>
       <c r="B378" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C378" s="37" t="s">
-        <v>2570</v>
+        <v>2777</v>
       </c>
       <c r="D378" t="s">
-        <v>2776</v>
+        <v>2713</v>
       </c>
     </row>
     <row r="379" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A379" s="16" t="s">
-        <v>2557</v>
+        <v>2515</v>
       </c>
       <c r="B379" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C379" s="37" t="s">
-        <v>2571</v>
+        <v>2778</v>
       </c>
       <c r="D379" t="s">
-        <v>2777</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="380" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A380" s="16" t="s">
-        <v>2558</v>
+        <v>2516</v>
       </c>
       <c r="B380" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C380" s="37" t="s">
-        <v>2572</v>
+        <v>2779</v>
       </c>
       <c r="D380" t="s">
-        <v>2778</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="381" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A381" s="16" t="s">
-        <v>2559</v>
+        <v>2517</v>
       </c>
       <c r="B381" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C381" s="37" t="s">
-        <v>2573</v>
+        <v>2780</v>
       </c>
       <c r="D381" t="s">
-        <v>2779</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="382" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A382" s="16" t="s">
-        <v>2560</v>
+        <v>2518</v>
       </c>
       <c r="B382" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C382" s="37" t="s">
-        <v>2567</v>
+        <v>2774</v>
       </c>
       <c r="D382" t="s">
-        <v>2780</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="383" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A383" s="16" t="s">
-        <v>2561</v>
+        <v>2519</v>
       </c>
       <c r="B383" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C383" s="37" t="s">
-        <v>2568</v>
+        <v>2775</v>
       </c>
       <c r="D383" t="s">
-        <v>2781</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="384" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A384" s="16" t="s">
-        <v>2562</v>
+        <v>2520</v>
       </c>
       <c r="B384" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C384" s="37" t="s">
-        <v>2569</v>
+        <v>2776</v>
       </c>
       <c r="D384" t="s">
-        <v>2782</v>
+        <v>2719</v>
       </c>
     </row>
     <row r="385" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A385" s="16" t="s">
-        <v>2563</v>
+        <v>2521</v>
       </c>
       <c r="B385" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C385" s="37" t="s">
-        <v>2570</v>
+        <v>2777</v>
       </c>
       <c r="D385" t="s">
-        <v>2783</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="386" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A386" s="16" t="s">
-        <v>2564</v>
+        <v>2522</v>
       </c>
       <c r="B386" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C386" s="37" t="s">
-        <v>2571</v>
+        <v>2778</v>
       </c>
       <c r="D386" t="s">
-        <v>2784</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="387" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A387" s="16" t="s">
-        <v>2565</v>
+        <v>2523</v>
       </c>
       <c r="B387" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C387" s="37" t="s">
-        <v>2572</v>
+        <v>2779</v>
       </c>
       <c r="D387" t="s">
-        <v>2785</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="388" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A388" s="16" t="s">
-        <v>2566</v>
+        <v>2524</v>
       </c>
       <c r="B388" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C388" s="37" t="s">
-        <v>2573</v>
+        <v>2780</v>
       </c>
       <c r="D388" t="s">
-        <v>2786</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="389" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A389" s="16" t="s">
-        <v>2574</v>
+        <v>2525</v>
       </c>
       <c r="B389" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C389" s="37" t="s">
-        <v>2595</v>
+        <v>2781</v>
       </c>
       <c r="D389" t="s">
-        <v>2754</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="390" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A390" s="16" t="s">
-        <v>2575</v>
+        <v>2526</v>
       </c>
       <c r="B390" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C390" s="37" t="s">
-        <v>2596</v>
+        <v>2782</v>
       </c>
       <c r="D390" t="s">
-        <v>2757</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="391" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A391" s="16" t="s">
-        <v>2576</v>
+        <v>2527</v>
       </c>
       <c r="B391" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C391" s="37" t="s">
-        <v>2597</v>
+        <v>2783</v>
       </c>
       <c r="D391" t="s">
-        <v>2758</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="392" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A392" s="16" t="s">
-        <v>2577</v>
+        <v>2528</v>
       </c>
       <c r="B392" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C392" s="37" t="s">
-        <v>2598</v>
+        <v>2784</v>
       </c>
       <c r="D392" t="s">
-        <v>2763</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="393" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A393" s="16" t="s">
-        <v>2578</v>
+        <v>2529</v>
       </c>
       <c r="B393" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C393" s="37" t="s">
-        <v>2599</v>
+        <v>2785</v>
       </c>
       <c r="D393" t="s">
-        <v>2764</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="394" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A394" s="16" t="s">
-        <v>2579</v>
+        <v>2530</v>
       </c>
       <c r="B394" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C394" s="37" t="s">
-        <v>2600</v>
+        <v>2786</v>
       </c>
       <c r="D394" t="s">
-        <v>2765</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="395" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A395" s="16" t="s">
-        <v>2580</v>
+        <v>2531</v>
       </c>
       <c r="B395" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C395" s="37" t="s">
-        <v>2601</v>
+        <v>2787</v>
       </c>
       <c r="D395" t="s">
-        <v>2766</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="396" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A396" s="16" t="s">
-        <v>2581</v>
+        <v>2532</v>
       </c>
       <c r="B396" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C396" s="37" t="s">
-        <v>2595</v>
+        <v>2781</v>
       </c>
       <c r="D396" t="s">
-        <v>2755</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="397" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A397" s="16" t="s">
-        <v>2582</v>
+        <v>2533</v>
       </c>
       <c r="B397" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C397" s="37" t="s">
-        <v>2596</v>
+        <v>2782</v>
       </c>
       <c r="D397" t="s">
-        <v>2759</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="398" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A398" s="16" t="s">
-        <v>2583</v>
+        <v>2534</v>
       </c>
       <c r="B398" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C398" s="37" t="s">
-        <v>2597</v>
+        <v>2783</v>
       </c>
       <c r="D398" t="s">
-        <v>2760</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="399" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A399" s="16" t="s">
-        <v>2584</v>
+        <v>2535</v>
       </c>
       <c r="B399" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C399" s="37" t="s">
-        <v>2598</v>
+        <v>2784</v>
       </c>
       <c r="D399" t="s">
-        <v>2767</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="400" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A400" s="16" t="s">
-        <v>2585</v>
+        <v>2536</v>
       </c>
       <c r="B400" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C400" s="37" t="s">
-        <v>2599</v>
+        <v>2785</v>
       </c>
       <c r="D400" t="s">
-        <v>2768</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="401" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A401" s="16" t="s">
-        <v>2586</v>
+        <v>2537</v>
       </c>
       <c r="B401" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C401" s="37" t="s">
-        <v>2600</v>
+        <v>2786</v>
       </c>
       <c r="D401" t="s">
-        <v>2769</v>
+        <v>2706</v>
       </c>
     </row>
     <row r="402" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A402" s="16" t="s">
-        <v>2587</v>
+        <v>2538</v>
       </c>
       <c r="B402" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C402" s="37" t="s">
-        <v>2601</v>
+        <v>2787</v>
       </c>
       <c r="D402" t="s">
-        <v>2787</v>
+        <v>2724</v>
       </c>
     </row>
     <row r="403" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A403" s="16" t="s">
-        <v>2588</v>
+        <v>2539</v>
       </c>
       <c r="B403" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C403" s="37" t="s">
-        <v>2595</v>
+        <v>2781</v>
       </c>
       <c r="D403" t="s">
-        <v>2788</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="404" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A404" s="16" t="s">
-        <v>2589</v>
+        <v>2540</v>
       </c>
       <c r="B404" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C404" s="37" t="s">
-        <v>2596</v>
+        <v>2782</v>
       </c>
       <c r="D404" t="s">
-        <v>2789</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="405" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A405" s="16" t="s">
-        <v>2590</v>
+        <v>2541</v>
       </c>
       <c r="B405" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C405" s="37" t="s">
-        <v>2597</v>
+        <v>2783</v>
       </c>
       <c r="D405" t="s">
-        <v>2790</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="406" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A406" s="16" t="s">
-        <v>2591</v>
+        <v>2542</v>
       </c>
       <c r="B406" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C406" s="37" t="s">
-        <v>2598</v>
+        <v>2784</v>
       </c>
       <c r="D406" t="s">
-        <v>2791</v>
+        <v>2728</v>
       </c>
     </row>
     <row r="407" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A407" s="16" t="s">
-        <v>2592</v>
+        <v>2543</v>
       </c>
       <c r="B407" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C407" s="37" t="s">
-        <v>2599</v>
+        <v>2785</v>
       </c>
       <c r="D407" t="s">
-        <v>2792</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="408" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A408" s="16" t="s">
-        <v>2593</v>
+        <v>2544</v>
       </c>
       <c r="B408" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C408" s="37" t="s">
-        <v>2600</v>
+        <v>2786</v>
       </c>
       <c r="D408" t="s">
-        <v>2793</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="409" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A409" s="16" t="s">
-        <v>2594</v>
+        <v>2545</v>
       </c>
       <c r="B409" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C409" s="37" t="s">
-        <v>2601</v>
+        <v>2787</v>
       </c>
       <c r="D409" t="s">
-        <v>2794</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="410" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A410" s="16" t="s">
-        <v>2602</v>
+        <v>2546</v>
       </c>
       <c r="B410" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C410" s="37" t="s">
-        <v>2623</v>
+        <v>2788</v>
       </c>
       <c r="D410" t="s">
-        <v>2795</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="411" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A411" s="16" t="s">
-        <v>2603</v>
+        <v>2547</v>
       </c>
       <c r="B411" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C411" s="37" t="s">
-        <v>2624</v>
+        <v>2789</v>
       </c>
       <c r="D411" t="s">
-        <v>2796</v>
+        <v>2733</v>
       </c>
     </row>
     <row r="412" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A412" s="16" t="s">
-        <v>2604</v>
+        <v>2548</v>
       </c>
       <c r="B412" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C412" s="37" t="s">
-        <v>2625</v>
+        <v>2790</v>
       </c>
       <c r="D412" t="s">
-        <v>2797</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="413" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A413" s="16" t="s">
-        <v>2605</v>
+        <v>2549</v>
       </c>
       <c r="B413" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C413" s="37" t="s">
-        <v>2626</v>
+        <v>2791</v>
       </c>
       <c r="D413" t="s">
-        <v>2798</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="414" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A414" s="16" t="s">
-        <v>2606</v>
+        <v>2550</v>
       </c>
       <c r="B414" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C414" s="37" t="s">
-        <v>2627</v>
+        <v>2792</v>
       </c>
       <c r="D414" t="s">
-        <v>2799</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="415" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A415" s="16" t="s">
-        <v>2607</v>
+        <v>2551</v>
       </c>
       <c r="B415" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C415" s="37" t="s">
-        <v>2628</v>
+        <v>2793</v>
       </c>
       <c r="D415" t="s">
-        <v>2800</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="416" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A416" s="16" t="s">
-        <v>2608</v>
+        <v>2552</v>
       </c>
       <c r="B416" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C416" s="37" t="s">
-        <v>2629</v>
+        <v>2794</v>
       </c>
       <c r="D416" t="s">
-        <v>2801</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A417" s="16" t="s">
-        <v>2609</v>
+        <v>2553</v>
       </c>
       <c r="B417" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C417" s="37" t="s">
-        <v>2623</v>
+        <v>2788</v>
       </c>
       <c r="D417" t="s">
-        <v>2802</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A418" s="16" t="s">
-        <v>2610</v>
+        <v>2554</v>
       </c>
       <c r="B418" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C418" s="37" t="s">
-        <v>2624</v>
+        <v>2789</v>
       </c>
       <c r="D418" t="s">
-        <v>2803</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="419" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A419" s="16" t="s">
-        <v>2611</v>
+        <v>2555</v>
       </c>
       <c r="B419" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C419" s="37" t="s">
-        <v>2625</v>
+        <v>2790</v>
       </c>
       <c r="D419" t="s">
-        <v>2804</v>
+        <v>2741</v>
       </c>
     </row>
     <row r="420" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A420" s="16" t="s">
-        <v>2612</v>
+        <v>2556</v>
       </c>
       <c r="B420" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C420" s="37" t="s">
-        <v>2626</v>
+        <v>2791</v>
       </c>
       <c r="D420" t="s">
-        <v>2805</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="421" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A421" s="16" t="s">
-        <v>2613</v>
+        <v>2557</v>
       </c>
       <c r="B421" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C421" s="37" t="s">
-        <v>2627</v>
+        <v>2792</v>
       </c>
       <c r="D421" t="s">
-        <v>2806</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="422" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A422" s="16" t="s">
-        <v>2614</v>
+        <v>2558</v>
       </c>
       <c r="B422" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C422" s="37" t="s">
-        <v>2628</v>
+        <v>2793</v>
       </c>
       <c r="D422" t="s">
-        <v>2807</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="423" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A423" s="16" t="s">
-        <v>2615</v>
+        <v>2559</v>
       </c>
       <c r="B423" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C423" s="37" t="s">
-        <v>2629</v>
+        <v>2794</v>
       </c>
       <c r="D423" t="s">
-        <v>2808</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A424" s="16" t="s">
-        <v>2616</v>
+        <v>2560</v>
       </c>
       <c r="B424" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C424" s="37" t="s">
-        <v>2623</v>
+        <v>2788</v>
       </c>
       <c r="D424" t="s">
-        <v>2809</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="425" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A425" s="16" t="s">
-        <v>2617</v>
+        <v>2561</v>
       </c>
       <c r="B425" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C425" s="37" t="s">
-        <v>2624</v>
+        <v>2789</v>
       </c>
       <c r="D425" t="s">
-        <v>2810</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="426" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A426" s="16" t="s">
-        <v>2618</v>
+        <v>2562</v>
       </c>
       <c r="B426" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C426" s="37" t="s">
-        <v>2625</v>
+        <v>2790</v>
       </c>
       <c r="D426" t="s">
-        <v>2811</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="427" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A427" s="16" t="s">
-        <v>2619</v>
+        <v>2563</v>
       </c>
       <c r="B427" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C427" s="37" t="s">
-        <v>2626</v>
+        <v>2791</v>
       </c>
       <c r="D427" t="s">
-        <v>2812</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="428" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A428" s="16" t="s">
-        <v>2620</v>
+        <v>2564</v>
       </c>
       <c r="B428" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C428" s="37" t="s">
-        <v>2627</v>
+        <v>2792</v>
       </c>
       <c r="D428" t="s">
-        <v>2813</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="429" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A429" s="16" t="s">
-        <v>2621</v>
+        <v>2565</v>
       </c>
       <c r="B429" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C429" s="37" t="s">
-        <v>2628</v>
+        <v>2793</v>
       </c>
       <c r="D429" t="s">
-        <v>2814</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="16.899999999999999" customHeight="1">
       <c r="A430" s="16" t="s">
-        <v>2622</v>
+        <v>2566</v>
       </c>
       <c r="B430" s="16" t="s">
         <v>2130</v>
       </c>
       <c r="C430" s="37" t="s">
-        <v>2629</v>
+        <v>2794</v>
       </c>
       <c r="D430" t="s">
-        <v>2815</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="431" spans="1:4">
       <c r="A431" s="16" t="s">
-        <v>2403</v>
+        <v>2382</v>
       </c>
       <c r="B431" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C431" s="37" t="s">
-        <v>2630</v>
+        <v>2567</v>
       </c>
       <c r="D431" t="s">
-        <v>2366</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="432" spans="1:4">
       <c r="A432" s="16" t="s">
-        <v>2367</v>
+        <v>2346</v>
       </c>
       <c r="B432" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C432" s="37" t="s">
-        <v>2631</v>
+        <v>2568</v>
       </c>
       <c r="D432" t="s">
-        <v>2633</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="433" spans="1:4">
       <c r="A433" s="16" t="s">
-        <v>2404</v>
+        <v>2383</v>
       </c>
       <c r="B433" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C433" s="37" t="s">
-        <v>2632</v>
+        <v>2569</v>
       </c>
       <c r="D433" t="s">
-        <v>2634</v>
+        <v>2571</v>
       </c>
     </row>
     <row r="434" spans="1:4">
       <c r="A434" s="16" t="s">
-        <v>2368</v>
+        <v>2347</v>
       </c>
       <c r="B434" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C434" s="37" t="s">
-        <v>2635</v>
+        <v>2572</v>
       </c>
       <c r="D434" t="s">
-        <v>2636</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="435" spans="1:4">
       <c r="A435" s="16" t="s">
-        <v>2637</v>
+        <v>2574</v>
       </c>
       <c r="B435" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C435" s="37" t="s">
-        <v>2644</v>
+        <v>2581</v>
       </c>
       <c r="D435" t="s">
-        <v>2646</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="436" spans="1:4">
       <c r="A436" s="16" t="s">
-        <v>2640</v>
+        <v>2577</v>
       </c>
       <c r="B436" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C436" s="32" t="s">
-        <v>2631</v>
+        <v>2568</v>
       </c>
       <c r="D436" t="s">
-        <v>2647</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="437" spans="1:4">
       <c r="A437" s="16" t="s">
-        <v>2638</v>
+        <v>2575</v>
       </c>
       <c r="B437" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C437" s="37" t="s">
-        <v>2645</v>
+        <v>2582</v>
       </c>
       <c r="D437" t="s">
-        <v>2649</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="438" spans="1:4">
       <c r="A438" s="16" t="s">
-        <v>2639</v>
+        <v>2576</v>
       </c>
       <c r="B438" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C438" s="32" t="s">
-        <v>2635</v>
+        <v>2572</v>
       </c>
       <c r="D438" t="s">
-        <v>2650</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="439" spans="1:4">
       <c r="A439" s="16" t="s">
-        <v>2641</v>
+        <v>2578</v>
       </c>
       <c r="B439" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C439" s="37" t="s">
-        <v>2630</v>
+        <v>2567</v>
       </c>
       <c r="D439" t="s">
-        <v>2652</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="440" spans="1:4">
       <c r="A440" s="16" t="s">
-        <v>2642</v>
+        <v>2579</v>
       </c>
       <c r="B440" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C440" s="32" t="s">
-        <v>2631</v>
+        <v>2568</v>
       </c>
       <c r="D440" t="s">
-        <v>2648</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="441" spans="1:4">
       <c r="A441" s="16" t="s">
-        <v>2654</v>
+        <v>2591</v>
       </c>
       <c r="B441" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C441" s="37" t="s">
-        <v>2632</v>
+        <v>2569</v>
       </c>
       <c r="D441" t="s">
-        <v>2653</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="442" spans="1:4">
       <c r="A442" s="16" t="s">
-        <v>2643</v>
+        <v>2580</v>
       </c>
       <c r="B442" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C442" s="32" t="s">
-        <v>2635</v>
+        <v>2572</v>
       </c>
       <c r="D442" t="s">
-        <v>2651</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="443" spans="1:4">
       <c r="A443" s="16" t="s">
-        <v>2662</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -30245,7 +30223,6 @@
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -30632,35 +30609,35 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>2303</v>
+        <v>2284</v>
       </c>
       <c r="C45" t="s">
-        <v>2304</v>
+        <v>2285</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>2305</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>2306</v>
+        <v>2287</v>
       </c>
       <c r="C46" t="s">
-        <v>2307</v>
+        <v>2288</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>2308</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>2309</v>
+        <v>2290</v>
       </c>
       <c r="C47" t="s">
-        <v>2310</v>
+        <v>2291</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>2311</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -30679,10 +30656,10 @@
         <v>1946</v>
       </c>
       <c r="C49" t="s">
-        <v>2432</v>
+        <v>2405</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>2313</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -30690,10 +30667,10 @@
         <v>1947</v>
       </c>
       <c r="C50" t="s">
-        <v>2433</v>
+        <v>2406</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>2314</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -30712,10 +30689,10 @@
         <v>1981</v>
       </c>
       <c r="C52" t="s">
-        <v>2430</v>
+        <v>2403</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>2315</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -30723,10 +30700,10 @@
         <v>1982</v>
       </c>
       <c r="C53" t="s">
-        <v>2431</v>
+        <v>2404</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>2316</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -30756,10 +30733,10 @@
         <v>2017</v>
       </c>
       <c r="C56" t="s">
-        <v>2429</v>
+        <v>2402</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>2312</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -30767,10 +30744,10 @@
         <v>2018</v>
       </c>
       <c r="C57" t="s">
-        <v>2428</v>
+        <v>2401</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>2317</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -30789,10 +30766,10 @@
         <v>2048</v>
       </c>
       <c r="C59" t="s">
-        <v>2318</v>
+        <v>2299</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>2320</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -30800,10 +30777,10 @@
         <v>2049</v>
       </c>
       <c r="C60" t="s">
-        <v>2319</v>
+        <v>2300</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>2321</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -30833,10 +30810,10 @@
         <v>2082</v>
       </c>
       <c r="C63" t="s">
-        <v>2323</v>
+        <v>2304</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>2324</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -30844,10 +30821,10 @@
         <v>2083</v>
       </c>
       <c r="C64" t="s">
-        <v>2322</v>
+        <v>2303</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>2325</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -30855,318 +30832,318 @@
         <v>2111</v>
       </c>
       <c r="C65" t="s">
-        <v>2327</v>
+        <v>2308</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>2326</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>2361</v>
+        <v>2340</v>
       </c>
       <c r="C66" t="s">
-        <v>2371</v>
+        <v>2350</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>2391</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>2372</v>
+        <v>2351</v>
       </c>
       <c r="C67" t="s">
-        <v>2380</v>
+        <v>2359</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>2392</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>2373</v>
+        <v>2352</v>
       </c>
       <c r="C68" t="s">
-        <v>2381</v>
+        <v>2360</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>2393</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>2422</v>
+        <v>2395</v>
       </c>
       <c r="C69" t="s">
-        <v>2426</v>
+        <v>2399</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>2444</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>2423</v>
+        <v>2396</v>
       </c>
       <c r="C70" t="s">
-        <v>2427</v>
+        <v>2400</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>2447</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>2424</v>
+        <v>2397</v>
       </c>
       <c r="C71" t="s">
-        <v>2434</v>
+        <v>2407</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>2445</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>2425</v>
+        <v>2398</v>
       </c>
       <c r="C72" t="s">
-        <v>2435</v>
+        <v>2408</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>2446</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>2362</v>
+        <v>2341</v>
       </c>
       <c r="C73" t="s">
-        <v>2384</v>
+        <v>2363</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>2395</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>2374</v>
+        <v>2353</v>
       </c>
       <c r="C74" t="s">
-        <v>2382</v>
+        <v>2361</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>2396</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>2375</v>
+        <v>2354</v>
       </c>
       <c r="C75" t="s">
-        <v>2383</v>
+        <v>2362</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>2394</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>2436</v>
+        <v>2409</v>
       </c>
       <c r="C76" t="s">
-        <v>2440</v>
+        <v>2413</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>2448</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>2437</v>
+        <v>2410</v>
       </c>
       <c r="C77" t="s">
-        <v>2443</v>
+        <v>2416</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>2449</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>2438</v>
+        <v>2411</v>
       </c>
       <c r="C78" t="s">
-        <v>2442</v>
+        <v>2415</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>2450</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>2439</v>
+        <v>2412</v>
       </c>
       <c r="C79" t="s">
-        <v>2441</v>
+        <v>2414</v>
       </c>
       <c r="D79" s="22" t="s">
-        <v>2451</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>2363</v>
+        <v>2342</v>
       </c>
       <c r="C80" t="s">
-        <v>2387</v>
+        <v>2366</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>2397</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>2376</v>
+        <v>2355</v>
       </c>
       <c r="C81" t="s">
-        <v>2385</v>
+        <v>2364</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>2398</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>2377</v>
+        <v>2356</v>
       </c>
       <c r="C82" t="s">
-        <v>2386</v>
+        <v>2365</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>2399</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>2452</v>
+        <v>2425</v>
       </c>
       <c r="C83" t="s">
-        <v>2453</v>
+        <v>2426</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>2457</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>2461</v>
+        <v>2434</v>
       </c>
       <c r="C84" t="s">
-        <v>2454</v>
+        <v>2427</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>2458</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>2462</v>
+        <v>2435</v>
       </c>
       <c r="C85" t="s">
-        <v>2455</v>
+        <v>2428</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>2459</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>2463</v>
+        <v>2436</v>
       </c>
       <c r="C86" t="s">
-        <v>2456</v>
+        <v>2429</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>2460</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>2364</v>
+        <v>2343</v>
       </c>
       <c r="C87" t="s">
-        <v>2388</v>
+        <v>2367</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>2400</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>2378</v>
+        <v>2357</v>
       </c>
       <c r="C88" t="s">
-        <v>2389</v>
+        <v>2368</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>2401</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>2379</v>
+        <v>2358</v>
       </c>
       <c r="C89" t="s">
-        <v>2390</v>
+        <v>2369</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>2402</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>2464</v>
+        <v>2437</v>
       </c>
       <c r="C90" t="s">
-        <v>2468</v>
+        <v>2441</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>2472</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>2465</v>
+        <v>2438</v>
       </c>
       <c r="C91" t="s">
-        <v>2469</v>
+        <v>2442</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>2473</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>2466</v>
+        <v>2439</v>
       </c>
       <c r="C92" t="s">
-        <v>2470</v>
+        <v>2443</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>2474</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>2467</v>
+        <v>2440</v>
       </c>
       <c r="C93" t="s">
-        <v>2471</v>
+        <v>2444</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>2475</v>
+        <v>2448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added cusp and trigonid/talonid structures
</commit_message>
<xml_diff>
--- a/Terms.xlsx
+++ b/Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7DA684-1653-460B-A824-F0199442AD3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9108EEBB-F583-415A-995A-8FBB4063B5B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{855B7C57-FE80-7B4E-8146-986771C66920}"/>
   </bookViews>
@@ -79,8 +79,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E66E2B85-9F4E-4CFA-AF28-5DD3AA585457}</author>
+  </authors>
+  <commentList>
+    <comment ref="D98" authorId="0" shapeId="0" xr:uid="{E66E2B85-9F4E-4CFA-AF28-5DD3AA585457}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check these</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5554" uniqueCount="2849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5575" uniqueCount="2870">
   <si>
     <t>Status</t>
   </si>
@@ -8700,12 +8718,75 @@
   <si>
     <t>occlusal surface' and ('part of' some 'lower molar 1')</t>
   </si>
+  <si>
+    <t>hypoconulid</t>
+  </si>
+  <si>
+    <t>entoconid</t>
+  </si>
+  <si>
+    <t>metaconid</t>
+  </si>
+  <si>
+    <t>paraconid</t>
+  </si>
+  <si>
+    <t>protoconid</t>
+  </si>
+  <si>
+    <t>The medial-most of three cusps on the talonid (posterior) end of lower molariform teeth (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>The lateral-most of three cusps on the trigonid (anterior) end of lower molariform teeth (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>The posterior-most of three cusps, located on the medial side of the trigonid (anterior) end of lower molariform teeth (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>The anterior-most of three cusps, located on the medial side of the trigonid (anterior) end of lower molariform teeth (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>The posterior-most of three cusps on the talonid (posterior) end of lower molariform teeth (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>hypoconulid' and ('part of' some 'molariform tooth')</t>
+  </si>
+  <si>
+    <t>entoconid' and ('part of' some 'molariform tooth')</t>
+  </si>
+  <si>
+    <t>metaconid' and ('part of' some 'molariform tooth')</t>
+  </si>
+  <si>
+    <t>paraconid' and ('part of' some 'molariform tooth')</t>
+  </si>
+  <si>
+    <t>protoconid' and ('part of' some 'molariform tooth')</t>
+  </si>
+  <si>
+    <t>trigonid</t>
+  </si>
+  <si>
+    <t>talonid</t>
+  </si>
+  <si>
+    <t>The anterior-most part of lower molariform teeth formed by the protoconid, paraconid, and metaconid (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>The posterior-most part of lower molariform teeth formed by the hypoconid, entoconid, and hypoconulid (modified from https://animaldiversity.org/collections/mammal_anatomy/cheek_teeth_structure/)</t>
+  </si>
+  <si>
+    <t>trigonid' and ('part of' some 'molariform tooth')</t>
+  </si>
+  <si>
+    <t>talonid' and ('part of' some 'molariform tooth')</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8813,6 +8894,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -9265,6 +9352,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D98" dT="2021-05-03T21:08:13.90" personId="{2C6E4DD5-C095-4E6A-BA57-16604D2292AC}" id="{E66E2B85-9F4E-4CFA-AF28-5DD3AA585457}">
+    <text>Check these</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581405C8-F852-7340-B9C9-201B714E3AD5}">
   <dimension ref="A1:D25"/>
@@ -23984,8 +24079,8 @@
   <dimension ref="A1:D500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C459" sqref="C459"/>
+      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -30596,11 +30691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
-  <dimension ref="A1:D93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C6BB58-E681-9A44-BAE6-1CC6AE173542}">
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -31515,9 +31610,87 @@
         <v>2448</v>
       </c>
     </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>2849</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2858</v>
+      </c>
+      <c r="D94" s="32" t="s">
+        <v>2859</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>2850</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2854</v>
+      </c>
+      <c r="D95" s="32" t="s">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>2851</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2856</v>
+      </c>
+      <c r="D96" s="32" t="s">
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>2852</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2857</v>
+      </c>
+      <c r="D97" s="32" t="s">
+        <v>2862</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>2853</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2855</v>
+      </c>
+      <c r="D98" s="32" t="s">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>2864</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2866</v>
+      </c>
+      <c r="D99" s="32" t="s">
+        <v>2868</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D100" s="32" t="s">
+        <v>2869</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>